<commit_message>
Karn has earned a price tag
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>4</v>
+        <v>3.89</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="6">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>0.82</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="6">
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="D36" s="7" t="n">
-        <v>3.83</v>
+        <v>3.76</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="6">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D37" s="7" t="n">
-        <v>3.66</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="6">
@@ -1636,10 +1636,8 @@
           <t>V.2</t>
         </is>
       </c>
-      <c r="D58" s="7" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
+      <c r="D58" s="7" t="n">
+        <v>3.39</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" s="6">

</xml_diff>

<commit_message>
Removed some cards from the album
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -463,10 +463,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D2" s="7" t="n">
-        <v>10.42</v>
+        <v>10.39</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D3" s="7" t="n">
-        <v>8.65</v>
+        <v>8.630000000000001</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="6">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="D4" s="7" t="n">
-        <v>13.03</v>
+        <v>12.96</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="6">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>16.1</v>
+        <v>16.27</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="6">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>3.09</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D7" s="7" t="n">
-        <v>8.69</v>
+        <v>8.710000000000001</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="6">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="D8" s="7" t="n">
-        <v>7.9</v>
+        <v>7.97</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="6">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="D9" s="7" t="n">
-        <v>5.22</v>
+        <v>5.47</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="6">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="D10" s="7" t="n">
-        <v>24.17</v>
+        <v>24.16</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>1.09</v>
+        <v>1.11</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>6</v>
+        <v>5.92</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="6">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>3.99</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="6">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>4.44</v>
+        <v>4.52</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="6">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>16.96</v>
+        <v>17.13</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="6">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>3.42</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="6">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>3.49</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="6">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>1.44</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="6">
@@ -877,38 +877,38 @@
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>6.75</v>
+        <v>6.77</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="6">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Cut Down</t>
+          <t>Deadly Dispute</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United Promos</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>0.6</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="6">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Deadly Dispute</t>
+          <t>Flame-Wreathed Phoenix</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
@@ -917,38 +917,38 @@
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>2.71</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="6">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>Flame-Wreathed Phoenix</t>
+          <t>Shivan Devastator</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>1.58</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="6">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>Shivan Devastator</t>
+          <t>Vexing Devil</t>
         </is>
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Avacyn Restored</t>
         </is>
       </c>
       <c r="C24" s="4" t="inlineStr">
@@ -957,58 +957,58 @@
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="25" ht="15" customHeight="1" s="6">
+        <v>4.64</v>
+      </c>
+    </row>
+    <row r="25" ht="13.5" customHeight="1" s="6">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>Vexing Devil</t>
+          <t>Fyndhorn Elves</t>
         </is>
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>Avacyn Restored</t>
+          <t>30th Anniversary Celebration</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>German</t>
         </is>
       </c>
       <c r="D25" s="7" t="n">
-        <v>4.67</v>
-      </c>
-    </row>
-    <row r="26" ht="13.5" customHeight="1" s="6">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="26" ht="15" customHeight="1" s="6">
       <c r="A26" s="4" t="inlineStr">
         <is>
-          <t>Fyndhorn Elves</t>
+          <t>Gyre Sage</t>
         </is>
       </c>
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>30th Anniversary Celebration</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C26" s="4" t="inlineStr">
         <is>
-          <t>German</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D26" s="7" t="n">
-        <v>2.27</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="6">
       <c r="A27" s="4" t="inlineStr">
         <is>
-          <t>Gyre Sage</t>
+          <t>Hardened Scales</t>
         </is>
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Khans of Tarkir</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
@@ -1017,18 +1017,18 @@
         </is>
       </c>
       <c r="D27" s="7" t="n">
-        <v>1.52</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" s="6">
       <c r="A28" s="4" t="inlineStr">
         <is>
-          <t>Hardened Scales</t>
+          <t>Life from the Loam</t>
         </is>
       </c>
       <c r="B28" s="4" t="inlineStr">
         <is>
-          <t>Khans of Tarkir</t>
+          <t>Duel Decks: Izzet vs Golgari</t>
         </is>
       </c>
       <c r="C28" s="4" t="inlineStr">
@@ -1037,27 +1037,27 @@
         </is>
       </c>
       <c r="D28" s="7" t="n">
-        <v>2.58</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="6">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>Life from the Loam</t>
+          <t>Majestic Genesis</t>
         </is>
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>Duel Decks: Izzet vs Golgari</t>
+          <t>Commander Legends: Battle For Baldur's Gate Promos</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D29" s="7" t="n">
-        <v>10</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="6">
@@ -1068,27 +1068,27 @@
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate Promos</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C30" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D30" s="7" t="n">
-        <v>2.87</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" s="6">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>Majestic Genesis</t>
+          <t>Nylea, God of the Hunt</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Theros</t>
         </is>
       </c>
       <c r="C31" s="4" t="inlineStr">
@@ -1097,18 +1097,18 @@
         </is>
       </c>
       <c r="D31" s="7" t="n">
-        <v>1.66</v>
+        <v>4.56</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="6">
       <c r="A32" s="4" t="inlineStr">
         <is>
-          <t>Nylea, God of the Hunt</t>
+          <t>Parallel Lives</t>
         </is>
       </c>
       <c r="B32" s="4" t="inlineStr">
         <is>
-          <t>Theros</t>
+          <t>Innistrad</t>
         </is>
       </c>
       <c r="C32" s="4" t="inlineStr">
@@ -1117,18 +1117,18 @@
         </is>
       </c>
       <c r="D32" s="7" t="n">
-        <v>4.59</v>
+        <v>27.94</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="6">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>Parallel Lives</t>
+          <t>Sphinx's Revelation</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>Innistrad</t>
+          <t>Return to Ravnica</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
@@ -1137,18 +1137,18 @@
         </is>
       </c>
       <c r="D33" s="7" t="n">
-        <v>26.62</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="6">
       <c r="A34" s="4" t="inlineStr">
         <is>
-          <t>Sphinx's Revelation</t>
+          <t>Ashiok, Nightmare Weaver</t>
         </is>
       </c>
       <c r="B34" s="4" t="inlineStr">
         <is>
-          <t>Return to Ravnica</t>
+          <t>Theros</t>
         </is>
       </c>
       <c r="C34" s="4" t="inlineStr">
@@ -1157,18 +1157,18 @@
         </is>
       </c>
       <c r="D34" s="7" t="n">
-        <v>2.04</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="6">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>Ashiok, Nightmare Weaver</t>
+          <t>Mind Grind</t>
         </is>
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>Theros</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C35" s="4" t="inlineStr">
@@ -1177,18 +1177,18 @@
         </is>
       </c>
       <c r="D35" s="7" t="n">
-        <v>3.83</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" s="6">
       <c r="A36" s="4" t="inlineStr">
         <is>
-          <t>Mind Grind</t>
+          <t>Kolaghan's Command</t>
         </is>
       </c>
       <c r="B36" s="4" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C36" s="4" t="inlineStr">
@@ -1197,18 +1197,18 @@
         </is>
       </c>
       <c r="D36" s="7" t="n">
-        <v>3.45</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="6">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>Kolaghan's Command</t>
+          <t>Mogis, God of Slaughter</t>
         </is>
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C37" s="4" t="inlineStr">
@@ -1217,133 +1217,133 @@
         </is>
       </c>
       <c r="D37" s="7" t="n">
-        <v>3.46</v>
+        <v>7.72</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="6">
       <c r="A38" s="4" t="inlineStr">
         <is>
-          <t>Mogis, God of Slaughter</t>
+          <t>Ajani, Sleeper Agent</t>
         </is>
       </c>
       <c r="B38" s="4" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C38" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D38" s="7" t="n">
-        <v>7.77</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="6">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>Ajani, Sleeper Agent</t>
+          <t>Ivy, Gleeful Spellthief</t>
         </is>
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Dominaria United Promos</t>
         </is>
       </c>
       <c r="C39" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>V.1</t>
         </is>
       </c>
       <c r="D39" s="7" t="n">
-        <v>3.9</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="6">
       <c r="A40" s="4" t="inlineStr">
         <is>
-          <t>Ivy, Gleeful Spellthief</t>
+          <t>Vorel of the Hull Clade</t>
         </is>
       </c>
       <c r="B40" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United Promos</t>
+          <t>Dragon's Maze</t>
         </is>
       </c>
       <c r="C40" s="4" t="inlineStr">
         <is>
-          <t>V.1</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D40" s="7" t="n">
-        <v>1.24</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="6">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>Vorel of the Hull Clade</t>
+          <t>Deathrite Shaman</t>
         </is>
       </c>
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>Dragon's Maze</t>
+          <t>Return to Ravnica</t>
         </is>
       </c>
       <c r="C41" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D41" s="7" t="n">
-        <v>1.87</v>
+        <v>6.19</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="6">
       <c r="A42" s="4" t="inlineStr">
         <is>
-          <t>Deathrite Shaman</t>
+          <t>Jarad, Golgari Lich Lord</t>
         </is>
       </c>
       <c r="B42" s="4" t="inlineStr">
         <is>
-          <t>Return to Ravnica</t>
+          <t>Duel Decks: Izzet vs Golgari</t>
         </is>
       </c>
       <c r="C42" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D42" s="7" t="n">
-        <v>6.25</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="6">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>Jarad, Golgari Lich Lord</t>
+          <t>The Gitrog Monster</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>Duel Decks: Izzet vs Golgari</t>
+          <t>Shadows over Innistrad</t>
         </is>
       </c>
       <c r="C43" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D43" s="7" t="n">
-        <v>1.72</v>
+        <v>3.71</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="6">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>The Gitrog Monster</t>
+          <t>Arlinn Kord: Arlinn, Embraced by the Moon</t>
         </is>
       </c>
       <c r="B44" s="4" t="inlineStr">
@@ -1357,18 +1357,18 @@
         </is>
       </c>
       <c r="D44" s="7" t="n">
-        <v>3.68</v>
+        <v>4.27</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="6">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>Arlinn Kord: Arlinn, Embraced by the Moon</t>
+          <t>Miirym, Sentinel Wyrm</t>
         </is>
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>Shadows over Innistrad</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C45" s="4" t="inlineStr">
@@ -1377,18 +1377,18 @@
         </is>
       </c>
       <c r="D45" s="7" t="n">
-        <v>4.57</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" s="6">
       <c r="A46" s="4" t="inlineStr">
         <is>
-          <t>Miirym, Sentinel Wyrm</t>
+          <t>Aether Vial</t>
         </is>
       </c>
       <c r="B46" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C46" s="4" t="inlineStr">
@@ -1397,18 +1397,18 @@
         </is>
       </c>
       <c r="D46" s="7" t="n">
-        <v>1.5</v>
+        <v>11.67</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="6">
       <c r="A47" s="4" t="inlineStr">
         <is>
-          <t>Aether Vial</t>
+          <t>Akroma's Memorial</t>
         </is>
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Magic 2013</t>
         </is>
       </c>
       <c r="C47" s="4" t="inlineStr">
@@ -1417,58 +1417,58 @@
         </is>
       </c>
       <c r="D47" s="7" t="n">
-        <v>12.03</v>
+        <v>8.289999999999999</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="6">
       <c r="A48" s="4" t="inlineStr">
         <is>
-          <t>Akroma's Memorial</t>
+          <t>Amulet of Vigor</t>
         </is>
       </c>
       <c r="B48" s="4" t="inlineStr">
         <is>
-          <t>Magic 2013</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C48" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D48" s="7" t="n">
-        <v>8.43</v>
+        <v>17.78</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="6">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>Amulet of Vigor</t>
+          <t>Astral Cornucopia</t>
         </is>
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C49" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D49" s="7" t="n">
-        <v>17.87</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" s="6">
       <c r="A50" s="4" t="inlineStr">
         <is>
-          <t>Astral Cornucopia</t>
+          <t>Coat of Arms</t>
         </is>
       </c>
       <c r="B50" s="4" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C50" s="4" t="inlineStr">
@@ -1477,13 +1477,13 @@
         </is>
       </c>
       <c r="D50" s="7" t="n">
-        <v>1.85</v>
+        <v>9.220000000000001</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" s="6">
       <c r="A51" s="4" t="inlineStr">
         <is>
-          <t>Coat of Arms</t>
+          <t>Dolmen Gate</t>
         </is>
       </c>
       <c r="B51" s="4" t="inlineStr">
@@ -1497,18 +1497,18 @@
         </is>
       </c>
       <c r="D51" s="7" t="n">
-        <v>8.9</v>
+        <v>8.76</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" s="6">
       <c r="A52" s="4" t="inlineStr">
         <is>
-          <t>Dolmen Gate</t>
+          <t>Elbrus, the Binding Blade: Withengar Unbound</t>
         </is>
       </c>
       <c r="B52" s="4" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Dark Ascension</t>
         </is>
       </c>
       <c r="C52" s="4" t="inlineStr">
@@ -1517,13 +1517,13 @@
         </is>
       </c>
       <c r="D52" s="7" t="n">
-        <v>8.869999999999999</v>
+        <v>3.46</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" s="6">
       <c r="A53" s="4" t="inlineStr">
         <is>
-          <t>Elbrus, the Binding Blade: Withengar Unbound</t>
+          <t>Grafdigger's Cage</t>
         </is>
       </c>
       <c r="B53" s="4" t="inlineStr">
@@ -1537,18 +1537,18 @@
         </is>
       </c>
       <c r="D53" s="7" t="n">
-        <v>2.88</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="6">
       <c r="A54" s="4" t="inlineStr">
         <is>
-          <t>Grafdigger's Cage</t>
+          <t>Illusionist's Bracers</t>
         </is>
       </c>
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C54" s="4" t="inlineStr">
@@ -1557,95 +1557,57 @@
         </is>
       </c>
       <c r="D54" s="7" t="n">
-        <v>2</v>
+        <v>5.24</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="6">
       <c r="A55" s="4" t="inlineStr">
         <is>
-          <t>Illusionist's Bracers</t>
+          <t>Karn, Living Legacy</t>
         </is>
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Dominaria United Promos</t>
         </is>
       </c>
       <c r="C55" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>V.2</t>
         </is>
       </c>
       <c r="D55" s="7" t="n">
-        <v>5.23</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="6">
       <c r="A56" s="4" t="inlineStr">
         <is>
-          <t>Karn, Living Legacy</t>
+          <t>Swiftfoot Boots</t>
         </is>
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United Promos</t>
+          <t>Commander 2017</t>
         </is>
       </c>
       <c r="C56" s="4" t="inlineStr">
         <is>
-          <t>V.2</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D56" s="7" t="n">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="57" ht="15" customHeight="1" s="6">
-      <c r="A57" s="4" t="inlineStr">
-        <is>
-          <t>Sol Ring</t>
-        </is>
-      </c>
-      <c r="B57" s="4" t="inlineStr">
-        <is>
-          <t>Commander 2017</t>
-        </is>
-      </c>
-      <c r="C57" s="4" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D57" s="7" t="n">
-        <v>0.9399999999999999</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" s="6">
-      <c r="A58" s="4" t="inlineStr">
-        <is>
-          <t>Swiftfoot Boots</t>
-        </is>
-      </c>
-      <c r="B58" s="4" t="inlineStr">
-        <is>
-          <t>Commander 2017</t>
-        </is>
-      </c>
-      <c r="C58" s="4" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D58" s="7" t="n">
-        <v>1.74</v>
-      </c>
-    </row>
-    <row r="60" ht="15" customHeight="1" s="6">
-      <c r="D60" s="5">
-        <f>SUM(D2:D58)</f>
+      <c r="D58" s="5">
+        <f>SUM(D2:D56)</f>
         <v/>
       </c>
     </row>
+    <row r="1048573" ht="12.75" customHeight="1" s="6"/>
+    <row r="1048574" ht="12.75" customHeight="1" s="6"/>
     <row r="1048575" ht="12.8" customHeight="1" s="6"/>
     <row r="1048576" ht="12.8" customHeight="1" s="6"/>
   </sheetData>

</xml_diff>

<commit_message>
Brothers' War Prerelease Pulls Added
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -463,15 +463,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="39.54" customWidth="1" style="4" min="1" max="1"/>
+    <col width="44.27" customWidth="1" style="4" min="1" max="1"/>
     <col width="46.64" customWidth="1" style="4" min="2" max="2"/>
     <col width="10.57" customWidth="1" style="4" min="3" max="3"/>
     <col width="9.57" customWidth="1" style="5" min="4" max="4"/>
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D2" s="7" t="n">
-        <v>10.53</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D3" s="7" t="n">
-        <v>8.609999999999999</v>
+        <v>8.73</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="6">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="D4" s="7" t="n">
-        <v>12.67</v>
+        <v>12.57</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="6">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>15.79</v>
+        <v>15.49</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="6">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>2.86</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D7" s="7" t="n">
-        <v>8.57</v>
+        <v>8.460000000000001</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="6">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="D8" s="7" t="n">
-        <v>7.91</v>
+        <v>7.83</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="6">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="D10" s="7" t="n">
-        <v>24.6</v>
+        <v>25.12</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
@@ -697,38 +697,38 @@
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>1.17</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="6">
       <c r="A12" s="4" t="inlineStr">
         <is>
-          <t>Lair of the Hydra</t>
+          <t>Argoth, Sanctum of Nature: Titania, Gaea Incarnate</t>
         </is>
       </c>
       <c r="B12" s="4" t="inlineStr">
         <is>
-          <t>Adventures in the Forgotten Realms</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C12" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>1.21</v>
+        <v>3.43</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>Ajani Steadfast</t>
+          <t>Lair of the Hydra</t>
         </is>
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>Magic 2015</t>
+          <t>Adventures in the Forgotten Realms</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr">
@@ -737,18 +737,18 @@
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>6.5</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="6">
       <c r="A14" s="4" t="inlineStr">
         <is>
-          <t>Sage of Hours</t>
+          <t>Ajani Steadfast</t>
         </is>
       </c>
       <c r="B14" s="4" t="inlineStr">
         <is>
-          <t>Journey into Nyx</t>
+          <t>Magic 2015</t>
         </is>
       </c>
       <c r="C14" s="4" t="inlineStr">
@@ -757,18 +757,18 @@
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>3.95</v>
+        <v>6.92</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="6">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Search for Azcanta: Azcanta the Sunken Ruin</t>
+          <t>Sage of Hours</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>Ixalan</t>
+          <t>Journey into Nyx</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr">
@@ -777,18 +777,18 @@
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>4.47</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="6">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>Ancient Brass Dragon</t>
+          <t>Search for Azcanta: Azcanta the Sunken Ruin</t>
         </is>
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Ixalan</t>
         </is>
       </c>
       <c r="C16" s="4" t="inlineStr">
@@ -797,18 +797,18 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>16.62</v>
+        <v>4.52</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="6">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>Dark Petition</t>
+          <t>Ancient Brass Dragon</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>Magic Origins</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr">
@@ -817,18 +817,18 @@
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>3.23</v>
+        <v>16.27</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="6">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>Gravecrawler</t>
+          <t>Dark Petition</t>
         </is>
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>Magic Origins</t>
         </is>
       </c>
       <c r="C18" s="4" t="inlineStr">
@@ -837,38 +837,38 @@
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>4.45</v>
+        <v>3.16</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="6">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>Scourge of the Skyclaves</t>
+          <t>Diabolic Intent</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>Zendikar Rising Promos</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
         <is>
-          <t>V.1</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>1.43</v>
+        <v>11.88</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="6">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>Tree of Perdition</t>
+          <t>Gravecrawler</t>
         </is>
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>Eldritch Moon</t>
+          <t>Dark Ascension</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
@@ -877,78 +877,78 @@
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>7.45</v>
+        <v>4.52</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="6">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Deadly Dispute</t>
+          <t>Scourge of the Skyclaves</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Zendikar Rising Promos</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>V.1</t>
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>2.51</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="6">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Flame-Wreathed Phoenix</t>
+          <t>Tree of Perdition</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Eldritch Moon</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>1.58</v>
+        <v>7.33</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="6">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>Shivan Devastator</t>
+          <t>Deadly Dispute</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>5.12</v>
+        <v>2.86</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="6">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>Vexing Devil</t>
+          <t>Brotherhood's End</t>
         </is>
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>Avacyn Restored</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C24" s="4" t="inlineStr">
@@ -957,38 +957,38 @@
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>4.49</v>
-      </c>
-    </row>
-    <row r="25" ht="13.5" customHeight="1" s="6">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="25" ht="15" customHeight="1" s="6">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>Fyndhorn Elves</t>
+          <t>Flame-Wreathed Phoenix</t>
         </is>
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>30th Anniversary Celebration</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
-          <t>German</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D25" s="7" t="n">
-        <v>2.4</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" s="6">
       <c r="A26" s="4" t="inlineStr">
         <is>
-          <t>Gyre Sage</t>
+          <t>Shivan Devastator</t>
         </is>
       </c>
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C26" s="4" t="inlineStr">
@@ -997,18 +997,18 @@
         </is>
       </c>
       <c r="D26" s="7" t="n">
-        <v>1.54</v>
+        <v>5.21</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="6">
       <c r="A27" s="4" t="inlineStr">
         <is>
-          <t>Hardened Scales</t>
+          <t>Skitterbeam Battalion</t>
         </is>
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>Khans of Tarkir</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
@@ -1017,18 +1017,18 @@
         </is>
       </c>
       <c r="D27" s="7" t="n">
-        <v>2.88</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" s="6">
       <c r="A28" s="4" t="inlineStr">
         <is>
-          <t>Life from the Loam</t>
+          <t>Vexing Devil</t>
         </is>
       </c>
       <c r="B28" s="4" t="inlineStr">
         <is>
-          <t>Duel Decks: Izzet vs Golgari</t>
+          <t>Avacyn Restored</t>
         </is>
       </c>
       <c r="C28" s="4" t="inlineStr">
@@ -1037,18 +1037,18 @@
         </is>
       </c>
       <c r="D28" s="7" t="n">
-        <v>10.5</v>
+        <v>4.71</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="6">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>Majestic Genesis</t>
+          <t>Arms Race</t>
         </is>
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate Promos</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
@@ -1057,18 +1057,18 @@
         </is>
       </c>
       <c r="D29" s="7" t="n">
-        <v>2.87</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="6">
       <c r="A30" s="4" t="inlineStr">
         <is>
-          <t>Majestic Genesis</t>
+          <t>Fauna Shaman</t>
         </is>
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C30" s="4" t="inlineStr">
@@ -1077,38 +1077,38 @@
         </is>
       </c>
       <c r="D30" s="7" t="n">
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="31" ht="15" customHeight="1" s="6">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="31" ht="13.5" customHeight="1" s="6">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>Nylea, God of the Hunt</t>
+          <t>Fyndhorn Elves</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>Theros</t>
+          <t>30th Anniversary Celebration</t>
         </is>
       </c>
       <c r="C31" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>German</t>
         </is>
       </c>
       <c r="D31" s="7" t="n">
-        <v>5</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="6">
       <c r="A32" s="4" t="inlineStr">
         <is>
-          <t>Parallel Lives</t>
+          <t>Gyre Sage</t>
         </is>
       </c>
       <c r="B32" s="4" t="inlineStr">
         <is>
-          <t>Innistrad</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C32" s="4" t="inlineStr">
@@ -1117,18 +1117,18 @@
         </is>
       </c>
       <c r="D32" s="7" t="n">
-        <v>28.63</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="6">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>Sphinx's Revelation</t>
+          <t>Hardened Scales</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>Return to Ravnica</t>
+          <t>Khans of Tarkir</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
@@ -1137,18 +1137,18 @@
         </is>
       </c>
       <c r="D33" s="7" t="n">
-        <v>2.33</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="6">
       <c r="A34" s="4" t="inlineStr">
         <is>
-          <t>Ashiok, Nightmare Weaver</t>
+          <t>Life from the Loam</t>
         </is>
       </c>
       <c r="B34" s="4" t="inlineStr">
         <is>
-          <t>Theros</t>
+          <t>Duel Decks: Izzet vs Golgari</t>
         </is>
       </c>
       <c r="C34" s="4" t="inlineStr">
@@ -1157,38 +1157,38 @@
         </is>
       </c>
       <c r="D34" s="7" t="n">
-        <v>3.76</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="6">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>Mind Grind</t>
+          <t>Majestic Genesis</t>
         </is>
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Commander Legends: Battle For Baldur's Gate Promos</t>
         </is>
       </c>
       <c r="C35" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D35" s="7" t="n">
-        <v>3.49</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" s="6">
       <c r="A36" s="4" t="inlineStr">
         <is>
-          <t>Kolaghan's Command</t>
+          <t>Majestic Genesis</t>
         </is>
       </c>
       <c r="B36" s="4" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C36" s="4" t="inlineStr">
@@ -1197,18 +1197,18 @@
         </is>
       </c>
       <c r="D36" s="7" t="n">
-        <v>3.39</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="6">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>Mogis, God of Slaughter</t>
+          <t>Nylea, God of the Hunt</t>
         </is>
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Theros</t>
         </is>
       </c>
       <c r="C37" s="4" t="inlineStr">
@@ -1217,73 +1217,73 @@
         </is>
       </c>
       <c r="D37" s="7" t="n">
-        <v>7.54</v>
+        <v>5.07</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="6">
       <c r="A38" s="4" t="inlineStr">
         <is>
-          <t>Ajani, Sleeper Agent</t>
+          <t>Parallel Lives</t>
         </is>
       </c>
       <c r="B38" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Innistrad</t>
         </is>
       </c>
       <c r="C38" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D38" s="7" t="n">
-        <v>4.01</v>
+        <v>27.97</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="6">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>Ivy, Gleeful Spellthief</t>
+          <t>Wall of Roots</t>
         </is>
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United Promos</t>
+          <t>30th Anniversary Celebration</t>
         </is>
       </c>
       <c r="C39" s="4" t="inlineStr">
         <is>
-          <t>V.1</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D39" s="7" t="n">
-        <v>1.24</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="6">
       <c r="A40" s="4" t="inlineStr">
         <is>
-          <t>Vorel of the Hull Clade</t>
+          <t>Haywire Mite</t>
         </is>
       </c>
       <c r="B40" s="4" t="inlineStr">
         <is>
-          <t>Dragon's Maze</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C40" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D40" s="7" t="n">
-        <v>1.94</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="6">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>Deathrite Shaman</t>
+          <t>Sphinx's Revelation</t>
         </is>
       </c>
       <c r="B41" s="4" t="inlineStr">
@@ -1297,38 +1297,38 @@
         </is>
       </c>
       <c r="D41" s="7" t="n">
-        <v>6.13</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="6">
       <c r="A42" s="4" t="inlineStr">
         <is>
-          <t>Jarad, Golgari Lich Lord</t>
+          <t>Ashiok, Nightmare Weaver</t>
         </is>
       </c>
       <c r="B42" s="4" t="inlineStr">
         <is>
-          <t>Duel Decks: Izzet vs Golgari</t>
+          <t>Theros</t>
         </is>
       </c>
       <c r="C42" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D42" s="7" t="n">
-        <v>1.94</v>
+        <v>3.77</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="6">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>The Gitrog Monster</t>
+          <t>Mind Grind</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>Shadows over Innistrad</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C43" s="4" t="inlineStr">
@@ -1337,18 +1337,18 @@
         </is>
       </c>
       <c r="D43" s="7" t="n">
-        <v>3.62</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="6">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>Arlinn Kord: Arlinn, Embraced by the Moon</t>
+          <t>Satoru Umezawa</t>
         </is>
       </c>
       <c r="B44" s="4" t="inlineStr">
         <is>
-          <t>Shadows over Innistrad</t>
+          <t>Buy a Box Promos</t>
         </is>
       </c>
       <c r="C44" s="4" t="inlineStr">
@@ -1357,18 +1357,18 @@
         </is>
       </c>
       <c r="D44" s="7" t="n">
-        <v>4.13</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="6">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>Miirym, Sentinel Wyrm</t>
+          <t>Legion's Initiative</t>
         </is>
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Dragon's Maze</t>
         </is>
       </c>
       <c r="C45" s="4" t="inlineStr">
@@ -1377,13 +1377,13 @@
         </is>
       </c>
       <c r="D45" s="7" t="n">
-        <v>1.44</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" s="6">
       <c r="A46" s="4" t="inlineStr">
         <is>
-          <t>Aether Vial</t>
+          <t>Kolaghan's Command</t>
         </is>
       </c>
       <c r="B46" s="4" t="inlineStr">
@@ -1397,18 +1397,18 @@
         </is>
       </c>
       <c r="D46" s="7" t="n">
-        <v>11.62</v>
+        <v>3.51</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="6">
       <c r="A47" s="4" t="inlineStr">
         <is>
-          <t>Akroma's Memorial</t>
+          <t>Mogis, God of Slaughter</t>
         </is>
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>Magic 2013</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C47" s="4" t="inlineStr">
@@ -1417,18 +1417,18 @@
         </is>
       </c>
       <c r="D47" s="7" t="n">
-        <v>7.99</v>
+        <v>7.76</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="6">
       <c r="A48" s="4" t="inlineStr">
         <is>
-          <t>Amulet of Vigor</t>
+          <t>Ajani, Sleeper Agent</t>
         </is>
       </c>
       <c r="B48" s="4" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C48" s="4" t="inlineStr">
@@ -1437,58 +1437,58 @@
         </is>
       </c>
       <c r="D48" s="7" t="n">
-        <v>17.45</v>
+        <v>3.94</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="6">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>Astral Cornucopia</t>
+          <t>Ivy, Gleeful Spellthief</t>
         </is>
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Dominaria United Promos</t>
         </is>
       </c>
       <c r="C49" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>V.1</t>
         </is>
       </c>
       <c r="D49" s="7" t="n">
-        <v>1.75</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" s="6">
       <c r="A50" s="4" t="inlineStr">
         <is>
-          <t>Coat of Arms</t>
+          <t>Vorel of the Hull Clade</t>
         </is>
       </c>
       <c r="B50" s="4" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Dragon's Maze</t>
         </is>
       </c>
       <c r="C50" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D50" s="7" t="n">
-        <v>8.98</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" s="6">
       <c r="A51" s="4" t="inlineStr">
         <is>
-          <t>Dolmen Gate</t>
+          <t>Deathrite Shaman</t>
         </is>
       </c>
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Return to Ravnica</t>
         </is>
       </c>
       <c r="C51" s="4" t="inlineStr">
@@ -1497,38 +1497,38 @@
         </is>
       </c>
       <c r="D51" s="7" t="n">
-        <v>9.19</v>
+        <v>6.26</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" s="6">
       <c r="A52" s="4" t="inlineStr">
         <is>
-          <t>Elbrus, the Binding Blade: Withengar Unbound</t>
+          <t>Jarad, Golgari Lich Lord</t>
         </is>
       </c>
       <c r="B52" s="4" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>Duel Decks: Izzet vs Golgari</t>
         </is>
       </c>
       <c r="C52" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D52" s="7" t="n">
-        <v>3.67</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" s="6">
       <c r="A53" s="4" t="inlineStr">
         <is>
-          <t>Grafdigger's Cage</t>
+          <t>The Gitrog Monster</t>
         </is>
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>Shadows over Innistrad</t>
         </is>
       </c>
       <c r="C53" s="4" t="inlineStr">
@@ -1537,18 +1537,18 @@
         </is>
       </c>
       <c r="D53" s="7" t="n">
-        <v>1.95</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="6">
       <c r="A54" s="4" t="inlineStr">
         <is>
-          <t>Illusionist's Bracers</t>
+          <t>Arlinn Kord: Arlinn, Embraced by the Moon</t>
         </is>
       </c>
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Shadows over Innistrad</t>
         </is>
       </c>
       <c r="C54" s="4" t="inlineStr">
@@ -1557,59 +1557,295 @@
         </is>
       </c>
       <c r="D54" s="7" t="n">
-        <v>5.19</v>
+        <v>4.22</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="6">
       <c r="A55" s="4" t="inlineStr">
         <is>
-          <t>Karn, Living Legacy</t>
+          <t>Miirym, Sentinel Wyrm</t>
         </is>
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United Promos</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C55" s="4" t="inlineStr">
         <is>
-          <t>V.2</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D55" s="7" t="n">
-        <v>3.84</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="6">
       <c r="A56" s="4" t="inlineStr">
         <is>
+          <t>Aether Vial</t>
+        </is>
+      </c>
+      <c r="B56" s="4" t="inlineStr">
+        <is>
+          <t>Double Masters 2022</t>
+        </is>
+      </c>
+      <c r="C56" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D56" s="7" t="n">
+        <v>11.48</v>
+      </c>
+    </row>
+    <row r="57" ht="15" customHeight="1" s="6">
+      <c r="A57" s="4" t="inlineStr">
+        <is>
+          <t>Akroma's Memorial</t>
+        </is>
+      </c>
+      <c r="B57" s="4" t="inlineStr">
+        <is>
+          <t>Magic 2013</t>
+        </is>
+      </c>
+      <c r="C57" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D57" s="7" t="n">
+        <v>8.07</v>
+      </c>
+    </row>
+    <row r="58" ht="15" customHeight="1" s="6">
+      <c r="A58" s="4" t="inlineStr">
+        <is>
+          <t>Amulet of Vigor</t>
+        </is>
+      </c>
+      <c r="B58" s="4" t="inlineStr">
+        <is>
+          <t>Mystery Booster</t>
+        </is>
+      </c>
+      <c r="C58" s="4" t="inlineStr">
+        <is>
+          <t>Foil</t>
+        </is>
+      </c>
+      <c r="D58" s="7" t="n">
+        <v>17.45</v>
+      </c>
+    </row>
+    <row r="59" ht="15" customHeight="1" s="6">
+      <c r="A59" s="4" t="inlineStr">
+        <is>
+          <t>Astral Cornucopia</t>
+        </is>
+      </c>
+      <c r="B59" s="4" t="inlineStr">
+        <is>
+          <t>Born of the Gods</t>
+        </is>
+      </c>
+      <c r="C59" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D59" s="7" t="n">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="60" ht="15" customHeight="1" s="6">
+      <c r="A60" s="4" t="inlineStr">
+        <is>
+          <t>Coat of Arms</t>
+        </is>
+      </c>
+      <c r="B60" s="4" t="inlineStr">
+        <is>
+          <t>Mystery Booster</t>
+        </is>
+      </c>
+      <c r="C60" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D60" s="7" t="n">
+        <v>9.06</v>
+      </c>
+    </row>
+    <row r="61" ht="15" customHeight="1" s="6">
+      <c r="A61" s="4" t="inlineStr">
+        <is>
+          <t>Dolmen Gate</t>
+        </is>
+      </c>
+      <c r="B61" s="4" t="inlineStr">
+        <is>
+          <t>Mystery Booster</t>
+        </is>
+      </c>
+      <c r="C61" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D61" s="7" t="n">
+        <v>9.23</v>
+      </c>
+    </row>
+    <row r="62" ht="15" customHeight="1" s="6">
+      <c r="A62" s="4" t="inlineStr">
+        <is>
+          <t>Elbrus, the Binding Blade: Withengar Unbound</t>
+        </is>
+      </c>
+      <c r="B62" s="4" t="inlineStr">
+        <is>
+          <t>Dark Ascension</t>
+        </is>
+      </c>
+      <c r="C62" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D62" s="7" t="n">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="63" ht="15" customHeight="1" s="6">
+      <c r="A63" s="4" t="inlineStr">
+        <is>
+          <t>Grafdigger's Cage</t>
+        </is>
+      </c>
+      <c r="B63" s="4" t="inlineStr">
+        <is>
+          <t>Dark Ascension</t>
+        </is>
+      </c>
+      <c r="C63" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D63" s="7" t="n">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="64" ht="15" customHeight="1" s="6">
+      <c r="A64" s="4" t="inlineStr">
+        <is>
+          <t>Illusionist's Bracers</t>
+        </is>
+      </c>
+      <c r="B64" s="4" t="inlineStr">
+        <is>
+          <t>Gatecrash</t>
+        </is>
+      </c>
+      <c r="C64" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D64" s="7" t="n">
+        <v>5.06</v>
+      </c>
+    </row>
+    <row r="65" ht="15" customHeight="1" s="6">
+      <c r="A65" s="4" t="inlineStr">
+        <is>
+          <t>Karn, Living Legacy</t>
+        </is>
+      </c>
+      <c r="B65" s="4" t="inlineStr">
+        <is>
+          <t>Dominaria United Promos</t>
+        </is>
+      </c>
+      <c r="C65" s="4" t="inlineStr">
+        <is>
+          <t>V.2</t>
+        </is>
+      </c>
+      <c r="D65" s="7" t="n">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="66" ht="15" customHeight="1" s="6">
+      <c r="A66" s="4" t="inlineStr">
+        <is>
+          <t>Mirror Box</t>
+        </is>
+      </c>
+      <c r="B66" s="4" t="inlineStr">
+        <is>
+          <t>Kamigawa: Neon Dynasty</t>
+        </is>
+      </c>
+      <c r="C66" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D66" s="7" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="67" ht="15" customHeight="1" s="6">
+      <c r="A67" s="4" t="inlineStr">
+        <is>
+          <t>Quicksilver Amulet</t>
+        </is>
+      </c>
+      <c r="B67" s="4" t="inlineStr">
+        <is>
+          <t>Retro Frame Artifacts</t>
+        </is>
+      </c>
+      <c r="C67" s="4" t="inlineStr">
+        <is>
+          <t>V.1</t>
+        </is>
+      </c>
+      <c r="D67" s="7" t="n">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="68" ht="15" customHeight="1" s="6">
+      <c r="A68" s="4" t="inlineStr">
+        <is>
           <t>Swiftfoot Boots</t>
         </is>
       </c>
-      <c r="B56" s="4" t="inlineStr">
+      <c r="B68" s="4" t="inlineStr">
         <is>
           <t>Commander 2017</t>
         </is>
       </c>
-      <c r="C56" s="4" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D56" s="7" t="n">
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="58" ht="15" customHeight="1" s="6">
-      <c r="D58" s="5">
-        <f>SUM(D2:D56)</f>
+      <c r="C68" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D68" s="7" t="n">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="70" ht="15" customHeight="1" s="6">
+      <c r="D70" s="5">
+        <f>SUM(D2:D68)</f>
         <v/>
       </c>
     </row>
-    <row r="1048573" ht="12.75" customHeight="1" s="6"/>
-    <row r="1048574" ht="12.75" customHeight="1" s="6"/>
-    <row r="1048575" ht="12.8" customHeight="1" s="6"/>
-    <row r="1048576" ht="12.8" customHeight="1" s="6"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Only the weekend had passed, and the prices have already dropped
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D2" s="7" t="n">
-        <v>10.5</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D3" s="7" t="n">
-        <v>8.73</v>
+        <v>8.84</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="6">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="D4" s="7" t="n">
-        <v>12.57</v>
+        <v>12.44</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="6">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>15.49</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="6">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>2.88</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D7" s="7" t="n">
-        <v>8.460000000000001</v>
+        <v>8.51</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="6">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="D8" s="7" t="n">
-        <v>7.83</v>
+        <v>7.73</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="6">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="D9" s="7" t="n">
-        <v>5.89</v>
+        <v>5.78</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="6">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="D10" s="7" t="n">
-        <v>25.12</v>
+        <v>24.96</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="6">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>3.43</v>
+        <v>3.29</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>1.28</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="6">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>6.92</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="6">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>3.85</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="6">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>4.52</v>
+        <v>4.82</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="6">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>16.27</v>
+        <v>16.02</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="6">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>3.16</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="6">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>11.88</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="6">
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>4.52</v>
+        <v>4.67</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="6">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>1.43</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="6">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>7.33</v>
+        <v>7.48</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="6">
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>2.86</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="6">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>3.18</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="6">
@@ -1037,7 +1037,7 @@
         </is>
       </c>
       <c r="D28" s="7" t="n">
-        <v>4.71</v>
+        <v>4.69</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="6">
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="D29" s="7" t="n">
-        <v>0.88</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="6">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="D30" s="7" t="n">
-        <v>1.85</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1" s="6">
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="D31" s="7" t="n">
-        <v>2.32</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="6">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D32" s="7" t="n">
-        <v>1.56</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="6">
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="D33" s="7" t="n">
-        <v>2.95</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="6">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="D34" s="7" t="n">
-        <v>10.7</v>
+        <v>10.79</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="6">
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="D36" s="7" t="n">
-        <v>1.86</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="6">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D37" s="7" t="n">
-        <v>5.07</v>
+        <v>5.41</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="6">
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="D38" s="7" t="n">
-        <v>27.97</v>
+        <v>25.66</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="6">
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="D39" s="7" t="n">
-        <v>3.2</v>
+        <v>2.47</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="6">
@@ -1277,7 +1277,7 @@
         </is>
       </c>
       <c r="D40" s="7" t="n">
-        <v>0.82</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="6">
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="D41" s="7" t="n">
-        <v>2.39</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="6">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="D44" s="7" t="n">
-        <v>1.07</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="6">
@@ -1377,7 +1377,7 @@
         </is>
       </c>
       <c r="D45" s="7" t="n">
-        <v>1.08</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" s="6">
@@ -1397,7 +1397,7 @@
         </is>
       </c>
       <c r="D46" s="7" t="n">
-        <v>3.51</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="6">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="D47" s="7" t="n">
-        <v>7.76</v>
+        <v>8.050000000000001</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="6">
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="D48" s="7" t="n">
-        <v>3.94</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="6">
@@ -1497,7 +1497,7 @@
         </is>
       </c>
       <c r="D51" s="7" t="n">
-        <v>6.26</v>
+        <v>6.09</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" s="6">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D52" s="7" t="n">
-        <v>1.91</v>
+        <v>1.93</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" s="6">
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="D54" s="7" t="n">
-        <v>4.22</v>
+        <v>4.06</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="6">
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="D55" s="7" t="n">
-        <v>1.43</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="6">
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="D56" s="7" t="n">
-        <v>11.48</v>
+        <v>11.06</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" s="6">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D57" s="7" t="n">
-        <v>8.07</v>
+        <v>8.17</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" s="6">
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="D59" s="7" t="n">
-        <v>1.84</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" s="6">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="D60" s="7" t="n">
-        <v>9.06</v>
+        <v>9.35</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" s="6">
@@ -1697,7 +1697,7 @@
         </is>
       </c>
       <c r="D61" s="7" t="n">
-        <v>9.23</v>
+        <v>8.68</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" s="6">
@@ -1717,7 +1717,7 @@
         </is>
       </c>
       <c r="D62" s="7" t="n">
-        <v>3.8</v>
+        <v>3.63</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" s="6">
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="D63" s="7" t="n">
-        <v>1.94</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" s="6">
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="D64" s="7" t="n">
-        <v>5.06</v>
+        <v>5.48</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" s="6">
@@ -1817,7 +1817,7 @@
         </is>
       </c>
       <c r="D67" s="7" t="n">
-        <v>0.97</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1" s="6">

</xml_diff>

<commit_message>
Not much has changed
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D2" s="7" t="n">
-        <v>10.7</v>
+        <v>10.83</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D3" s="7" t="n">
-        <v>8.84</v>
+        <v>8.92</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="6">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="D4" s="7" t="n">
-        <v>12.44</v>
+        <v>12.35</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="6">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>15.25</v>
+        <v>15.29</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="6">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>3.21</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D7" s="7" t="n">
-        <v>8.51</v>
+        <v>8.44</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="6">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="D8" s="7" t="n">
-        <v>7.73</v>
+        <v>7.64</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="6">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="D9" s="7" t="n">
-        <v>5.78</v>
+        <v>5.63</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="6">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="D10" s="7" t="n">
-        <v>24.96</v>
+        <v>24.72</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>1.19</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="6">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>3.29</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>1.26</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="6">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>6.8</v>
+        <v>6.74</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="6">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>3.83</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="6">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>4.82</v>
+        <v>4.77</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="6">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>16.02</v>
+        <v>16.13</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="6">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>3.08</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="6">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>12.7</v>
+        <v>12.93</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="6">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>1.33</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="6">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>7.48</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="6">
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>2.87</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="6">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>3.36</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="6">
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="D26" s="7" t="n">
-        <v>5.21</v>
+        <v>5.22</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="6">
@@ -1037,7 +1037,7 @@
         </is>
       </c>
       <c r="D28" s="7" t="n">
-        <v>4.69</v>
+        <v>4.62</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="6">
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="D29" s="7" t="n">
-        <v>0.79</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="6">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="D30" s="7" t="n">
-        <v>1.48</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1" s="6">
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="D31" s="7" t="n">
-        <v>2.25</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="6">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D32" s="7" t="n">
-        <v>1.49</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="6">
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="D33" s="7" t="n">
-        <v>2.85</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="6">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D37" s="7" t="n">
-        <v>5.41</v>
+        <v>5.47</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="6">
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="D38" s="7" t="n">
-        <v>25.66</v>
+        <v>26.63</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="6">
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="D39" s="7" t="n">
-        <v>2.47</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="6">
@@ -1277,7 +1277,7 @@
         </is>
       </c>
       <c r="D40" s="7" t="n">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="6">
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="D41" s="7" t="n">
-        <v>2.31</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="6">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D42" s="7" t="n">
-        <v>3.77</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="6">
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="D43" s="7" t="n">
-        <v>3.45</v>
+        <v>3.37</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="6">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="D44" s="7" t="n">
-        <v>1</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="6">
@@ -1397,7 +1397,7 @@
         </is>
       </c>
       <c r="D46" s="7" t="n">
-        <v>3.42</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="6">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="D47" s="7" t="n">
-        <v>8.050000000000001</v>
+        <v>8.01</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="6">
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="D48" s="7" t="n">
-        <v>3.95</v>
+        <v>4.32</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="6">
@@ -1497,7 +1497,7 @@
         </is>
       </c>
       <c r="D51" s="7" t="n">
-        <v>6.09</v>
+        <v>6.07</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" s="6">
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="D53" s="7" t="n">
-        <v>3.59</v>
+        <v>3.69</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="6">
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="D54" s="7" t="n">
-        <v>4.06</v>
+        <v>4.02</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="6">
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="D55" s="7" t="n">
-        <v>1.37</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="6">
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="D56" s="7" t="n">
-        <v>11.06</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" s="6">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D57" s="7" t="n">
-        <v>8.17</v>
+        <v>8.35</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" s="6">
@@ -1637,7 +1637,7 @@
         </is>
       </c>
       <c r="D58" s="7" t="n">
-        <v>17.45</v>
+        <v>17.04</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" s="6">
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="D59" s="7" t="n">
-        <v>1.66</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" s="6">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="D60" s="7" t="n">
-        <v>9.35</v>
+        <v>9.42</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" s="6">
@@ -1697,7 +1697,7 @@
         </is>
       </c>
       <c r="D61" s="7" t="n">
-        <v>8.68</v>
+        <v>8.539999999999999</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" s="6">
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="D63" s="7" t="n">
-        <v>1.89</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" s="6">
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="D64" s="7" t="n">
-        <v>5.48</v>
+        <v>5.55</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" s="6">
@@ -1797,7 +1797,7 @@
         </is>
       </c>
       <c r="D66" s="7" t="n">
-        <v>1.1</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" s="6">
@@ -1817,7 +1817,7 @@
         </is>
       </c>
       <c r="D67" s="7" t="n">
-        <v>0.31</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1" s="6">

</xml_diff>

<commit_message>
I can't compete with the riders in the other heats
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D2" s="7" t="n">
-        <v>10.83</v>
+        <v>10.86</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D3" s="7" t="n">
-        <v>8.92</v>
+        <v>9.039999999999999</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="6">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="D4" s="7" t="n">
-        <v>12.35</v>
+        <v>12.41</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="6">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>15.29</v>
+        <v>15.42</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="6">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>3.11</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D7" s="7" t="n">
-        <v>8.44</v>
+        <v>8.539999999999999</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="6">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="D8" s="7" t="n">
-        <v>7.64</v>
+        <v>7.66</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="6">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="D9" s="7" t="n">
-        <v>5.63</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="6">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="D10" s="7" t="n">
-        <v>24.72</v>
+        <v>25.09</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>1.21</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="6">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>3.23</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>1.27</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="6">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>6.74</v>
+        <v>6.46</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="6">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>3.87</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="6">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>4.77</v>
+        <v>4.68</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="6">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>16.13</v>
+        <v>16.1</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="6">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>3.14</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="6">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>12.93</v>
+        <v>13.12</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="6">
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>4.67</v>
+        <v>4.85</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="6">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>1.36</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="6">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>7.3</v>
+        <v>7.26</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="6">
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>2.96</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="6">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>3.32</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="6">
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="D26" s="7" t="n">
-        <v>5.22</v>
+        <v>5.19</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="6">
@@ -1037,7 +1037,7 @@
         </is>
       </c>
       <c r="D28" s="7" t="n">
-        <v>4.62</v>
+        <v>4.57</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="6">
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="D29" s="7" t="n">
-        <v>0.78</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="6">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="D30" s="7" t="n">
-        <v>1.37</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1" s="6">
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="D31" s="7" t="n">
-        <v>2.26</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="6">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D32" s="7" t="n">
-        <v>1.41</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="6">
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="D33" s="7" t="n">
-        <v>2.78</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="6">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="D34" s="7" t="n">
-        <v>10.79</v>
+        <v>11.02</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="6">
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="D36" s="7" t="n">
-        <v>1.85</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="6">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D37" s="7" t="n">
-        <v>5.47</v>
+        <v>5.38</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="6">
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="D38" s="7" t="n">
-        <v>26.63</v>
+        <v>26.58</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="6">
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="D39" s="7" t="n">
-        <v>2.12</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="6">
@@ -1277,7 +1277,7 @@
         </is>
       </c>
       <c r="D40" s="7" t="n">
-        <v>0.93</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="6">
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="D43" s="7" t="n">
-        <v>3.37</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="6">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="D44" s="7" t="n">
-        <v>0.96</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="6">
@@ -1377,7 +1377,7 @@
         </is>
       </c>
       <c r="D45" s="7" t="n">
-        <v>1.06</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" s="6">
@@ -1397,7 +1397,7 @@
         </is>
       </c>
       <c r="D46" s="7" t="n">
-        <v>3.35</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="6">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="D47" s="7" t="n">
-        <v>8.01</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="6">
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="D48" s="7" t="n">
-        <v>4.32</v>
+        <v>4.22</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="6">
@@ -1457,7 +1457,7 @@
         </is>
       </c>
       <c r="D49" s="7" t="n">
-        <v>1.24</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" s="6">
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="D50" s="7" t="n">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" s="6">
@@ -1497,7 +1497,7 @@
         </is>
       </c>
       <c r="D51" s="7" t="n">
-        <v>6.07</v>
+        <v>6.09</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" s="6">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D52" s="7" t="n">
-        <v>1.93</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" s="6">
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="D53" s="7" t="n">
-        <v>3.69</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="6">
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="D54" s="7" t="n">
-        <v>4.02</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="6">
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="D55" s="7" t="n">
-        <v>1.35</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="6">
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="D56" s="7" t="n">
-        <v>11.1</v>
+        <v>10.86</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" s="6">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D57" s="7" t="n">
-        <v>8.35</v>
+        <v>8.07</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" s="6">
@@ -1637,7 +1637,7 @@
         </is>
       </c>
       <c r="D58" s="7" t="n">
-        <v>17.04</v>
+        <v>16.79</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" s="6">
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="D59" s="7" t="n">
-        <v>1.57</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" s="6">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="D60" s="7" t="n">
-        <v>9.42</v>
+        <v>9.16</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" s="6">
@@ -1697,7 +1697,7 @@
         </is>
       </c>
       <c r="D61" s="7" t="n">
-        <v>8.539999999999999</v>
+        <v>8.94</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" s="6">
@@ -1717,7 +1717,7 @@
         </is>
       </c>
       <c r="D62" s="7" t="n">
-        <v>3.63</v>
+        <v>3.71</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" s="6">
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="D63" s="7" t="n">
-        <v>1.88</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" s="6">
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="D64" s="7" t="n">
-        <v>5.55</v>
+        <v>6.06</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" s="6">
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="D65" s="7" t="n">
-        <v>3.84</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" s="6">
@@ -1797,7 +1797,7 @@
         </is>
       </c>
       <c r="D66" s="7" t="n">
-        <v>1.08</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" s="6">
@@ -1817,7 +1817,7 @@
         </is>
       </c>
       <c r="D67" s="7" t="n">
-        <v>0.11</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1" s="6">

</xml_diff>

<commit_message>
I hear the secrets that you keep
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D2" s="7" t="n">
-        <v>10.76</v>
+        <v>10.33</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D3" s="7" t="n">
-        <v>8.789999999999999</v>
+        <v>8.779999999999999</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="6">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="D4" s="7" t="n">
-        <v>12.13</v>
+        <v>12.39</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="6">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>15.81</v>
+        <v>15.87</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D7" s="7" t="n">
-        <v>8.6</v>
+        <v>8.460000000000001</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="6">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="D9" s="7" t="n">
-        <v>5.75</v>
+        <v>5.92</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="6">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="D10" s="7" t="n">
-        <v>25.14</v>
+        <v>24.02</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>1.21</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="6">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>2.97</v>
+        <v>2.84</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>1.29</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="6">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>6.62</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="6">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>3.78</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="6">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>4.58</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="6">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>16.2</v>
+        <v>16.54</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="6">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>3.38</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="6">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>13.08</v>
+        <v>12.75</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="6">
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>4.85</v>
+        <v>4.83</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="6">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>1.31</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="6">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>7.09</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="6">
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>3.15</v>
+        <v>2.91</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="6">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>3.47</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="6">
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="D26" s="7" t="n">
-        <v>5.11</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="6">
@@ -1037,7 +1037,7 @@
         </is>
       </c>
       <c r="D28" s="7" t="n">
-        <v>4.46</v>
+        <v>4.37</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="6">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="D30" s="7" t="n">
-        <v>1.07</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1" s="6">
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="D31" s="7" t="n">
-        <v>2.05</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="6">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D32" s="7" t="n">
-        <v>1.37</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="6">
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="D33" s="7" t="n">
-        <v>2.93</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="6">
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="D36" s="7" t="n">
-        <v>1.94</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="6">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D37" s="7" t="n">
-        <v>5.43</v>
+        <v>5.38</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="6">
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="D38" s="7" t="n">
-        <v>24.75</v>
+        <v>25.98</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="6">
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="D39" s="7" t="n">
-        <v>1.15</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="6">
@@ -1277,7 +1277,7 @@
         </is>
       </c>
       <c r="D40" s="7" t="n">
-        <v>1.08</v>
+        <v>1.11</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="6">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D42" s="7" t="n">
-        <v>3.67</v>
+        <v>3.63</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="6">
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="D43" s="7" t="n">
-        <v>3.31</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="6">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="D44" s="7" t="n">
-        <v>0.73</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="6">
@@ -1397,7 +1397,7 @@
         </is>
       </c>
       <c r="D46" s="7" t="n">
-        <v>3.46</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="6">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="D47" s="7" t="n">
-        <v>7.92</v>
+        <v>8.380000000000001</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="6">
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="D48" s="7" t="n">
-        <v>4.21</v>
+        <v>4.35</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="6">
@@ -1457,7 +1457,7 @@
         </is>
       </c>
       <c r="D49" s="7" t="n">
-        <v>1.26</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" s="6">
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="D50" s="7" t="n">
-        <v>2.03</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" s="6">
@@ -1497,7 +1497,7 @@
         </is>
       </c>
       <c r="D51" s="7" t="n">
-        <v>6.03</v>
+        <v>6.07</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" s="6">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D52" s="7" t="n">
-        <v>2.05</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" s="6">
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="D53" s="7" t="n">
-        <v>3.57</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="6">
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="D54" s="7" t="n">
-        <v>3.56</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="6">
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="D55" s="7" t="n">
-        <v>1.45</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="6">
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="D56" s="7" t="n">
-        <v>11.02</v>
+        <v>10.99</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" s="6">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D57" s="7" t="n">
-        <v>8.359999999999999</v>
+        <v>8.58</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" s="6">
@@ -1637,7 +1637,7 @@
         </is>
       </c>
       <c r="D58" s="7" t="n">
-        <v>16.75</v>
+        <v>16.33</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" s="6">
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="D59" s="7" t="n">
-        <v>1.54</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" s="6">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="D60" s="7" t="n">
-        <v>8.9</v>
+        <v>8.859999999999999</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" s="6">
@@ -1697,7 +1697,7 @@
         </is>
       </c>
       <c r="D61" s="7" t="n">
-        <v>8.99</v>
+        <v>9.029999999999999</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" s="6">
@@ -1717,7 +1717,7 @@
         </is>
       </c>
       <c r="D62" s="7" t="n">
-        <v>3.78</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" s="6">
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="D63" s="7" t="n">
-        <v>1.85</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" s="6">
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="D64" s="7" t="n">
-        <v>5.59</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" s="6">
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="D65" s="7" t="n">
-        <v>3.53</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" s="6">
@@ -1797,7 +1797,7 @@
         </is>
       </c>
       <c r="D66" s="7" t="n">
-        <v>0.99</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" s="6">

</xml_diff>

<commit_message>
When you're talking in your sleep
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D2" s="7" t="n">
-        <v>10.33</v>
+        <v>10.13</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="6">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="D4" s="7" t="n">
-        <v>12.39</v>
+        <v>12.28</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="6">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>15.87</v>
+        <v>15.72</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="6">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>2.83</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D7" s="7" t="n">
-        <v>8.460000000000001</v>
+        <v>8.59</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="6">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="D8" s="7" t="n">
-        <v>7.58</v>
+        <v>7.56</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="6">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="D9" s="7" t="n">
-        <v>5.92</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="6">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="D10" s="7" t="n">
-        <v>24.02</v>
+        <v>24.16</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>1.26</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="6">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>2.84</v>
+        <v>2.82</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>1.24</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="6">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>6.4</v>
+        <v>6.45</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="6">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>4.4</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="6">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>16.54</v>
+        <v>16.71</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="6">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>3.5</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="6">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>12.75</v>
+        <v>12.64</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="6">
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>4.83</v>
+        <v>4.81</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="6">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>1.47</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="6">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>6.84</v>
+        <v>6.69</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="6">
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>2.91</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="6">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>3.59</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="6">
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="D26" s="7" t="n">
-        <v>4.95</v>
+        <v>4.91</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="6">
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="D29" s="7" t="n">
-        <v>0.62</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="6">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="D30" s="7" t="n">
-        <v>0.96</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1" s="6">
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="D31" s="7" t="n">
-        <v>2.08</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="6">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="D34" s="7" t="n">
-        <v>10.1</v>
+        <v>9.960000000000001</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="6">
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="D36" s="7" t="n">
-        <v>1.79</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="6">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D37" s="7" t="n">
-        <v>5.38</v>
+        <v>5.22</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="6">
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="D38" s="7" t="n">
-        <v>25.98</v>
+        <v>25.33</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="6">
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="D39" s="7" t="n">
-        <v>0.93</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="6">
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="D41" s="7" t="n">
-        <v>2.1</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="6">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D42" s="7" t="n">
-        <v>3.63</v>
+        <v>3.64</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="6">
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="D43" s="7" t="n">
-        <v>3.18</v>
+        <v>3.16</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="6">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="D44" s="7" t="n">
-        <v>0.66</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="6">
@@ -1397,7 +1397,7 @@
         </is>
       </c>
       <c r="D46" s="7" t="n">
-        <v>3.44</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="6">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="D47" s="7" t="n">
-        <v>8.380000000000001</v>
+        <v>8.140000000000001</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="6">
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="D53" s="7" t="n">
-        <v>3.54</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="6">
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="D54" s="7" t="n">
-        <v>3.57</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="6">
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="D56" s="7" t="n">
-        <v>10.99</v>
+        <v>11.01</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" s="6">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D57" s="7" t="n">
-        <v>8.58</v>
+        <v>8.51</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" s="6">
@@ -1637,7 +1637,7 @@
         </is>
       </c>
       <c r="D58" s="7" t="n">
-        <v>16.33</v>
+        <v>16.45</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" s="6">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="D60" s="7" t="n">
-        <v>8.859999999999999</v>
+        <v>8.74</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" s="6">
@@ -1697,7 +1697,7 @@
         </is>
       </c>
       <c r="D61" s="7" t="n">
-        <v>9.029999999999999</v>
+        <v>8.970000000000001</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" s="6">
@@ -1717,7 +1717,7 @@
         </is>
       </c>
       <c r="D62" s="7" t="n">
-        <v>3.52</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" s="6">
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="D63" s="7" t="n">
-        <v>1.83</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" s="6">
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="D64" s="7" t="n">
-        <v>5.6</v>
+        <v>5.58</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" s="6">
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="D65" s="7" t="n">
-        <v>3.61</v>
+        <v>3.81</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" s="6">
@@ -1797,7 +1797,7 @@
         </is>
       </c>
       <c r="D66" s="7" t="n">
-        <v>1.01</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" s="6">

</xml_diff>

<commit_message>
Argoth promo appeared on the market
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -466,7 +466,7 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
+      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D2" s="7" t="n">
-        <v>10.13</v>
+        <v>9.99</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D3" s="7" t="n">
-        <v>8.779999999999999</v>
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="6">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="D4" s="7" t="n">
-        <v>12.28</v>
+        <v>12.36</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="6">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>15.72</v>
+        <v>16.01</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="6">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>2.8</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D7" s="7" t="n">
-        <v>8.59</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="6">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="D8" s="7" t="n">
-        <v>7.56</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="6">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="D10" s="7" t="n">
-        <v>24.16</v>
+        <v>23.49</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>1.27</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="6">
@@ -708,16 +708,16 @@
       </c>
       <c r="B12" s="4" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>The Brothers' War Promos</t>
         </is>
       </c>
       <c r="C12" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>2.82</v>
+        <v>5.93</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>1.2</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="6">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>6.45</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="6">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>3.75</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="6">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>4.41</v>
+        <v>4.29</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="6">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>16.71</v>
+        <v>16.75</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="6">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>3.42</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="6">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>12.64</v>
+        <v>11.78</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="6">
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>4.81</v>
+        <v>4.66</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="6">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>1.51</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="6">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>6.69</v>
+        <v>6.72</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="6">
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>2.9</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="6">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>3.61</v>
+        <v>3.68</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="6">
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="D26" s="7" t="n">
-        <v>4.91</v>
+        <v>4.76</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="6">
@@ -1037,7 +1037,7 @@
         </is>
       </c>
       <c r="D28" s="7" t="n">
-        <v>4.37</v>
+        <v>4.36</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="6">
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="D29" s="7" t="n">
-        <v>0.58</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="6">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="D30" s="7" t="n">
-        <v>0.93</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1" s="6">
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="D31" s="7" t="n">
-        <v>2</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="6">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D32" s="7" t="n">
-        <v>1.43</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="6">
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="D33" s="7" t="n">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="6">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="D34" s="7" t="n">
-        <v>9.960000000000001</v>
+        <v>9.779999999999999</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="6">
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="D36" s="7" t="n">
-        <v>1.85</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="6">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D37" s="7" t="n">
-        <v>5.22</v>
+        <v>5.28</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="6">
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="D38" s="7" t="n">
-        <v>25.33</v>
+        <v>24.87</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="6">
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="D39" s="7" t="n">
-        <v>0.85</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="6">
@@ -1277,7 +1277,7 @@
         </is>
       </c>
       <c r="D40" s="7" t="n">
-        <v>1.11</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="6">
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="D41" s="7" t="n">
-        <v>2.05</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="6">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D42" s="7" t="n">
-        <v>3.64</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="6">
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="D43" s="7" t="n">
-        <v>3.16</v>
+        <v>3.43</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="6">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="D44" s="7" t="n">
-        <v>0.76</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="6">
@@ -1377,7 +1377,7 @@
         </is>
       </c>
       <c r="D45" s="7" t="n">
-        <v>1.09</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" s="6">
@@ -1397,7 +1397,7 @@
         </is>
       </c>
       <c r="D46" s="7" t="n">
-        <v>3.62</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="6">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="D47" s="7" t="n">
-        <v>8.140000000000001</v>
+        <v>8.02</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="6">
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="D48" s="7" t="n">
-        <v>4.35</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="6">
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="D50" s="7" t="n">
-        <v>1.78</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" s="6">
@@ -1497,7 +1497,7 @@
         </is>
       </c>
       <c r="D51" s="7" t="n">
-        <v>6.07</v>
+        <v>5.84</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" s="6">
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="D53" s="7" t="n">
-        <v>3.47</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="6">
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="D54" s="7" t="n">
-        <v>3.53</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="6">
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="D55" s="7" t="n">
-        <v>1.44</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="6">
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="D56" s="7" t="n">
-        <v>11.01</v>
+        <v>10.89</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" s="6">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D57" s="7" t="n">
-        <v>8.51</v>
+        <v>8.539999999999999</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" s="6">
@@ -1637,7 +1637,7 @@
         </is>
       </c>
       <c r="D58" s="7" t="n">
-        <v>16.45</v>
+        <v>16.63</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" s="6">
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="D59" s="7" t="n">
-        <v>1.34</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" s="6">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="D60" s="7" t="n">
-        <v>8.74</v>
+        <v>8.81</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" s="6">
@@ -1697,7 +1697,7 @@
         </is>
       </c>
       <c r="D61" s="7" t="n">
-        <v>8.970000000000001</v>
+        <v>8.69</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" s="6">
@@ -1717,7 +1717,7 @@
         </is>
       </c>
       <c r="D62" s="7" t="n">
-        <v>3.5</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" s="6">
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="D63" s="7" t="n">
-        <v>1.66</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" s="6">
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="D64" s="7" t="n">
-        <v>5.58</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" s="6">
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="D65" s="7" t="n">
-        <v>3.81</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" s="6">
@@ -1797,7 +1797,7 @@
         </is>
       </c>
       <c r="D66" s="7" t="n">
-        <v>0.97</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" s="6">
@@ -1837,7 +1837,7 @@
         </is>
       </c>
       <c r="D68" s="7" t="n">
-        <v>1.63</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1" s="6">

</xml_diff>

<commit_message>
The prices have plummet
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D2" s="7" t="n">
-        <v>10.01</v>
+        <v>9.470000000000001</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D3" s="7" t="n">
-        <v>8.789999999999999</v>
+        <v>8.68</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="6">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="D4" s="7" t="n">
-        <v>12.66</v>
+        <v>13.29</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="6">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>16.81</v>
+        <v>16.93</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="6">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>2.94</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D7" s="7" t="n">
-        <v>8.82</v>
+        <v>9.07</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="6">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="D8" s="7" t="n">
-        <v>7.9</v>
+        <v>7.47</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="6">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="D9" s="7" t="n">
-        <v>5.37</v>
+        <v>5.51</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="6">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="D10" s="7" t="n">
-        <v>25.08</v>
+        <v>24.51</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>1</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="6">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>1.15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>6.74</v>
+        <v>5.93</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="6">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>1.33</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="6">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>6.37</v>
+        <v>6.52</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="6">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>3.58</v>
+        <v>3.71</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="6">
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>1.58</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="6">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>1.07</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="6">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>1.34</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="6">
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>17.13</v>
+        <v>15.69</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="6">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>3.88</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="6">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>9.19</v>
+        <v>8.130000000000001</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="6">
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>4.22</v>
+        <v>4.56</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="6">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>1.38</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="6">
@@ -977,7 +977,7 @@
         </is>
       </c>
       <c r="D25" s="7" t="n">
-        <v>5.96</v>
+        <v>6.66</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" s="6">
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="D26" s="7" t="n">
-        <v>2.84</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="6">
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="D27" s="7" t="n">
-        <v>6.34</v>
+        <v>8.359999999999999</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" s="6">
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="D29" s="7" t="n">
-        <v>4.99</v>
+        <v>4.96</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="6">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="D30" s="7" t="n">
-        <v>0.82</v>
+        <v>0.8100000000000001</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" s="6">
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="D31" s="7" t="n">
-        <v>4.26</v>
+        <v>4.21</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="6">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D32" s="7" t="n">
-        <v>0.38</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="6">
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="D33" s="7" t="n">
-        <v>1.13</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1" s="6">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="D34" s="7" t="n">
-        <v>1.9</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="6">
@@ -1177,7 +1177,7 @@
         </is>
       </c>
       <c r="D35" s="7" t="n">
-        <v>1.68</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" s="6">
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="D36" s="7" t="n">
-        <v>2.85</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="6">
@@ -1217,7 +1217,7 @@
         </is>
       </c>
       <c r="D37" s="7" t="n">
-        <v>9.56</v>
+        <v>9.93</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="6">
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="D39" s="7" t="n">
-        <v>1.62</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="6">
@@ -1277,7 +1277,7 @@
         </is>
       </c>
       <c r="D40" s="7" t="n">
-        <v>4.84</v>
+        <v>5.07</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="6">
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="D41" s="7" t="n">
-        <v>27.18</v>
+        <v>26.16</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="6">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D42" s="7" t="n">
-        <v>0.42</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="6">
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="D43" s="7" t="n">
-        <v>1.27</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="6">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="D44" s="7" t="n">
-        <v>1.72</v>
+        <v>2.03</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="6">
@@ -1397,7 +1397,7 @@
         </is>
       </c>
       <c r="D46" s="7" t="n">
-        <v>3.41</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="6">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="D47" s="7" t="n">
-        <v>0.92</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="6">
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="D48" s="7" t="n">
-        <v>1.49</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="6">
@@ -1457,7 +1457,7 @@
         </is>
       </c>
       <c r="D49" s="7" t="n">
-        <v>4.22</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" s="6">
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="D50" s="7" t="n">
-        <v>2.98</v>
+        <v>2.91</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" s="6">
@@ -1497,7 +1497,7 @@
         </is>
       </c>
       <c r="D51" s="7" t="n">
-        <v>7.05</v>
+        <v>6.44</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" s="6">
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="D52" s="7" t="n">
-        <v>3.53</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" s="6">
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="D53" s="7" t="n">
-        <v>1.84</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="6">
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="D54" s="7" t="n">
-        <v>1.61</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="6">
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="D55" s="7" t="n">
-        <v>6.12</v>
+        <v>6.02</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="6">
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="D56" s="7" t="n">
-        <v>1.71</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" s="6">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D57" s="7" t="n">
-        <v>3.22</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" s="6">
@@ -1637,7 +1637,7 @@
         </is>
       </c>
       <c r="D58" s="7" t="n">
-        <v>4.68</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" s="6">
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="D59" s="7" t="n">
-        <v>1.47</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" s="6">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="D60" s="7" t="n">
-        <v>10.59</v>
+        <v>10.73</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" s="6">
@@ -1697,7 +1697,7 @@
         </is>
       </c>
       <c r="D61" s="7" t="n">
-        <v>7.63</v>
+        <v>8.16</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" s="6">
@@ -1717,7 +1717,7 @@
         </is>
       </c>
       <c r="D62" s="7" t="n">
-        <v>17.7</v>
+        <v>17.87</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" s="6">
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="D63" s="7" t="n">
-        <v>1.22</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" s="6">
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="D64" s="7" t="n">
-        <v>9.34</v>
+        <v>9.710000000000001</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" s="6">
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="D65" s="7" t="n">
-        <v>9.42</v>
+        <v>9.07</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" s="6">
@@ -1797,7 +1797,7 @@
         </is>
       </c>
       <c r="D66" s="7" t="n">
-        <v>3.69</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" s="6">
@@ -1817,7 +1817,7 @@
         </is>
       </c>
       <c r="D67" s="7" t="n">
-        <v>2.07</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1" s="6">
@@ -1837,7 +1837,7 @@
         </is>
       </c>
       <c r="D68" s="7" t="n">
-        <v>5.14</v>
+        <v>5.21</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1" s="6">
@@ -1857,7 +1857,7 @@
         </is>
       </c>
       <c r="D69" s="7" t="n">
-        <v>3.89</v>
+        <v>3.98</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1" s="6">
@@ -1877,7 +1877,7 @@
         </is>
       </c>
       <c r="D70" s="7" t="n">
-        <v>1.07</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1" s="6">
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="D71" s="7" t="n">
-        <v>0.45</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1" s="6">
@@ -1917,7 +1917,7 @@
         </is>
       </c>
       <c r="D72" s="7" t="n">
-        <v>1.56</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1" s="6">

</xml_diff>

<commit_message>
Added pulls from the collector's booster
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -463,10 +463,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D54" activeCellId="0" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D3" s="7" t="n">
-        <v>8.57</v>
+        <v>8.58</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="6">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="D4" s="7" t="n">
-        <v>13.43</v>
+        <v>13.67</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="6">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>16.91</v>
+        <v>16.88</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="6">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>2.64</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D7" s="7" t="n">
-        <v>9.09</v>
+        <v>9.039999999999999</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="6">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="D8" s="7" t="n">
-        <v>7.54</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="6">
@@ -677,18 +677,18 @@
         </is>
       </c>
       <c r="D10" s="7" t="n">
-        <v>24.82</v>
+        <v>24.94</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>Argoth, Sanctum of Nature: Titania, Gaea Incarnate</t>
+          <t>Yavimaya Coast</t>
         </is>
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>The Brothers' War Promos</t>
+          <t>Dominaria United: Extras</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr">
@@ -697,18 +697,18 @@
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>5.45</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="6">
       <c r="A12" s="4" t="inlineStr">
         <is>
-          <t>Lair of the Hydra</t>
+          <t>Argoth, Sanctum of Nature: Titania, Gaea Incarnate</t>
         </is>
       </c>
       <c r="B12" s="4" t="inlineStr">
         <is>
-          <t>Adventures in the Forgotten Realms</t>
+          <t>The Brothers' War Promos</t>
         </is>
       </c>
       <c r="C12" s="4" t="inlineStr">
@@ -717,18 +717,18 @@
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>1.39</v>
+        <v>5.19</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>Ajani Steadfast</t>
+          <t>Lair of the Hydra</t>
         </is>
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>Magic 2015</t>
+          <t>Adventures in the Forgotten Realms</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr">
@@ -737,18 +737,18 @@
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>6.43</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="6">
       <c r="A14" s="4" t="inlineStr">
         <is>
-          <t>Sage of Hours</t>
+          <t>Ajani Steadfast</t>
         </is>
       </c>
       <c r="B14" s="4" t="inlineStr">
         <is>
-          <t>Journey into Nyx</t>
+          <t>Magic 2015</t>
         </is>
       </c>
       <c r="C14" s="4" t="inlineStr">
@@ -757,18 +757,18 @@
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>3.87</v>
+        <v>6.48</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="6">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Ancient Brass Dragon</t>
+          <t>Sage of Hours</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Journey into Nyx</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr">
@@ -777,18 +777,18 @@
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>15</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="6">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>Dark Petition</t>
+          <t>Ancient Brass Dragon</t>
         </is>
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>Magic Origins</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C16" s="4" t="inlineStr">
@@ -797,18 +797,18 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>3.81</v>
+        <v>14.99</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="6">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>Diabolic Intent</t>
+          <t>Dark Petition</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Magic Origins</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr">
@@ -817,18 +817,18 @@
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>7.56</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="6">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>Gravecrawler</t>
+          <t>Diabolic Intent</t>
         </is>
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C18" s="4" t="inlineStr">
@@ -837,138 +837,138 @@
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>4.39</v>
+        <v>7.56</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="6">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>Scourge of the Skyclaves</t>
+          <t>Gravecrawler</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>Zendikar Rising Promos</t>
+          <t>Dark Ascension</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
         <is>
-          <t>V.1</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>0.93</v>
+        <v>4.43</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="6">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>Tree of Perdition</t>
+          <t>Scourge of the Skyclaves</t>
         </is>
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>Eldritch Moon</t>
+          <t>Zendikar Rising Promos</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>V.1</t>
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>6.12</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="6">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Deadly Dispute</t>
+          <t>Tree of Perdition</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Eldritch Moon</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>2.82</v>
+        <v>6.12</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="6">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Brotherhood's End</t>
+          <t>Deadly Dispute</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>8.24</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="6">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>Flame-Wreathed Phoenix</t>
+          <t>Brotherhood's End</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>1.58</v>
+        <v>8.19</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="6">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>Shivan Devastator</t>
+          <t>Flame-Wreathed Phoenix</t>
         </is>
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C24" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>5.04</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="6">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>Vexing Devil</t>
+          <t>Shivan Devastator</t>
         </is>
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>Avacyn Restored</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
@@ -977,78 +977,78 @@
         </is>
       </c>
       <c r="D25" s="7" t="n">
-        <v>3.8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" s="6">
       <c r="A26" s="4" t="inlineStr">
         <is>
+          <t>Vexing Devil</t>
+        </is>
+      </c>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>Avacyn Restored</t>
+        </is>
+      </c>
+      <c r="C26" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D26" s="7" t="n">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="27" ht="15" customHeight="1" s="6">
+      <c r="A27" s="4" t="inlineStr">
+        <is>
           <t>Fauna Shaman</t>
         </is>
       </c>
-      <c r="B26" s="4" t="inlineStr">
+      <c r="B27" s="4" t="inlineStr">
         <is>
           <t>The Brothers' War</t>
         </is>
       </c>
-      <c r="C26" s="4" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D26" s="7" t="n">
+      <c r="C27" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D27" s="7" t="n">
         <v>1.04</v>
       </c>
     </row>
-    <row r="27" ht="13.5" customHeight="1" s="6">
-      <c r="A27" s="4" t="inlineStr">
+    <row r="28" ht="13.5" customHeight="1" s="6">
+      <c r="A28" s="4" t="inlineStr">
         <is>
           <t>Fyndhorn Elves</t>
         </is>
       </c>
-      <c r="B27" s="4" t="inlineStr">
+      <c r="B28" s="4" t="inlineStr">
         <is>
           <t>30th Anniversary Celebration</t>
         </is>
       </c>
-      <c r="C27" s="4" t="inlineStr">
+      <c r="C28" s="4" t="inlineStr">
         <is>
           <t>German</t>
         </is>
       </c>
-      <c r="D27" s="7" t="n">
-        <v>1.91</v>
-      </c>
-    </row>
-    <row r="28" ht="15" customHeight="1" s="6">
-      <c r="A28" s="4" t="inlineStr">
-        <is>
-          <t>Gyre Sage</t>
-        </is>
-      </c>
-      <c r="B28" s="4" t="inlineStr">
-        <is>
-          <t>Gatecrash</t>
-        </is>
-      </c>
-      <c r="C28" s="4" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
       <c r="D28" s="7" t="n">
-        <v>1.3</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="6">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>Hardened Scales</t>
+          <t>Gyre Sage</t>
         </is>
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>Khans of Tarkir</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
@@ -1057,18 +1057,18 @@
         </is>
       </c>
       <c r="D29" s="7" t="n">
-        <v>2.81</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="6">
       <c r="A30" s="4" t="inlineStr">
         <is>
-          <t>Life from the Loam</t>
+          <t>Hardened Scales</t>
         </is>
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>Duel Decks: Izzet vs Golgari</t>
+          <t>Khans of Tarkir</t>
         </is>
       </c>
       <c r="C30" s="4" t="inlineStr">
@@ -1077,27 +1077,27 @@
         </is>
       </c>
       <c r="D30" s="7" t="n">
-        <v>10.23</v>
+        <v>2.86</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" s="6">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>Majestic Genesis</t>
+          <t>Life from the Loam</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate Promos</t>
+          <t>Duel Decks: Izzet vs Golgari</t>
         </is>
       </c>
       <c r="C31" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D31" s="7" t="n">
-        <v>2.46</v>
+        <v>10.23</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="6">
@@ -1108,27 +1108,27 @@
       </c>
       <c r="B32" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Commander Legends: Battle For Baldur's Gate Promos</t>
         </is>
       </c>
       <c r="C32" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D32" s="7" t="n">
-        <v>1.73</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="6">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>Nylea, God of the Hunt</t>
+          <t>Majestic Genesis</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>Theros</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
@@ -1137,18 +1137,18 @@
         </is>
       </c>
       <c r="D33" s="7" t="n">
-        <v>4.87</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="6">
       <c r="A34" s="4" t="inlineStr">
         <is>
-          <t>Parallel Lives</t>
+          <t>Nylea, God of the Hunt</t>
         </is>
       </c>
       <c r="B34" s="4" t="inlineStr">
         <is>
-          <t>Innistrad</t>
+          <t>Theros</t>
         </is>
       </c>
       <c r="C34" s="4" t="inlineStr">
@@ -1157,18 +1157,18 @@
         </is>
       </c>
       <c r="D34" s="7" t="n">
-        <v>26.32</v>
+        <v>5.01</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="6">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>Haywire Mite</t>
+          <t>Parallel Lives</t>
         </is>
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Innistrad</t>
         </is>
       </c>
       <c r="C35" s="4" t="inlineStr">
@@ -1177,18 +1177,18 @@
         </is>
       </c>
       <c r="D35" s="7" t="n">
-        <v>1.3</v>
+        <v>27.15</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" s="6">
       <c r="A36" s="4" t="inlineStr">
         <is>
-          <t>Sphinx's Revelation</t>
+          <t>Silverback Elder</t>
         </is>
       </c>
       <c r="B36" s="4" t="inlineStr">
         <is>
-          <t>Return to Ravnica</t>
+          <t>Dominaria United: Extras</t>
         </is>
       </c>
       <c r="C36" s="4" t="inlineStr">
@@ -1197,18 +1197,18 @@
         </is>
       </c>
       <c r="D36" s="7" t="n">
-        <v>2.01</v>
+        <v>10.35</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="6">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>Ashiok, Nightmare Weaver</t>
+          <t>Haywire Mite</t>
         </is>
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>Theros</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C37" s="4" t="inlineStr">
@@ -1217,18 +1217,18 @@
         </is>
       </c>
       <c r="D37" s="7" t="n">
-        <v>3.52</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="6">
       <c r="A38" s="4" t="inlineStr">
         <is>
-          <t>Mind Grind</t>
+          <t>Sphinx's Revelation</t>
         </is>
       </c>
       <c r="B38" s="4" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Return to Ravnica</t>
         </is>
       </c>
       <c r="C38" s="4" t="inlineStr">
@@ -1237,18 +1237,18 @@
         </is>
       </c>
       <c r="D38" s="7" t="n">
-        <v>3.76</v>
+        <v>2.07</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="6">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>Satoru Umezawa</t>
+          <t>Ashiok, Nightmare Weaver</t>
         </is>
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>Buy a Box Promos</t>
+          <t>Theros</t>
         </is>
       </c>
       <c r="C39" s="4" t="inlineStr">
@@ -1257,18 +1257,18 @@
         </is>
       </c>
       <c r="D39" s="7" t="n">
-        <v>1.23</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="6">
       <c r="A40" s="4" t="inlineStr">
         <is>
-          <t>Legion's Initiative</t>
+          <t>Mind Grind</t>
         </is>
       </c>
       <c r="B40" s="4" t="inlineStr">
         <is>
-          <t>Dragon's Maze</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C40" s="4" t="inlineStr">
@@ -1277,18 +1277,18 @@
         </is>
       </c>
       <c r="D40" s="7" t="n">
-        <v>1.13</v>
+        <v>3.77</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="6">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>Expressive Iteration</t>
+          <t>Satoru Umezawa</t>
         </is>
       </c>
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>Strixhaven: School of Mages</t>
+          <t>Buy a Box Promos</t>
         </is>
       </c>
       <c r="C41" s="4" t="inlineStr">
@@ -1297,18 +1297,18 @@
         </is>
       </c>
       <c r="D41" s="7" t="n">
-        <v>2.98</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="6">
       <c r="A42" s="4" t="inlineStr">
         <is>
-          <t>Kolaghan's Command</t>
+          <t>Legion's Initiative</t>
         </is>
       </c>
       <c r="B42" s="4" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Dragon's Maze</t>
         </is>
       </c>
       <c r="C42" s="4" t="inlineStr">
@@ -1317,18 +1317,18 @@
         </is>
       </c>
       <c r="D42" s="7" t="n">
-        <v>3.15</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="6">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>Mogis, God of Slaughter</t>
+          <t>Expressive Iteration</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Strixhaven: School of Mages</t>
         </is>
       </c>
       <c r="C43" s="4" t="inlineStr">
@@ -1337,138 +1337,138 @@
         </is>
       </c>
       <c r="D43" s="7" t="n">
-        <v>6.74</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="6">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>Ajani, Sleeper Agent</t>
+          <t>Jhoira, Ageless Innovator</t>
         </is>
       </c>
       <c r="B44" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Dominaria United: Extras</t>
         </is>
       </c>
       <c r="C44" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>V.2</t>
         </is>
       </c>
       <c r="D44" s="7" t="n">
-        <v>3.15</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="6">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>Ivy, Gleeful Spellthief</t>
+          <t>Kolaghan's Command</t>
         </is>
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United Promos</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C45" s="4" t="inlineStr">
         <is>
-          <t>V.1</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D45" s="7" t="n">
-        <v>1.86</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" s="6">
       <c r="A46" s="4" t="inlineStr">
         <is>
-          <t>Vorel of the Hull Clade</t>
+          <t>Mogis, God of Slaughter</t>
         </is>
       </c>
       <c r="B46" s="4" t="inlineStr">
         <is>
-          <t>Dragon's Maze</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C46" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D46" s="7" t="n">
-        <v>1.5</v>
+        <v>6.93</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="6">
       <c r="A47" s="4" t="inlineStr">
         <is>
-          <t>Deathrite Shaman</t>
+          <t>Ajani, Sleeper Agent</t>
         </is>
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>Return to Ravnica</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C47" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D47" s="7" t="n">
-        <v>5.42</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="6">
       <c r="A48" s="4" t="inlineStr">
         <is>
-          <t>Jarad, Golgari Lich Lord</t>
+          <t>Ivy, Gleeful Spellthief</t>
         </is>
       </c>
       <c r="B48" s="4" t="inlineStr">
         <is>
-          <t>Duel Decks: Izzet vs Golgari</t>
+          <t>Dominaria United Promos</t>
         </is>
       </c>
       <c r="C48" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>V.1</t>
         </is>
       </c>
       <c r="D48" s="7" t="n">
-        <v>1.55</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="6">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>The Gitrog Monster</t>
+          <t>Vorel of the Hull Clade</t>
         </is>
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>Shadows over Innistrad</t>
+          <t>Dragon's Maze</t>
         </is>
       </c>
       <c r="C49" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D49" s="7" t="n">
-        <v>3.54</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" s="6">
       <c r="A50" s="4" t="inlineStr">
         <is>
-          <t>Arlinn Kord: Arlinn, Embraced by the Moon</t>
+          <t>Deathrite Shaman</t>
         </is>
       </c>
       <c r="B50" s="4" t="inlineStr">
         <is>
-          <t>Shadows over Innistrad</t>
+          <t>Return to Ravnica</t>
         </is>
       </c>
       <c r="C50" s="4" t="inlineStr">
@@ -1477,38 +1477,38 @@
         </is>
       </c>
       <c r="D50" s="7" t="n">
-        <v>3.82</v>
+        <v>5.31</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" s="6">
       <c r="A51" s="4" t="inlineStr">
         <is>
-          <t>Miirym, Sentinel Wyrm</t>
+          <t>Jarad, Golgari Lich Lord</t>
         </is>
       </c>
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Duel Decks: Izzet vs Golgari</t>
         </is>
       </c>
       <c r="C51" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D51" s="7" t="n">
-        <v>1.35</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" s="6">
       <c r="A52" s="4" t="inlineStr">
         <is>
-          <t>Aether Vial</t>
+          <t>The Gitrog Monster</t>
         </is>
       </c>
       <c r="B52" s="4" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Shadows over Innistrad</t>
         </is>
       </c>
       <c r="C52" s="4" t="inlineStr">
@@ -1517,18 +1517,18 @@
         </is>
       </c>
       <c r="D52" s="7" t="n">
-        <v>10.64</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" s="6">
       <c r="A53" s="4" t="inlineStr">
         <is>
-          <t>Akroma's Memorial</t>
+          <t>Arlinn Kord: Arlinn, Embraced by the Moon</t>
         </is>
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>Magic 2013</t>
+          <t>Shadows over Innistrad</t>
         </is>
       </c>
       <c r="C53" s="4" t="inlineStr">
@@ -1537,38 +1537,38 @@
         </is>
       </c>
       <c r="D53" s="7" t="n">
-        <v>7.06</v>
+        <v>4.12</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="6">
       <c r="A54" s="4" t="inlineStr">
         <is>
-          <t>Amulet of Vigor</t>
+          <t>Rith, Liberated Primeval</t>
         </is>
       </c>
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Dominaria United: Extras</t>
         </is>
       </c>
       <c r="C54" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>V.2</t>
         </is>
       </c>
       <c r="D54" s="7" t="n">
-        <v>18.22</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="6">
       <c r="A55" s="4" t="inlineStr">
         <is>
-          <t>Astral Cornucopia</t>
+          <t>Miirym, Sentinel Wyrm</t>
         </is>
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C55" s="4" t="inlineStr">
@@ -1577,18 +1577,18 @@
         </is>
       </c>
       <c r="D55" s="7" t="n">
-        <v>1.43</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="6">
       <c r="A56" s="4" t="inlineStr">
         <is>
-          <t>Coat of Arms</t>
+          <t>Aether Vial</t>
         </is>
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C56" s="4" t="inlineStr">
@@ -1597,18 +1597,18 @@
         </is>
       </c>
       <c r="D56" s="7" t="n">
-        <v>9.58</v>
+        <v>10.64</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" s="6">
       <c r="A57" s="4" t="inlineStr">
         <is>
-          <t>Dolmen Gate</t>
+          <t>Akroma's Memorial</t>
         </is>
       </c>
       <c r="B57" s="4" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Magic 2013</t>
         </is>
       </c>
       <c r="C57" s="4" t="inlineStr">
@@ -1617,38 +1617,38 @@
         </is>
       </c>
       <c r="D57" s="7" t="n">
-        <v>8.470000000000001</v>
+        <v>7.06</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" s="6">
       <c r="A58" s="4" t="inlineStr">
         <is>
-          <t>Elbrus, the Binding Blade: Withengar Unbound</t>
+          <t>Amulet of Vigor</t>
         </is>
       </c>
       <c r="B58" s="4" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C58" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D58" s="7" t="n">
-        <v>5.06</v>
+        <v>18.11</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" s="6">
       <c r="A59" s="4" t="inlineStr">
         <is>
-          <t>Grafdigger's Cage</t>
+          <t>Astral Cornucopia</t>
         </is>
       </c>
       <c r="B59" s="4" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C59" s="4" t="inlineStr">
@@ -1657,18 +1657,18 @@
         </is>
       </c>
       <c r="D59" s="7" t="n">
-        <v>2.38</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" s="6">
       <c r="A60" s="4" t="inlineStr">
         <is>
-          <t>Illusionist's Bracers</t>
+          <t>Coat of Arms</t>
         </is>
       </c>
       <c r="B60" s="4" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C60" s="4" t="inlineStr">
@@ -1677,65 +1677,141 @@
         </is>
       </c>
       <c r="D60" s="7" t="n">
-        <v>5.23</v>
+        <v>9.609999999999999</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" s="6">
       <c r="A61" s="4" t="inlineStr">
         <is>
-          <t>Karn, Living Legacy</t>
+          <t>Dolmen Gate</t>
         </is>
       </c>
       <c r="B61" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United Promos</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C61" s="4" t="inlineStr">
         <is>
-          <t>V.2</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D61" s="7" t="n">
-        <v>3.72</v>
+        <v>8.720000000000001</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" s="6">
       <c r="A62" s="4" t="inlineStr">
         <is>
+          <t>Elbrus, the Binding Blade: Withengar Unbound</t>
+        </is>
+      </c>
+      <c r="B62" s="4" t="inlineStr">
+        <is>
+          <t>Dark Ascension</t>
+        </is>
+      </c>
+      <c r="C62" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D62" s="7" t="n">
+        <v>4.89</v>
+      </c>
+    </row>
+    <row r="63" ht="15" customHeight="1" s="6">
+      <c r="A63" s="4" t="inlineStr">
+        <is>
+          <t>Grafdigger's Cage</t>
+        </is>
+      </c>
+      <c r="B63" s="4" t="inlineStr">
+        <is>
+          <t>Dark Ascension</t>
+        </is>
+      </c>
+      <c r="C63" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D63" s="7" t="n">
+        <v>2.32</v>
+      </c>
+    </row>
+    <row r="64" ht="15" customHeight="1" s="6">
+      <c r="A64" s="4" t="inlineStr">
+        <is>
+          <t>Illusionist's Bracers</t>
+        </is>
+      </c>
+      <c r="B64" s="4" t="inlineStr">
+        <is>
+          <t>Gatecrash</t>
+        </is>
+      </c>
+      <c r="C64" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D64" s="7" t="n">
+        <v>5.09</v>
+      </c>
+    </row>
+    <row r="65" ht="15" customHeight="1" s="6">
+      <c r="A65" s="4" t="inlineStr">
+        <is>
+          <t>Karn, Living Legacy</t>
+        </is>
+      </c>
+      <c r="B65" s="4" t="inlineStr">
+        <is>
+          <t>Dominaria United Promos</t>
+        </is>
+      </c>
+      <c r="C65" s="4" t="inlineStr">
+        <is>
+          <t>V.2</t>
+        </is>
+      </c>
+      <c r="D65" s="7" t="n">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="66" ht="15" customHeight="1" s="6">
+      <c r="A66" s="4" t="inlineStr">
+        <is>
           <t>Swiftfoot Boots</t>
         </is>
       </c>
-      <c r="B62" s="4" t="inlineStr">
+      <c r="B66" s="4" t="inlineStr">
         <is>
           <t>Commander 2017</t>
         </is>
       </c>
-      <c r="C62" s="4" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D62" s="7" t="n">
+      <c r="C66" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D66" s="7" t="n">
         <v>1.28</v>
       </c>
     </row>
-    <row r="64" ht="15" customHeight="1" s="6">
-      <c r="D64" s="5">
-        <f>SUM(D2:D62)</f>
+    <row r="68" ht="15" customHeight="1" s="6">
+      <c r="D68" s="5">
+        <f>SUM(D2:D66)</f>
         <v/>
       </c>
     </row>
-    <row r="1048567" ht="12.8" customHeight="1" s="6"/>
-    <row r="1048568" ht="12.8" customHeight="1" s="6"/>
-    <row r="1048569" ht="12.8" customHeight="1" s="6"/>
-    <row r="1048570" ht="12.8" customHeight="1" s="6"/>
-    <row r="1048571" ht="12.8" customHeight="1" s="6"/>
-    <row r="1048572" ht="12.8" customHeight="1" s="6"/>
-    <row r="1048573" ht="12.8" customHeight="1" s="6"/>
-    <row r="1048574" ht="12.8" customHeight="1" s="6"/>
-    <row r="1048575" ht="12.8" customHeight="1" s="6"/>
-    <row r="1048576" ht="12.8" customHeight="1" s="6"/>
+    <row r="1048571" ht="12.75" customHeight="1" s="6"/>
+    <row r="1048572" ht="12.75" customHeight="1" s="6"/>
+    <row r="1048573" ht="12.75" customHeight="1" s="6"/>
+    <row r="1048574" ht="12.75" customHeight="1" s="6"/>
+    <row r="1048575" ht="12.75" customHeight="1" s="6"/>
+    <row r="1048576" ht="12.75" customHeight="1" s="6"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Opened a Dominaria Remastered Collector Booster
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -463,10 +463,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D54" activeCellId="0" sqref="D54"/>
+      <selection pane="topLeft" activeCell="E69" activeCellId="0" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D2" s="7" t="n">
-        <v>9.630000000000001</v>
+        <v>9.699999999999999</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D3" s="7" t="n">
-        <v>8.470000000000001</v>
+        <v>8.720000000000001</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="6">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="D4" s="7" t="n">
-        <v>13.94</v>
+        <v>13.29</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="6">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>16.8</v>
+        <v>16.32</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="6">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>2.77</v>
+        <v>2.94</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D7" s="7" t="n">
-        <v>9.15</v>
+        <v>8.720000000000001</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="6">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="D8" s="7" t="n">
-        <v>7.51</v>
+        <v>7.95</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="6">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="D9" s="7" t="n">
-        <v>5.62</v>
+        <v>4.32</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="6">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="D10" s="7" t="n">
-        <v>25.32</v>
+        <v>26.63</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>1.52</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="6">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>5.19</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>1.37</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="6">
@@ -757,38 +757,38 @@
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>6.65</v>
+        <v>6.11</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="6">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Sage of Hours</t>
+          <t>Glory</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>Journey into Nyx</t>
+          <t>Dominaria Remastered: Extras</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>3.86</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="6">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>Ancient Brass Dragon</t>
+          <t>Sage of Hours</t>
         </is>
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Journey into Nyx</t>
         </is>
       </c>
       <c r="C16" s="4" t="inlineStr">
@@ -797,18 +797,18 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>15.19</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="6">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>Dark Petition</t>
+          <t>Ancient Brass Dragon</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>Magic Origins</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr">
@@ -817,18 +817,18 @@
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>3.57</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="6">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>Diabolic Intent</t>
+          <t>Dark Petition</t>
         </is>
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Magic Origins</t>
         </is>
       </c>
       <c r="C18" s="4" t="inlineStr">
@@ -837,18 +837,18 @@
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>7.46</v>
+        <v>3.89</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="6">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>Gravecrawler</t>
+          <t>Diabolic Intent</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
@@ -857,38 +857,38 @@
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>4.15</v>
+        <v>6.93</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="6">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>Scourge of the Skyclaves</t>
+          <t>Entomb</t>
         </is>
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>Zendikar Rising Promos</t>
+          <t>Dominaria Remastered: Extras</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>V.1</t>
+          <t>V.2</t>
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>0.82</v>
+        <v>19.83</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="6">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Tree of Perdition</t>
+          <t>Gravecrawler</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>Eldritch Moon</t>
+          <t>Dark Ascension</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
@@ -897,38 +897,38 @@
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>6.04</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="6">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Deadly Dispute</t>
+          <t>Scourge of the Skyclaves</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Zendikar Rising Promos</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>V.1</t>
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>2.62</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="6">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>Brotherhood's End</t>
+          <t>Tree of Perdition</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Eldritch Moon</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
@@ -937,18 +937,18 @@
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>7.73</v>
+        <v>5.21</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="6">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>Flame-Wreathed Phoenix</t>
+          <t>Deadly Dispute</t>
         </is>
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C24" s="4" t="inlineStr">
@@ -957,18 +957,18 @@
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>1.58</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="6">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>Shivan Devastator</t>
+          <t>Brotherhood's End</t>
         </is>
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
@@ -977,38 +977,38 @@
         </is>
       </c>
       <c r="D25" s="7" t="n">
-        <v>5.1</v>
+        <v>7.32</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" s="6">
       <c r="A26" s="4" t="inlineStr">
         <is>
-          <t>Vexing Devil</t>
+          <t>Flame-Wreathed Phoenix</t>
         </is>
       </c>
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>Avacyn Restored</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C26" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D26" s="7" t="n">
-        <v>3.72</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="6">
       <c r="A27" s="4" t="inlineStr">
         <is>
-          <t>Fauna Shaman</t>
+          <t>Shivan Devastator</t>
         </is>
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
@@ -1017,38 +1017,38 @@
         </is>
       </c>
       <c r="D27" s="7" t="n">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="28" ht="13.5" customHeight="1" s="6">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="28" ht="15" customHeight="1" s="6">
       <c r="A28" s="4" t="inlineStr">
         <is>
-          <t>Fyndhorn Elves</t>
+          <t>Vexing Devil</t>
         </is>
       </c>
       <c r="B28" s="4" t="inlineStr">
         <is>
-          <t>30th Anniversary Celebration</t>
+          <t>Avacyn Restored</t>
         </is>
       </c>
       <c r="C28" s="4" t="inlineStr">
         <is>
-          <t>German</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D28" s="7" t="n">
-        <v>2.2</v>
+        <v>4.16</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="6">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>Gyre Sage</t>
+          <t>Fauna Shaman</t>
         </is>
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
@@ -1057,38 +1057,38 @@
         </is>
       </c>
       <c r="D29" s="7" t="n">
-        <v>1.42</v>
-      </c>
-    </row>
-    <row r="30" ht="15" customHeight="1" s="6">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="30" ht="13.5" customHeight="1" s="6">
       <c r="A30" s="4" t="inlineStr">
         <is>
-          <t>Hardened Scales</t>
+          <t>Fyndhorn Elves</t>
         </is>
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>Khans of Tarkir</t>
+          <t>30th Anniversary Celebration</t>
         </is>
       </c>
       <c r="C30" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>German</t>
         </is>
       </c>
       <c r="D30" s="7" t="n">
-        <v>2.88</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" s="6">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>Life from the Loam</t>
+          <t>Gyre Sage</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>Duel Decks: Izzet vs Golgari</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C31" s="4" t="inlineStr">
@@ -1097,38 +1097,38 @@
         </is>
       </c>
       <c r="D31" s="7" t="n">
-        <v>10.49</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="6">
       <c r="A32" s="4" t="inlineStr">
         <is>
-          <t>Majestic Genesis</t>
+          <t>Hardened Scales</t>
         </is>
       </c>
       <c r="B32" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate Promos</t>
+          <t>Khans of Tarkir</t>
         </is>
       </c>
       <c r="C32" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D32" s="7" t="n">
-        <v>2.46</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="6">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>Majestic Genesis</t>
+          <t>Life from the Loam</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Duel Decks: Izzet vs Golgari</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
@@ -1137,38 +1137,38 @@
         </is>
       </c>
       <c r="D33" s="7" t="n">
-        <v>1.58</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="6">
       <c r="A34" s="4" t="inlineStr">
         <is>
-          <t>Nylea, God of the Hunt</t>
+          <t>Majestic Genesis</t>
         </is>
       </c>
       <c r="B34" s="4" t="inlineStr">
         <is>
-          <t>Theros</t>
+          <t>Commander Legends: Battle For Baldur's Gate Promos</t>
         </is>
       </c>
       <c r="C34" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D34" s="7" t="n">
-        <v>5.13</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="6">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>Parallel Lives</t>
+          <t>Majestic Genesis</t>
         </is>
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>Innistrad</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C35" s="4" t="inlineStr">
@@ -1177,18 +1177,18 @@
         </is>
       </c>
       <c r="D35" s="7" t="n">
-        <v>26.8</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" s="6">
       <c r="A36" s="4" t="inlineStr">
         <is>
-          <t>Silverback Elder</t>
+          <t>Nylea, God of the Hunt</t>
         </is>
       </c>
       <c r="B36" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United: Extras</t>
+          <t>Theros</t>
         </is>
       </c>
       <c r="C36" s="4" t="inlineStr">
@@ -1197,18 +1197,18 @@
         </is>
       </c>
       <c r="D36" s="7" t="n">
-        <v>10.79</v>
+        <v>4.93</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="6">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>Haywire Mite</t>
+          <t>Parallel Lives</t>
         </is>
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Innistrad</t>
         </is>
       </c>
       <c r="C37" s="4" t="inlineStr">
@@ -1217,18 +1217,18 @@
         </is>
       </c>
       <c r="D37" s="7" t="n">
-        <v>1.27</v>
+        <v>29.65</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="6">
       <c r="A38" s="4" t="inlineStr">
         <is>
-          <t>Sphinx's Revelation</t>
+          <t>Silverback Elder</t>
         </is>
       </c>
       <c r="B38" s="4" t="inlineStr">
         <is>
-          <t>Return to Ravnica</t>
+          <t>Dominaria United: Extras</t>
         </is>
       </c>
       <c r="C38" s="4" t="inlineStr">
@@ -1237,18 +1237,18 @@
         </is>
       </c>
       <c r="D38" s="7" t="n">
-        <v>1.95</v>
+        <v>9.73</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="6">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>Ashiok, Nightmare Weaver</t>
+          <t>Haywire Mite</t>
         </is>
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>Theros</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C39" s="4" t="inlineStr">
@@ -1257,18 +1257,18 @@
         </is>
       </c>
       <c r="D39" s="7" t="n">
-        <v>3.57</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="6">
       <c r="A40" s="4" t="inlineStr">
         <is>
-          <t>Mind Grind</t>
+          <t>Sphinx's Revelation</t>
         </is>
       </c>
       <c r="B40" s="4" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Return to Ravnica</t>
         </is>
       </c>
       <c r="C40" s="4" t="inlineStr">
@@ -1277,18 +1277,18 @@
         </is>
       </c>
       <c r="D40" s="7" t="n">
-        <v>3.77</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="6">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>Satoru Umezawa</t>
+          <t>Ashiok, Nightmare Weaver</t>
         </is>
       </c>
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>Buy a Box Promos</t>
+          <t>Theros</t>
         </is>
       </c>
       <c r="C41" s="4" t="inlineStr">
@@ -1297,18 +1297,18 @@
         </is>
       </c>
       <c r="D41" s="7" t="n">
-        <v>1.05</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="6">
       <c r="A42" s="4" t="inlineStr">
         <is>
-          <t>Legion's Initiative</t>
+          <t>Mind Grind</t>
         </is>
       </c>
       <c r="B42" s="4" t="inlineStr">
         <is>
-          <t>Dragon's Maze</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C42" s="4" t="inlineStr">
@@ -1317,18 +1317,18 @@
         </is>
       </c>
       <c r="D42" s="7" t="n">
-        <v>1.13</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="6">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>Expressive Iteration</t>
+          <t>Satoru Umezawa</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>Strixhaven: School of Mages</t>
+          <t>Buy a Box Promos</t>
         </is>
       </c>
       <c r="C43" s="4" t="inlineStr">
@@ -1337,38 +1337,38 @@
         </is>
       </c>
       <c r="D43" s="7" t="n">
-        <v>3</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="6">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>Jhoira, Ageless Innovator</t>
+          <t>Legion's Initiative</t>
         </is>
       </c>
       <c r="B44" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United: Extras</t>
+          <t>Dragon's Maze</t>
         </is>
       </c>
       <c r="C44" s="4" t="inlineStr">
         <is>
-          <t>V.2</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D44" s="7" t="n">
-        <v>1.59</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="6">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>Kolaghan's Command</t>
+          <t>Expressive Iteration</t>
         </is>
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Strixhaven: School of Mages</t>
         </is>
       </c>
       <c r="C45" s="4" t="inlineStr">
@@ -1377,78 +1377,78 @@
         </is>
       </c>
       <c r="D45" s="7" t="n">
-        <v>3.07</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" s="6">
       <c r="A46" s="4" t="inlineStr">
         <is>
-          <t>Mogis, God of Slaughter</t>
+          <t>Jhoira, Ageless Innovator</t>
         </is>
       </c>
       <c r="B46" s="4" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Dominaria United: Extras</t>
         </is>
       </c>
       <c r="C46" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>V.2</t>
         </is>
       </c>
       <c r="D46" s="7" t="n">
-        <v>7.25</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="6">
       <c r="A47" s="4" t="inlineStr">
         <is>
-          <t>Ajani, Sleeper Agent</t>
+          <t>Kolaghan's Command</t>
         </is>
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C47" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D47" s="7" t="n">
-        <v>3.22</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="6">
       <c r="A48" s="4" t="inlineStr">
         <is>
-          <t>Ivy, Gleeful Spellthief</t>
+          <t>Mogis, God of Slaughter</t>
         </is>
       </c>
       <c r="B48" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United Promos</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C48" s="4" t="inlineStr">
         <is>
-          <t>V.1</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D48" s="7" t="n">
-        <v>1.8</v>
+        <v>7.53</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="6">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>Vorel of the Hull Clade</t>
+          <t>Ajani, Sleeper Agent</t>
         </is>
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>Dragon's Maze</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C49" s="4" t="inlineStr">
@@ -1457,38 +1457,38 @@
         </is>
       </c>
       <c r="D49" s="7" t="n">
-        <v>1.48</v>
+        <v>3.37</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" s="6">
       <c r="A50" s="4" t="inlineStr">
         <is>
-          <t>Deathrite Shaman</t>
+          <t>Ivy, Gleeful Spellthief</t>
         </is>
       </c>
       <c r="B50" s="4" t="inlineStr">
         <is>
-          <t>Return to Ravnica</t>
+          <t>Dominaria United Promos</t>
         </is>
       </c>
       <c r="C50" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>V.1</t>
         </is>
       </c>
       <c r="D50" s="7" t="n">
-        <v>5.18</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" s="6">
       <c r="A51" s="4" t="inlineStr">
         <is>
-          <t>Jarad, Golgari Lich Lord</t>
+          <t>Vorel of the Hull Clade</t>
         </is>
       </c>
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>Duel Decks: Izzet vs Golgari</t>
+          <t>Dragon's Maze</t>
         </is>
       </c>
       <c r="C51" s="4" t="inlineStr">
@@ -1497,18 +1497,18 @@
         </is>
       </c>
       <c r="D51" s="7" t="n">
-        <v>1.5</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" s="6">
       <c r="A52" s="4" t="inlineStr">
         <is>
-          <t>The Gitrog Monster</t>
+          <t>Deathrite Shaman</t>
         </is>
       </c>
       <c r="B52" s="4" t="inlineStr">
         <is>
-          <t>Shadows over Innistrad</t>
+          <t>Return to Ravnica</t>
         </is>
       </c>
       <c r="C52" s="4" t="inlineStr">
@@ -1517,58 +1517,58 @@
         </is>
       </c>
       <c r="D52" s="7" t="n">
-        <v>3.84</v>
+        <v>5.22</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" s="6">
       <c r="A53" s="4" t="inlineStr">
         <is>
-          <t>Arlinn Kord: Arlinn, Embraced by the Moon</t>
+          <t>Jarad, Golgari Lich Lord</t>
         </is>
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>Shadows over Innistrad</t>
+          <t>Duel Decks: Izzet vs Golgari</t>
         </is>
       </c>
       <c r="C53" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D53" s="7" t="n">
-        <v>3.82</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="6">
       <c r="A54" s="4" t="inlineStr">
         <is>
-          <t>Rith, Liberated Primeval</t>
+          <t>The Gitrog Monster</t>
         </is>
       </c>
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United: Extras</t>
+          <t>Shadows over Innistrad</t>
         </is>
       </c>
       <c r="C54" s="4" t="inlineStr">
         <is>
-          <t>V.2</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D54" s="7" t="n">
-        <v>2.79</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="6">
       <c r="A55" s="4" t="inlineStr">
         <is>
-          <t>Miirym, Sentinel Wyrm</t>
+          <t>Arlinn Kord: Arlinn, Embraced by the Moon</t>
         </is>
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Shadows over Innistrad</t>
         </is>
       </c>
       <c r="C55" s="4" t="inlineStr">
@@ -1577,38 +1577,38 @@
         </is>
       </c>
       <c r="D55" s="7" t="n">
-        <v>1.42</v>
+        <v>4.32</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="6">
       <c r="A56" s="4" t="inlineStr">
         <is>
-          <t>Aether Vial</t>
+          <t>Rith, Liberated Primeval</t>
         </is>
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Dominaria United: Extras</t>
         </is>
       </c>
       <c r="C56" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>V.2</t>
         </is>
       </c>
       <c r="D56" s="7" t="n">
-        <v>11.07</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" s="6">
       <c r="A57" s="4" t="inlineStr">
         <is>
-          <t>Akroma's Memorial</t>
+          <t>Miirym, Sentinel Wyrm</t>
         </is>
       </c>
       <c r="B57" s="4" t="inlineStr">
         <is>
-          <t>Magic 2013</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C57" s="4" t="inlineStr">
@@ -1617,38 +1617,38 @@
         </is>
       </c>
       <c r="D57" s="7" t="n">
-        <v>6.74</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" s="6">
       <c r="A58" s="4" t="inlineStr">
         <is>
-          <t>Amulet of Vigor</t>
+          <t>Aether Vial</t>
         </is>
       </c>
       <c r="B58" s="4" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C58" s="4" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D58" s="7" t="n">
-        <v>17.87</v>
+        <v>11.89</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" s="6">
       <c r="A59" s="4" t="inlineStr">
         <is>
-          <t>Astral Cornucopia</t>
+          <t>Akroma's Memorial</t>
         </is>
       </c>
       <c r="B59" s="4" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Magic 2013</t>
         </is>
       </c>
       <c r="C59" s="4" t="inlineStr">
@@ -1657,13 +1657,13 @@
         </is>
       </c>
       <c r="D59" s="7" t="n">
-        <v>1.34</v>
+        <v>7.22</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" s="6">
       <c r="A60" s="4" t="inlineStr">
         <is>
-          <t>Coat of Arms</t>
+          <t>Amulet of Vigor</t>
         </is>
       </c>
       <c r="B60" s="4" t="inlineStr">
@@ -1673,22 +1673,22 @@
       </c>
       <c r="C60" s="4" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D60" s="7" t="n">
-        <v>9.970000000000001</v>
+        <v>17.82</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" s="6">
       <c r="A61" s="4" t="inlineStr">
         <is>
-          <t>Dolmen Gate</t>
+          <t>Astral Cornucopia</t>
         </is>
       </c>
       <c r="B61" s="4" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C61" s="4" t="inlineStr">
@@ -1697,18 +1697,18 @@
         </is>
       </c>
       <c r="D61" s="7" t="n">
-        <v>8.82</v>
+        <v>1.15</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" s="6">
       <c r="A62" s="4" t="inlineStr">
         <is>
-          <t>Elbrus, the Binding Blade: Withengar Unbound</t>
+          <t>Coat of Arms</t>
         </is>
       </c>
       <c r="B62" s="4" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C62" s="4" t="inlineStr">
@@ -1717,18 +1717,18 @@
         </is>
       </c>
       <c r="D62" s="7" t="n">
-        <v>4.28</v>
+        <v>10.17</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" s="6">
       <c r="A63" s="4" t="inlineStr">
         <is>
-          <t>Grafdigger's Cage</t>
+          <t>Dolmen Gate</t>
         </is>
       </c>
       <c r="B63" s="4" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C63" s="4" t="inlineStr">
@@ -1737,18 +1737,18 @@
         </is>
       </c>
       <c r="D63" s="7" t="n">
-        <v>2.17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" s="6">
       <c r="A64" s="4" t="inlineStr">
         <is>
-          <t>Illusionist's Bracers</t>
+          <t>Elbrus, the Binding Blade: Withengar Unbound</t>
         </is>
       </c>
       <c r="B64" s="4" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Dark Ascension</t>
         </is>
       </c>
       <c r="C64" s="4" t="inlineStr">
@@ -1757,58 +1757,115 @@
         </is>
       </c>
       <c r="D64" s="7" t="n">
-        <v>5.42</v>
+        <v>3.64</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" s="6">
       <c r="A65" s="4" t="inlineStr">
         <is>
-          <t>Karn, Living Legacy</t>
+          <t>Grafdigger's Cage</t>
         </is>
       </c>
       <c r="B65" s="4" t="inlineStr">
         <is>
-          <t>Dominaria United Promos</t>
+          <t>Dark Ascension</t>
         </is>
       </c>
       <c r="C65" s="4" t="inlineStr">
         <is>
-          <t>V.2</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D65" s="7" t="n">
-        <v>3.72</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" s="6">
       <c r="A66" s="4" t="inlineStr">
         <is>
+          <t>Helm of Awakening</t>
+        </is>
+      </c>
+      <c r="B66" s="4" t="inlineStr">
+        <is>
+          <t>Dominaria Remastered</t>
+        </is>
+      </c>
+      <c r="C66" s="4" t="inlineStr">
+        <is>
+          <t>Foil</t>
+        </is>
+      </c>
+      <c r="D66" s="7" t="n">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="67" ht="15" customHeight="1" s="6">
+      <c r="A67" s="4" t="inlineStr">
+        <is>
+          <t>Illusionist's Bracers</t>
+        </is>
+      </c>
+      <c r="B67" s="4" t="inlineStr">
+        <is>
+          <t>Gatecrash</t>
+        </is>
+      </c>
+      <c r="C67" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D67" s="7" t="n">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="68" ht="15" customHeight="1" s="6">
+      <c r="A68" s="4" t="inlineStr">
+        <is>
+          <t>Karn, Living Legacy</t>
+        </is>
+      </c>
+      <c r="B68" s="4" t="inlineStr">
+        <is>
+          <t>Dominaria United Promos</t>
+        </is>
+      </c>
+      <c r="C68" s="4" t="inlineStr">
+        <is>
+          <t>V.2</t>
+        </is>
+      </c>
+      <c r="D68" s="7" t="n">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="69" ht="15" customHeight="1" s="6">
+      <c r="A69" s="4" t="inlineStr">
+        <is>
           <t>Swiftfoot Boots</t>
         </is>
       </c>
-      <c r="B66" s="4" t="inlineStr">
+      <c r="B69" s="4" t="inlineStr">
         <is>
           <t>Commander 2017</t>
         </is>
       </c>
-      <c r="C66" s="4" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D66" s="7" t="n">
-        <v>1.28</v>
-      </c>
-    </row>
-    <row r="68" ht="15" customHeight="1" s="6">
-      <c r="D68" s="5">
-        <f>SUM(D2:D66)</f>
+      <c r="C69" s="4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D69" s="7" t="n">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="71" ht="15" customHeight="1" s="6">
+      <c r="D71" s="5">
+        <f>SUM(D2:D69)</f>
         <v/>
       </c>
     </row>
-    <row r="1048571" ht="12.75" customHeight="1" s="6"/>
-    <row r="1048572" ht="12.75" customHeight="1" s="6"/>
-    <row r="1048573" ht="12.75" customHeight="1" s="6"/>
     <row r="1048574" ht="12.75" customHeight="1" s="6"/>
     <row r="1048575" ht="12.75" customHeight="1" s="6"/>
     <row r="1048576" ht="12.75" customHeight="1" s="6"/>

</xml_diff>

<commit_message>
Removed cards from the Duel Decks
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="106">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -208,12 +208,6 @@
     <t xml:space="preserve">Khans of Tarkir</t>
   </si>
   <si>
-    <t xml:space="preserve">Life from the Loam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duel Decks: Izzet vs Golgari</t>
-  </si>
-  <si>
     <t xml:space="preserve">Majestic Genesis</t>
   </si>
   <si>
@@ -284,9 +278,6 @@
   </si>
   <si>
     <t xml:space="preserve">Deathrite Shaman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jarad, Golgari Lich Lord</t>
   </si>
   <si>
     <t xml:space="preserve">The Gitrog Monster</t>
@@ -460,8 +451,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -915,24 +906,24 @@
         <v>63</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D32" s="3" t="n">
-        <v>10.65</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D33" s="3" t="n">
-        <v>2.9</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -940,27 +931,27 @@
         <v>64</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="3" t="n">
-        <v>1.7</v>
+        <v>4.54</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="3" t="n">
-        <v>4.54</v>
+        <v>27.85</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -968,83 +959,83 @@
         <v>67</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="3" t="n">
-        <v>27.85</v>
+        <v>9.79</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="3" t="n">
-        <v>9.79</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="3" t="n">
-        <v>1.42</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="3" t="n">
-        <v>1.97</v>
+        <v>3.55</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="3" t="n">
-        <v>3.55</v>
+        <v>3.76</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="3" t="n">
-        <v>3.76</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1052,27 +1043,27 @@
         <v>74</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="3" t="n">
-        <v>1.02</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="C43" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="3" t="n">
-        <v>1.37</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1080,27 +1071,27 @@
         <v>77</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D44" s="3" t="n">
-        <v>3.39</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D45" s="3" t="n">
-        <v>1.46</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1108,41 +1099,41 @@
         <v>80</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="3" t="n">
-        <v>3.07</v>
+        <v>7.22</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D47" s="3" t="n">
-        <v>7.22</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="C48" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D48" s="3" t="n">
-        <v>3.53</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1150,41 +1141,41 @@
         <v>84</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D49" s="3" t="n">
-        <v>1.49</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D50" s="3" t="n">
-        <v>1.51</v>
+        <v>5.42</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C51" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="3" t="n">
-        <v>5.42</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1192,13 +1183,13 @@
         <v>88</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D52" s="3" t="n">
-        <v>1.61</v>
+        <v>4.03</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1206,69 +1197,69 @@
         <v>89</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D53" s="3" t="n">
-        <v>3.57</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="3" t="n">
-        <v>4.03</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D55" s="3" t="n">
-        <v>2.79</v>
+        <v>11.16</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="3" t="n">
-        <v>1.56</v>
+        <v>7.07</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="C57" s="1" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D57" s="3" t="n">
-        <v>11.16</v>
+        <v>17.86</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1276,13 +1267,13 @@
         <v>95</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D58" s="3" t="n">
-        <v>7.07</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1290,69 +1281,69 @@
         <v>96</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D59" s="3" t="n">
-        <v>17.86</v>
+        <v>10.35</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="3" t="n">
-        <v>1.16</v>
+        <v>8.98</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="3" t="n">
-        <v>10.35</v>
+        <v>3.29</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D62" s="3" t="n">
-        <v>8.98</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C63" s="1" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D63" s="3" t="n">
-        <v>3.29</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1360,13 +1351,13 @@
         <v>102</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D64" s="3" t="n">
-        <v>1.83</v>
+        <v>6.05</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1374,66 +1365,40 @@
         <v>103</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D65" s="3" t="n">
-        <v>0.87</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C66" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D66" s="3" t="n">
-        <v>6.05</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D67" s="3" t="n">
-        <v>3.73</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="3" t="n">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D70" s="2" t="n">
-        <f aca="false">SUM(D2:D68)</f>
-        <v>369.61</v>
-      </c>
-    </row>
+      <c r="D68" s="2" t="n">
+        <f aca="false">SUM(D2:D66)</f>
+        <v>357.35</v>
+      </c>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
It matters where you are
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>8.09</v>
+        <v>9.449999999999999</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>13.42</v>
+        <v>13.81</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>17.36</v>
+        <v>17.16</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>9.65</v>
+        <v>9.51</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>8.65</v>
+        <v>8.81</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.45</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.82</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>1.43</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>1.06</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>3.23</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>2.6</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0.35</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0.63</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1">
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0.58</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1">
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>2.66</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="D21" s="2" t="n">
-        <v>3.33</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1">
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0.73</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1">
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="D23" s="2" t="n">
-        <v>4.39</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>31.74</v>
+        <v>32.63</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1">
@@ -930,7 +930,7 @@
         </is>
       </c>
       <c r="D25" s="2" t="n">
-        <v>6.37</v>
+        <v>6.19</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1">
@@ -950,7 +950,7 @@
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>18.94</v>
+        <v>19.18</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="D27" s="2" t="n">
-        <v>2.31</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1">
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>0.97</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1">
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="D29" s="2" t="n">
-        <v>3.62</v>
+        <v>4.66</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1">
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>3.92</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="D31" s="2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.8100000000000001</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>0.74</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1">
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="D33" s="2" t="n">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1">
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>0.85</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1">
@@ -1130,7 +1130,7 @@
         </is>
       </c>
       <c r="D35" s="2" t="n">
-        <v>15.65</v>
+        <v>15.48</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>5.01</v>
+        <v>4.83</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="D37" s="2" t="n">
-        <v>6.64</v>
+        <v>6.74</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1">
@@ -1190,7 +1190,7 @@
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>7.61</v>
+        <v>7.82</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1">
@@ -1210,7 +1210,7 @@
         </is>
       </c>
       <c r="D39" s="2" t="n">
-        <v>3.84</v>
+        <v>3.94</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1">
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1">
@@ -1250,7 +1250,7 @@
         </is>
       </c>
       <c r="D41" s="2" t="n">
-        <v>0.93</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1">
@@ -1270,7 +1270,7 @@
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>57.09</v>
+        <v>56.45</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1">
@@ -1290,7 +1290,7 @@
         </is>
       </c>
       <c r="D43" s="2" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1">
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="D44" s="2" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1">
@@ -1330,7 +1330,7 @@
         </is>
       </c>
       <c r="D45" s="2" t="n">
-        <v>4.78</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1">
@@ -1370,7 +1370,7 @@
         </is>
       </c>
       <c r="D47" s="2" t="n">
-        <v>2.89</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1">
@@ -1390,7 +1390,7 @@
         </is>
       </c>
       <c r="D48" s="2" t="n">
-        <v>7.3</v>
+        <v>7.49</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1">
@@ -1410,7 +1410,7 @@
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>1.89</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1">
@@ -1450,7 +1450,7 @@
         </is>
       </c>
       <c r="D51" s="2" t="n">
-        <v>4.87</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1">
@@ -1470,7 +1470,7 @@
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>0.96</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1">
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="D53" s="2" t="n">
-        <v>3.35</v>
+        <v>2.84</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1">
@@ -1510,7 +1510,7 @@
         </is>
       </c>
       <c r="D54" s="2" t="n">
-        <v>3.17</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1">
@@ -1530,7 +1530,7 @@
         </is>
       </c>
       <c r="D55" s="2" t="n">
-        <v>1.32</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1">
@@ -1550,7 +1550,7 @@
         </is>
       </c>
       <c r="D56" s="2" t="n">
-        <v>1.2</v>
+        <v>1.63</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1">
@@ -1570,7 +1570,7 @@
         </is>
       </c>
       <c r="D57" s="2" t="n">
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1">
@@ -1590,7 +1590,7 @@
         </is>
       </c>
       <c r="D58" s="2" t="n">
-        <v>1.35</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="59" ht="13.5" customHeight="1">
@@ -1610,7 +1610,7 @@
         </is>
       </c>
       <c r="D59" s="2" t="n">
-        <v>1.91</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1">
@@ -1630,7 +1630,7 @@
         </is>
       </c>
       <c r="D60" s="2" t="n">
-        <v>1.57</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1">
@@ -1670,7 +1670,7 @@
         </is>
       </c>
       <c r="D62" s="2" t="n">
-        <v>3.65</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="D63" s="2" t="n">
-        <v>1.71</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1">
@@ -1710,7 +1710,7 @@
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>4.94</v>
+        <v>4.72</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1">
@@ -1730,7 +1730,7 @@
         </is>
       </c>
       <c r="D65" s="2" t="n">
-        <v>26.63</v>
+        <v>27.68</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1">
@@ -1750,7 +1750,7 @@
         </is>
       </c>
       <c r="D66" s="2" t="n">
-        <v>9.74</v>
+        <v>9.630000000000001</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1">
@@ -1770,7 +1770,7 @@
         </is>
       </c>
       <c r="D67" s="2" t="n">
-        <v>1.52</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1">
@@ -1810,7 +1810,7 @@
         </is>
       </c>
       <c r="D69" s="2" t="n">
-        <v>3.4</v>
+        <v>3.43</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1">
@@ -1830,7 +1830,7 @@
         </is>
       </c>
       <c r="D70" s="2" t="n">
-        <v>4</v>
+        <v>4.11</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1">
@@ -1850,7 +1850,7 @@
         </is>
       </c>
       <c r="D71" s="2" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1">
@@ -1870,7 +1870,7 @@
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>1.08</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1">
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="D73" s="2" t="n">
-        <v>2.5</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1">
@@ -1910,7 +1910,7 @@
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>3</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1">
@@ -1930,7 +1930,7 @@
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>5.55</v>
+        <v>6.52</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1">
@@ -1950,7 +1950,7 @@
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>4.76</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1">
@@ -1970,7 +1970,7 @@
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="78" ht="15" customHeight="1">
@@ -1990,7 +1990,7 @@
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>1.04</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1">
@@ -2010,7 +2010,7 @@
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>5.81</v>
+        <v>5.92</v>
       </c>
     </row>
     <row r="80" ht="15" customHeight="1">
@@ -2030,7 +2030,7 @@
         </is>
       </c>
       <c r="D80" s="2" t="n">
-        <v>3.6</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="81" ht="15" customHeight="1">
@@ -2050,7 +2050,7 @@
         </is>
       </c>
       <c r="D81" s="2" t="n">
-        <v>4.51</v>
+        <v>4.43</v>
       </c>
     </row>
     <row r="82" ht="15" customHeight="1">
@@ -2070,7 +2070,7 @@
         </is>
       </c>
       <c r="D82" s="2" t="n">
-        <v>1.53</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="83" ht="15" customHeight="1">
@@ -2090,7 +2090,7 @@
         </is>
       </c>
       <c r="D83" s="2" t="n">
-        <v>1.44</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="84" ht="15" customHeight="1">
@@ -2110,7 +2110,7 @@
         </is>
       </c>
       <c r="D84" s="2" t="n">
-        <v>9.960000000000001</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="85" ht="15" customHeight="1">
@@ -2130,7 +2130,7 @@
         </is>
       </c>
       <c r="D85" s="2" t="n">
-        <v>7.56</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="86" ht="15" customHeight="1">
@@ -2150,7 +2150,7 @@
         </is>
       </c>
       <c r="D86" s="2" t="n">
-        <v>17.39</v>
+        <v>16.94</v>
       </c>
     </row>
     <row r="87" ht="15" customHeight="1">
@@ -2170,7 +2170,7 @@
         </is>
       </c>
       <c r="D87" s="2" t="n">
-        <v>1.39</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="88" ht="15" customHeight="1">
@@ -2190,7 +2190,7 @@
         </is>
       </c>
       <c r="D88" s="2" t="n">
-        <v>9.970000000000001</v>
+        <v>10.84</v>
       </c>
     </row>
     <row r="89" ht="15" customHeight="1">
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="D89" s="2" t="n">
-        <v>8.84</v>
+        <v>9.130000000000001</v>
       </c>
     </row>
     <row r="90" ht="15" customHeight="1">
@@ -2230,7 +2230,7 @@
         </is>
       </c>
       <c r="D90" s="2" t="n">
-        <v>3.27</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="91" ht="15" customHeight="1">
@@ -2250,7 +2250,7 @@
         </is>
       </c>
       <c r="D91" s="2" t="n">
-        <v>2.03</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="92" ht="15" customHeight="1">
@@ -2270,7 +2270,7 @@
         </is>
       </c>
       <c r="D92" s="2" t="n">
-        <v>0.63</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="93" ht="15" customHeight="1">
@@ -2290,7 +2290,7 @@
         </is>
       </c>
       <c r="D93" s="2" t="n">
-        <v>6.15</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="94" ht="15" customHeight="1">
@@ -2330,7 +2330,7 @@
         </is>
       </c>
       <c r="D95" s="2" t="n">
-        <v>0.99</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="96" ht="15" customHeight="1">
@@ -2350,7 +2350,7 @@
         </is>
       </c>
       <c r="D96" s="2" t="n">
-        <v>0.85</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="97" ht="15" customHeight="1">
@@ -2370,7 +2370,7 @@
         </is>
       </c>
       <c r="D97" s="2" t="n">
-        <v>1.75</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="98" ht="15" customHeight="1">
@@ -2390,7 +2390,7 @@
         </is>
       </c>
       <c r="D98" s="2" t="n">
-        <v>0.76</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="99" ht="15" customHeight="1">
@@ -2410,7 +2410,7 @@
         </is>
       </c>
       <c r="D99" s="2" t="n">
-        <v>0.8</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="100" ht="15" customHeight="1">

</xml_diff>

<commit_message>
I am falling, I am fading
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>9.449999999999999</v>
+        <v>9.630000000000001</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>13.81</v>
+        <v>13.86</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>17.16</v>
+        <v>17.06</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>9.51</v>
+        <v>9.58</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>8.81</v>
+        <v>8.73</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.87</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>1.45</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>3.27</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0.57</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0.59</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1">
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="D19" s="2" t="n">
-        <v>7.93</v>
+        <v>7.97</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1">
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>2.6</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="D21" s="2" t="n">
-        <v>2.93</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1">
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0.75</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>32.63</v>
+        <v>32.43</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1">
@@ -930,7 +930,7 @@
         </is>
       </c>
       <c r="D25" s="2" t="n">
-        <v>6.19</v>
+        <v>6.43</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1">
@@ -950,7 +950,7 @@
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>19.18</v>
+        <v>19.22</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1">
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1">
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="D29" s="2" t="n">
-        <v>4.66</v>
+        <v>4.73</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1">
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>3.88</v>
+        <v>3.93</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1">
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>0.88</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1">
@@ -1130,7 +1130,7 @@
         </is>
       </c>
       <c r="D35" s="2" t="n">
-        <v>15.48</v>
+        <v>15.28</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>4.83</v>
+        <v>4.69</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="D37" s="2" t="n">
-        <v>6.74</v>
+        <v>6.79</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1">
@@ -1190,7 +1190,7 @@
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>7.82</v>
+        <v>7.89</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1">
@@ -1210,7 +1210,7 @@
         </is>
       </c>
       <c r="D39" s="2" t="n">
-        <v>3.94</v>
+        <v>3.86</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1">
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>0.71</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1">
@@ -1270,7 +1270,7 @@
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>56.45</v>
+        <v>56.96</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1">
@@ -1290,7 +1290,7 @@
         </is>
       </c>
       <c r="D43" s="2" t="n">
-        <v>0.79</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1">
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="D44" s="2" t="n">
-        <v>0.79</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1">
@@ -1330,7 +1330,7 @@
         </is>
       </c>
       <c r="D45" s="2" t="n">
-        <v>4.6</v>
+        <v>4.82</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1">
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="D46" s="2" t="n">
-        <v>0.78</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1">
@@ -1370,7 +1370,7 @@
         </is>
       </c>
       <c r="D47" s="2" t="n">
-        <v>3</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1">
@@ -1390,7 +1390,7 @@
         </is>
       </c>
       <c r="D48" s="2" t="n">
-        <v>7.49</v>
+        <v>7.52</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1">
@@ -1410,7 +1410,7 @@
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>1.74</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1">
@@ -1450,7 +1450,7 @@
         </is>
       </c>
       <c r="D51" s="2" t="n">
-        <v>4.8</v>
+        <v>4.93</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1">
@@ -1470,7 +1470,7 @@
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>1.13</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1">
@@ -1530,7 +1530,7 @@
         </is>
       </c>
       <c r="D55" s="2" t="n">
-        <v>1.19</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1">
@@ -1570,7 +1570,7 @@
         </is>
       </c>
       <c r="D57" s="2" t="n">
-        <v>1.5</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1">
@@ -1590,7 +1590,7 @@
         </is>
       </c>
       <c r="D58" s="2" t="n">
-        <v>1.5</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="59" ht="13.5" customHeight="1">
@@ -1610,7 +1610,7 @@
         </is>
       </c>
       <c r="D59" s="2" t="n">
-        <v>2.08</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1">
@@ -1630,7 +1630,7 @@
         </is>
       </c>
       <c r="D60" s="2" t="n">
-        <v>1.51</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1">
@@ -1650,7 +1650,7 @@
         </is>
       </c>
       <c r="D61" s="2" t="n">
-        <v>2.76</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="D63" s="2" t="n">
-        <v>1.7</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1">
@@ -1710,7 +1710,7 @@
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>4.72</v>
+        <v>4.76</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1">
@@ -1730,7 +1730,7 @@
         </is>
       </c>
       <c r="D65" s="2" t="n">
-        <v>27.68</v>
+        <v>26.92</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1">
@@ -1810,7 +1810,7 @@
         </is>
       </c>
       <c r="D69" s="2" t="n">
-        <v>3.43</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1">
@@ -1830,7 +1830,7 @@
         </is>
       </c>
       <c r="D70" s="2" t="n">
-        <v>4.11</v>
+        <v>4.09</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1">
@@ -1850,7 +1850,7 @@
         </is>
       </c>
       <c r="D71" s="2" t="n">
-        <v>0.58</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1">
@@ -1870,7 +1870,7 @@
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>1.04</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1">
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="D73" s="2" t="n">
-        <v>2.68</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1">
@@ -1910,7 +1910,7 @@
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>3.06</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1">
@@ -1930,7 +1930,7 @@
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>6.52</v>
+        <v>6.95</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1">
@@ -2010,7 +2010,7 @@
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>5.92</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" ht="15" customHeight="1">
@@ -2030,7 +2030,7 @@
         </is>
       </c>
       <c r="D80" s="2" t="n">
-        <v>3.79</v>
+        <v>3.86</v>
       </c>
     </row>
     <row r="81" ht="15" customHeight="1">
@@ -2050,7 +2050,7 @@
         </is>
       </c>
       <c r="D81" s="2" t="n">
-        <v>4.43</v>
+        <v>4.35</v>
       </c>
     </row>
     <row r="82" ht="15" customHeight="1">
@@ -2090,7 +2090,7 @@
         </is>
       </c>
       <c r="D83" s="2" t="n">
-        <v>1.4</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="84" ht="15" customHeight="1">
@@ -2110,7 +2110,7 @@
         </is>
       </c>
       <c r="D84" s="2" t="n">
-        <v>11.7</v>
+        <v>11.83</v>
       </c>
     </row>
     <row r="85" ht="15" customHeight="1">
@@ -2130,7 +2130,7 @@
         </is>
       </c>
       <c r="D85" s="2" t="n">
-        <v>5.9</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="86" ht="15" customHeight="1">
@@ -2150,7 +2150,7 @@
         </is>
       </c>
       <c r="D86" s="2" t="n">
-        <v>16.94</v>
+        <v>17.02</v>
       </c>
     </row>
     <row r="87" ht="15" customHeight="1">
@@ -2170,7 +2170,7 @@
         </is>
       </c>
       <c r="D87" s="2" t="n">
-        <v>1.25</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="88" ht="15" customHeight="1">
@@ -2190,7 +2190,7 @@
         </is>
       </c>
       <c r="D88" s="2" t="n">
-        <v>10.84</v>
+        <v>10.93</v>
       </c>
     </row>
     <row r="89" ht="15" customHeight="1">
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="D89" s="2" t="n">
-        <v>9.130000000000001</v>
+        <v>9.470000000000001</v>
       </c>
     </row>
     <row r="90" ht="15" customHeight="1">
@@ -2230,7 +2230,7 @@
         </is>
       </c>
       <c r="D90" s="2" t="n">
-        <v>3.53</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="91" ht="15" customHeight="1">
@@ -2250,7 +2250,7 @@
         </is>
       </c>
       <c r="D91" s="2" t="n">
-        <v>1.89</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="92" ht="15" customHeight="1">
@@ -2290,7 +2290,7 @@
         </is>
       </c>
       <c r="D93" s="2" t="n">
-        <v>5.88</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="94" ht="15" customHeight="1">
@@ -2370,7 +2370,7 @@
         </is>
       </c>
       <c r="D97" s="2" t="n">
-        <v>1.89</v>
+        <v>1.93</v>
       </c>
     </row>
     <row r="98" ht="15" customHeight="1">
@@ -2430,7 +2430,7 @@
         </is>
       </c>
       <c r="D100" s="2" t="n">
-        <v>0.95</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="102" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Solid as a rock
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>10.19</v>
+        <v>10.03</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>13.63</v>
+        <v>13.81</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>17.12</v>
+        <v>17.11</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>10.05</v>
+        <v>9.81</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>8.83</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.52</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.89</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>1.46</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>1.25</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>3.28</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>2.66</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1">
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0.62</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1">
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="D19" s="2" t="n">
-        <v>7.85</v>
+        <v>7.82</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1">
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>2.55</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1">
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="D23" s="2" t="n">
-        <v>3.95</v>
+        <v>3.51</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>31.68</v>
+        <v>30.94</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1">
@@ -930,7 +930,7 @@
         </is>
       </c>
       <c r="D25" s="2" t="n">
-        <v>6.76</v>
+        <v>6.57</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1">
@@ -950,7 +950,7 @@
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>19.31</v>
+        <v>19.61</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="D27" s="2" t="n">
-        <v>2.31</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1">
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>0.85</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1">
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="D29" s="2" t="n">
-        <v>4.62</v>
+        <v>4.54</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1">
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>3.89</v>
+        <v>3.98</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1">
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="D33" s="2" t="n">
-        <v>0.77</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1">
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>0.98</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1">
@@ -1130,7 +1130,7 @@
         </is>
       </c>
       <c r="D35" s="2" t="n">
-        <v>15.49</v>
+        <v>15.16</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>4.58</v>
+        <v>4.83</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="D37" s="2" t="n">
-        <v>6.69</v>
+        <v>6.64</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1">
@@ -1190,7 +1190,7 @@
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>7.93</v>
+        <v>8.119999999999999</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1">
@@ -1210,7 +1210,7 @@
         </is>
       </c>
       <c r="D39" s="2" t="n">
-        <v>3.83</v>
+        <v>4.39</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1">
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>0.7</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1">
@@ -1250,7 +1250,7 @@
         </is>
       </c>
       <c r="D41" s="2" t="n">
-        <v>1.12</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1">
@@ -1270,7 +1270,7 @@
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>57.04</v>
+        <v>55.18</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1">
@@ -1290,7 +1290,7 @@
         </is>
       </c>
       <c r="D43" s="2" t="n">
-        <v>0.87</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1">
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="D44" s="2" t="n">
-        <v>0.87</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1">
@@ -1330,7 +1330,7 @@
         </is>
       </c>
       <c r="D45" s="2" t="n">
-        <v>4.99</v>
+        <v>4.76</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1">
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="D46" s="2" t="n">
-        <v>0.95</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1">
@@ -1370,7 +1370,7 @@
         </is>
       </c>
       <c r="D47" s="2" t="n">
-        <v>3.55</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1">
@@ -1390,7 +1390,7 @@
         </is>
       </c>
       <c r="D48" s="2" t="n">
-        <v>7.25</v>
+        <v>6.35</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1">
@@ -1410,7 +1410,7 @@
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>1.5</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1">
@@ -1450,7 +1450,7 @@
         </is>
       </c>
       <c r="D51" s="2" t="n">
-        <v>4.98</v>
+        <v>4.84</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1">
@@ -1470,7 +1470,7 @@
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>1.02</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1">
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="D53" s="2" t="n">
-        <v>3.5</v>
+        <v>4.36</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1">
@@ -1510,7 +1510,7 @@
         </is>
       </c>
       <c r="D54" s="2" t="n">
-        <v>3.43</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1">
@@ -1530,7 +1530,7 @@
         </is>
       </c>
       <c r="D55" s="2" t="n">
-        <v>1.23</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1">
@@ -1550,7 +1550,7 @@
         </is>
       </c>
       <c r="D56" s="2" t="n">
-        <v>1.45</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1">
@@ -1570,7 +1570,7 @@
         </is>
       </c>
       <c r="D57" s="2" t="n">
-        <v>1.45</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1">
@@ -1590,7 +1590,7 @@
         </is>
       </c>
       <c r="D58" s="2" t="n">
-        <v>1.45</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="59" ht="13.5" customHeight="1">
@@ -1610,7 +1610,7 @@
         </is>
       </c>
       <c r="D59" s="2" t="n">
-        <v>1.74</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1">
@@ -1630,7 +1630,7 @@
         </is>
       </c>
       <c r="D60" s="2" t="n">
-        <v>1.58</v>
+        <v>1.63</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1">
@@ -1650,7 +1650,7 @@
         </is>
       </c>
       <c r="D61" s="2" t="n">
-        <v>2.72</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="D63" s="2" t="n">
-        <v>1.63</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1">
@@ -1710,7 +1710,7 @@
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>5.12</v>
+        <v>5.27</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1">
@@ -1730,7 +1730,7 @@
         </is>
       </c>
       <c r="D65" s="2" t="n">
-        <v>27.4</v>
+        <v>28.32</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1">
@@ -1750,7 +1750,7 @@
         </is>
       </c>
       <c r="D66" s="2" t="n">
-        <v>9.949999999999999</v>
+        <v>9.789999999999999</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1">
@@ -1770,7 +1770,7 @@
         </is>
       </c>
       <c r="D67" s="2" t="n">
-        <v>1.53</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1">
@@ -1790,7 +1790,7 @@
         </is>
       </c>
       <c r="D68" s="2" t="n">
-        <v>1.23</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1">
@@ -1810,7 +1810,7 @@
         </is>
       </c>
       <c r="D69" s="2" t="n">
-        <v>3.53</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1">
@@ -1830,7 +1830,7 @@
         </is>
       </c>
       <c r="D70" s="2" t="n">
-        <v>4.06</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1">
@@ -1850,7 +1850,7 @@
         </is>
       </c>
       <c r="D71" s="2" t="n">
-        <v>0.58</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1">
@@ -1870,7 +1870,7 @@
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>0.93</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1">
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="D73" s="2" t="n">
-        <v>2.63</v>
+        <v>2.55</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1">
@@ -1910,7 +1910,7 @@
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>2.94</v>
+        <v>2.82</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1">
@@ -1930,7 +1930,7 @@
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>7.16</v>
+        <v>6.94</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1">
@@ -1950,7 +1950,7 @@
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>4.46</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1">
@@ -1970,7 +1970,7 @@
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>0.89</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="78" ht="15" customHeight="1">
@@ -1990,7 +1990,7 @@
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>1.09</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1">
@@ -2010,7 +2010,7 @@
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>6.1</v>
+        <v>6.06</v>
       </c>
     </row>
     <row r="80" ht="15" customHeight="1">
@@ -2030,7 +2030,7 @@
         </is>
       </c>
       <c r="D80" s="2" t="n">
-        <v>3.86</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="81" ht="15" customHeight="1">
@@ -2050,7 +2050,7 @@
         </is>
       </c>
       <c r="D81" s="2" t="n">
-        <v>4.22</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="82" ht="15" customHeight="1">
@@ -2070,7 +2070,7 @@
         </is>
       </c>
       <c r="D82" s="2" t="n">
-        <v>1.71</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="83" ht="15" customHeight="1">
@@ -2090,7 +2090,7 @@
         </is>
       </c>
       <c r="D83" s="2" t="n">
-        <v>1.42</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="84" ht="15" customHeight="1">
@@ -2110,7 +2110,7 @@
         </is>
       </c>
       <c r="D84" s="2" t="n">
-        <v>11.17</v>
+        <v>10.09</v>
       </c>
     </row>
     <row r="85" ht="15" customHeight="1">
@@ -2130,7 +2130,7 @@
         </is>
       </c>
       <c r="D85" s="2" t="n">
-        <v>7</v>
+        <v>7.42</v>
       </c>
     </row>
     <row r="86" ht="15" customHeight="1">
@@ -2150,7 +2150,7 @@
         </is>
       </c>
       <c r="D86" s="2" t="n">
-        <v>17.59</v>
+        <v>17.85</v>
       </c>
     </row>
     <row r="87" ht="15" customHeight="1">
@@ -2170,7 +2170,7 @@
         </is>
       </c>
       <c r="D87" s="2" t="n">
-        <v>1.18</v>
+        <v>1.15</v>
       </c>
     </row>
     <row r="88" ht="15" customHeight="1">
@@ -2190,7 +2190,7 @@
         </is>
       </c>
       <c r="D88" s="2" t="n">
-        <v>10.04</v>
+        <v>9.539999999999999</v>
       </c>
     </row>
     <row r="89" ht="15" customHeight="1">
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="D89" s="2" t="n">
-        <v>9.01</v>
+        <v>9.130000000000001</v>
       </c>
     </row>
     <row r="90" ht="15" customHeight="1">
@@ -2230,7 +2230,7 @@
         </is>
       </c>
       <c r="D90" s="2" t="n">
-        <v>3.5</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="91" ht="15" customHeight="1">
@@ -2250,7 +2250,7 @@
         </is>
       </c>
       <c r="D91" s="2" t="n">
-        <v>1.95</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="92" ht="15" customHeight="1">
@@ -2270,7 +2270,7 @@
         </is>
       </c>
       <c r="D92" s="2" t="n">
-        <v>0.6</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="93" ht="15" customHeight="1">
@@ -2290,7 +2290,7 @@
         </is>
       </c>
       <c r="D93" s="2" t="n">
-        <v>5.76</v>
+        <v>5.31</v>
       </c>
     </row>
     <row r="94" ht="15" customHeight="1">
@@ -2330,7 +2330,7 @@
         </is>
       </c>
       <c r="D95" s="2" t="n">
-        <v>0.84</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="96" ht="15" customHeight="1">
@@ -2350,7 +2350,7 @@
         </is>
       </c>
       <c r="D96" s="2" t="n">
-        <v>0.84</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="97" ht="15" customHeight="1">
@@ -2370,7 +2370,7 @@
         </is>
       </c>
       <c r="D97" s="2" t="n">
-        <v>1.87</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="98" ht="15" customHeight="1">
@@ -2390,7 +2390,7 @@
         </is>
       </c>
       <c r="D98" s="2" t="n">
-        <v>0.96</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="99" ht="15" customHeight="1">
@@ -2410,7 +2410,7 @@
         </is>
       </c>
       <c r="D99" s="2" t="n">
-        <v>0.73</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="100" ht="15" customHeight="1">
@@ -2430,7 +2430,7 @@
         </is>
       </c>
       <c r="D100" s="2" t="n">
-        <v>1.09</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="102" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Sold Dark Petition to a hot guy
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -417,10 +417,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>10.03</v>
+        <v>9.76</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>13.81</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>17.11</v>
+        <v>17.13</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>9.81</v>
+        <v>9.26</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>8.75</v>
+        <v>8.77</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.93</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>1.66</v>
+        <v>1.63</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>1.27</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>3.45</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>2.85</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0.71</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0.63</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1">
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0.68</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1">
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="D19" s="2" t="n">
-        <v>7.82</v>
+        <v>7.81</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1">
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>2.75</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1">
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1">
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="D23" s="2" t="n">
-        <v>3.51</v>
+        <v>3.64</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>30.94</v>
+        <v>30.54</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1">
@@ -930,7 +930,7 @@
         </is>
       </c>
       <c r="D25" s="2" t="n">
-        <v>6.57</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1">
@@ -950,7 +950,7 @@
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>19.61</v>
+        <v>20.05</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="D27" s="2" t="n">
-        <v>2.23</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1">
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>0.76</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1">
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="D29" s="2" t="n">
-        <v>4.54</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1">
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>3.98</v>
+        <v>4.07</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="D31" s="2" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>0.78</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1">
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>1.02</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1">
@@ -1130,18 +1130,18 @@
         </is>
       </c>
       <c r="D35" s="2" t="n">
-        <v>15.16</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Dark Petition</t>
+          <t>Diabolic Intent</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Magic Origins</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1150,58 +1150,58 @@
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>4.83</v>
+        <v>6.61</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Diabolic Intent</t>
+          <t>Entomb</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Dominaria Remastered: Extras</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>V.2</t>
         </is>
       </c>
       <c r="D37" s="2" t="n">
-        <v>6.64</v>
+        <v>8.08</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Entomb</t>
+          <t>Gravecrawler</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Dominaria Remastered: Extras</t>
+          <t>Dark Ascension</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>V.2</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>8.119999999999999</v>
+        <v>4.14</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Gravecrawler</t>
+          <t>Painful Quandary</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1210,67 +1210,67 @@
         </is>
       </c>
       <c r="D39" s="2" t="n">
-        <v>4.39</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Painful Quandary</t>
+          <t>Scourge of the Skyclaves</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Zendikar Rising: Promos</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>V.1</t>
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>0.76</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Scourge of the Skyclaves</t>
+          <t>Sheoldred, the Apocalypse</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Zendikar Rising: Promos</t>
+          <t>Dominaria United: Promos</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>V.1</t>
+          <t>V.2</t>
         </is>
       </c>
       <c r="D41" s="2" t="n">
-        <v>1.18</v>
+        <v>54.62</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Sheoldred, the Apocalypse</t>
+          <t>The Cruelty of Gix</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Dominaria United: Promos</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>V.2</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>55.18</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1">
@@ -1290,18 +1290,18 @@
         </is>
       </c>
       <c r="D43" s="2" t="n">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1">
       <c r="A44" t="inlineStr">
         <is>
-          <t>The Cruelty of Gix</t>
+          <t>Tree of Perdition</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Eldritch Moon</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1310,18 +1310,18 @@
         </is>
       </c>
       <c r="D44" s="2" t="n">
-        <v>0.95</v>
+        <v>5.06</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Tree of Perdition</t>
+          <t>Inquisition of Kozilek</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Eldritch Moon</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1330,58 +1330,58 @@
         </is>
       </c>
       <c r="D45" s="2" t="n">
-        <v>4.76</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Inquisition of Kozilek</t>
+          <t>Deadly Dispute</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D46" s="2" t="n">
-        <v>1.05</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Deadly Dispute</t>
+          <t>Brotherhood's End</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D47" s="2" t="n">
-        <v>3.36</v>
+        <v>6.07</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Brotherhood's End</t>
+          <t>Capricious Hellraiser</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Phyrexia: All Will Be One</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1390,58 +1390,58 @@
         </is>
       </c>
       <c r="D48" s="2" t="n">
-        <v>6.35</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Capricious Hellraiser</t>
+          <t>Flame-Wreathed Phoenix</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Phyrexia: All Will Be One</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>1.53</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Flame-Wreathed Phoenix</t>
+          <t>Shivan Devastator</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D50" s="2" t="n">
-        <v>1.6</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Shivan Devastator</t>
+          <t>Skitterbeam Battalion</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1450,18 +1450,18 @@
         </is>
       </c>
       <c r="D51" s="2" t="n">
-        <v>4.84</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Skitterbeam Battalion</t>
+          <t>Vexing Devil</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Avacyn Restored</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1470,18 +1470,18 @@
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>0.9399999999999999</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Vexing Devil</t>
+          <t>Bane of Progress</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Avacyn Restored</t>
+          <t>Commander 2015</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1490,58 +1490,58 @@
         </is>
       </c>
       <c r="D53" s="2" t="n">
-        <v>4.36</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Bane of Progress</t>
+          <t>Conduit of Worlds</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Commander 2015</t>
+          <t>Phyrexia: All Will Be One: Promos</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>V.2</t>
         </is>
       </c>
       <c r="D54" s="2" t="n">
-        <v>3.36</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Conduit of Worlds</t>
+          <t>Eidolon of Blossoms</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Phyrexia: All Will Be One: Promos</t>
+          <t>Buy a Box Promos</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>V.2</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D55" s="2" t="n">
-        <v>1.26</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Eidolon of Blossoms</t>
+          <t>Fauna Shaman</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Buy a Box Promos</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1550,7 +1550,7 @@
         </is>
       </c>
       <c r="D56" s="2" t="n">
-        <v>1.54</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1">
@@ -1570,58 +1570,58 @@
         </is>
       </c>
       <c r="D57" s="2" t="n">
-        <v>1.41</v>
-      </c>
-    </row>
-    <row r="58" ht="15" customHeight="1">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="58" ht="13.5" customHeight="1">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Fauna Shaman</t>
+          <t>Fyndhorn Elves</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>30th Anniversary Celebration</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>German</t>
         </is>
       </c>
       <c r="D58" s="2" t="n">
-        <v>1.41</v>
-      </c>
-    </row>
-    <row r="59" ht="13.5" customHeight="1">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="59" ht="15" customHeight="1">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Fyndhorn Elves</t>
+          <t>Gyre Sage</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>30th Anniversary Celebration</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>German</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D59" s="2" t="n">
-        <v>1.7</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Gyre Sage</t>
+          <t>Hardened Scales</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Khans of Tarkir</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1630,27 +1630,27 @@
         </is>
       </c>
       <c r="D60" s="2" t="n">
-        <v>1.63</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Hardened Scales</t>
+          <t>Majestic Genesis</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Khans of Tarkir</t>
+          <t>Commander Legends: Battle For Baldur's Gate: Promos</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D61" s="2" t="n">
-        <v>2.61</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1">
@@ -1661,27 +1661,27 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate: Promos</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D62" s="2" t="n">
-        <v>3.53</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Majestic Genesis</t>
+          <t>Nylea, God of the Hunt</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Theros</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1690,18 +1690,18 @@
         </is>
       </c>
       <c r="D63" s="2" t="n">
-        <v>1.87</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Nylea, God of the Hunt</t>
+          <t>Parallel Lives</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Theros</t>
+          <t>Innistrad</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1710,18 +1710,18 @@
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>5.27</v>
+        <v>27.63</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Parallel Lives</t>
+          <t>Silverback Elder</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Innistrad</t>
+          <t>Dominaria United: Extras</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1730,18 +1730,18 @@
         </is>
       </c>
       <c r="D65" s="2" t="n">
-        <v>28.32</v>
+        <v>9.49</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Silverback Elder</t>
+          <t>Haywire Mite</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Dominaria United: Extras</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1750,18 +1750,18 @@
         </is>
       </c>
       <c r="D66" s="2" t="n">
-        <v>9.789999999999999</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Haywire Mite</t>
+          <t>Sphinx's Revelation</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Return to Ravnica</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1770,18 +1770,18 @@
         </is>
       </c>
       <c r="D67" s="2" t="n">
-        <v>1.55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Sphinx's Revelation</t>
+          <t>Ashiok, Nightmare Weaver</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Return to Ravnica</t>
+          <t>Theros</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1790,18 +1790,18 @@
         </is>
       </c>
       <c r="D68" s="2" t="n">
-        <v>1.04</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Ashiok, Nightmare Weaver</t>
+          <t>Mind Grind</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Theros</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1810,18 +1810,18 @@
         </is>
       </c>
       <c r="D69" s="2" t="n">
-        <v>3.52</v>
+        <v>4.19</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Mind Grind</t>
+          <t>Satoru Umezawa</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Buy a Box Promos</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1830,18 +1830,18 @@
         </is>
       </c>
       <c r="D70" s="2" t="n">
-        <v>4.17</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Satoru Umezawa</t>
+          <t>Legion's Initiative</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Buy a Box Promos</t>
+          <t>Dragon's Maze</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1850,18 +1850,18 @@
         </is>
       </c>
       <c r="D71" s="2" t="n">
-        <v>0.6</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Legion's Initiative</t>
+          <t>Expressive Iteration</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Dragon's Maze</t>
+          <t>Strixhaven: School of Mages</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1870,18 +1870,18 @@
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>0.83</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Expressive Iteration</t>
+          <t>Kolaghan's Command</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Strixhaven: School of Mages</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1890,18 +1890,18 @@
         </is>
       </c>
       <c r="D73" s="2" t="n">
-        <v>2.55</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Kolaghan's Command</t>
+          <t>Mogis, God of Slaughter</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1910,98 +1910,98 @@
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>2.82</v>
+        <v>6.76</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Mogis, God of Slaughter</t>
+          <t>Ajani, Sleeper Agent</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>6.94</v>
+        <v>4.94</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Ajani, Sleeper Agent</t>
+          <t>Ivy, Gleeful Spellthief</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Dominaria United: Promos</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>V.1</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>4.9</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Ivy, Gleeful Spellthief</t>
+          <t>Vorel of the Hull Clade</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Dominaria United: Promos</t>
+          <t>Dragon's Maze</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>V.1</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>0.96</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="78" ht="15" customHeight="1">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Vorel of the Hull Clade</t>
+          <t>Deathrite Shaman</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Dragon's Maze</t>
+          <t>Return to Ravnica</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>1.13</v>
+        <v>6.07</v>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Deathrite Shaman</t>
+          <t>The Gitrog Monster</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Return to Ravnica</t>
+          <t>Shadows over Innistrad</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2010,13 +2010,13 @@
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>6.06</v>
+        <v>3.76</v>
       </c>
     </row>
     <row r="80" ht="15" customHeight="1">
       <c r="A80" t="inlineStr">
         <is>
-          <t>The Gitrog Monster</t>
+          <t>Arlinn Kord: Arlinn, Embraced by the Moon</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2030,58 +2030,58 @@
         </is>
       </c>
       <c r="D80" s="2" t="n">
-        <v>3.87</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="81" ht="15" customHeight="1">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Arlinn Kord: Arlinn, Embraced by the Moon</t>
+          <t>Rith, Liberated Primeval V1</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Shadows over Innistrad</t>
+          <t>Dominaria United: Extras</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D81" s="2" t="n">
-        <v>3.48</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="82" ht="15" customHeight="1">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Rith, Liberated Primeval V1</t>
+          <t>Miirym, Sentinel Wyrm</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Dominaria United: Extras</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D82" s="2" t="n">
-        <v>1.62</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="83" ht="15" customHeight="1">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Miirym, Sentinel Wyrm</t>
+          <t>Aether Vial</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2090,18 +2090,18 @@
         </is>
       </c>
       <c r="D83" s="2" t="n">
-        <v>1.37</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="84" ht="15" customHeight="1">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Aether Vial</t>
+          <t>Akroma's Memorial</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Magic 2013</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2110,58 +2110,58 @@
         </is>
       </c>
       <c r="D84" s="2" t="n">
-        <v>10.09</v>
+        <v>7.28</v>
       </c>
     </row>
     <row r="85" ht="15" customHeight="1">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Akroma's Memorial</t>
+          <t>Amulet of Vigor</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Magic 2013</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D85" s="2" t="n">
-        <v>7.42</v>
+        <v>18.29</v>
       </c>
     </row>
     <row r="86" ht="15" customHeight="1">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Amulet of Vigor</t>
+          <t>Astral Cornucopia</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D86" s="2" t="n">
-        <v>17.85</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="87" ht="15" customHeight="1">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Astral Cornucopia</t>
+          <t>Coat of Arms</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2170,13 +2170,13 @@
         </is>
       </c>
       <c r="D87" s="2" t="n">
-        <v>1.15</v>
+        <v>9.699999999999999</v>
       </c>
     </row>
     <row r="88" ht="15" customHeight="1">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Coat of Arms</t>
+          <t>Dolmen Gate</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2190,18 +2190,18 @@
         </is>
       </c>
       <c r="D88" s="2" t="n">
-        <v>9.539999999999999</v>
+        <v>9.33</v>
       </c>
     </row>
     <row r="89" ht="15" customHeight="1">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Dolmen Gate</t>
+          <t>Elbrus, the Binding Blade: Withengar Unbound</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Dark Ascension</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2210,13 +2210,13 @@
         </is>
       </c>
       <c r="D89" s="2" t="n">
-        <v>9.130000000000001</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="90" ht="15" customHeight="1">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Elbrus, the Binding Blade: Withengar Unbound</t>
+          <t>Grafdigger's Cage</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2230,98 +2230,98 @@
         </is>
       </c>
       <c r="D90" s="2" t="n">
-        <v>3.08</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="91" ht="15" customHeight="1">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Grafdigger's Cage</t>
+          <t>Helm of Awakening</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>Dominaria Remastered</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D91" s="2" t="n">
-        <v>1.99</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="92" ht="15" customHeight="1">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Helm of Awakening</t>
+          <t>Illusionist's Bracers</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Dominaria Remastered</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Foil</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D92" s="2" t="n">
-        <v>0.66</v>
+        <v>4.82</v>
       </c>
     </row>
     <row r="93" ht="15" customHeight="1">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Illusionist's Bracers</t>
+          <t>Karn, Living Legacy</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Dominaria United: Promos</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>V.2</t>
         </is>
       </c>
       <c r="D93" s="2" t="n">
-        <v>5.31</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="94" ht="15" customHeight="1">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Karn, Living Legacy</t>
+          <t>Mirror Box</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Dominaria United: Promos</t>
+          <t>Kamigawa: Neon Dynasty</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>V.2</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D94" s="2" t="n">
-        <v>3.61</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="95" ht="15" customHeight="1">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Mirror Box</t>
+          <t>Clock of Omens</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Kamigawa: Neon Dynasty</t>
+          <t>Magic 2013</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2330,53 +2330,53 @@
         </is>
       </c>
       <c r="D95" s="2" t="n">
-        <v>0.76</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="96" ht="15" customHeight="1">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Clock of Omens</t>
+          <t>Mishra's Bauble</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Magic 2013</t>
+          <t>Retro Frame Artifacts</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>V.1</t>
         </is>
       </c>
       <c r="D96" s="2" t="n">
-        <v>0.5600000000000001</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="97" ht="15" customHeight="1">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Mishra's Bauble</t>
+          <t>Sol Ring</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Retro Frame Artifacts</t>
+          <t>Commander 2017</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>V.1</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D97" s="2" t="n">
-        <v>1.77</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="98" ht="15" customHeight="1">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Sol Ring</t>
+          <t>Swiftfoot Boots</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2390,52 +2390,32 @@
         </is>
       </c>
       <c r="D98" s="2" t="n">
-        <v>0.86</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="99" ht="15" customHeight="1">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Swiftfoot Boots</t>
+          <t>Pili-Pala</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Commander 2017</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Foil</t>
         </is>
       </c>
       <c r="D99" s="2" t="n">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="100" ht="15" customHeight="1">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>Pili-Pala</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Mystery Booster</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>Foil</t>
-        </is>
-      </c>
-      <c r="D100" s="2" t="n">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="102" ht="15" customHeight="1">
-      <c r="D102" s="1">
-        <f>SUM(D2:D100)</f>
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="101" ht="15" customHeight="1">
+      <c r="D101" s="1">
+        <f>SUM(D2:D99)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Sold a lot of cards to Tin and Filip :heart:
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -417,10 +417,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -469,8 +469,10 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>9.76</v>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
@@ -489,8 +491,10 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>14.25</v>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
@@ -509,8 +513,10 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D4" s="2" t="n">
-        <v>17.13</v>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
@@ -529,8 +535,10 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D5" s="2" t="n">
-        <v>9.26</v>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
@@ -549,8 +557,10 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D6" s="2" t="n">
-        <v>8.77</v>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -569,8 +579,10 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D7" s="2" t="n">
-        <v>0.59</v>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
@@ -589,8 +601,10 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D8" s="2" t="n">
-        <v>0.95</v>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
@@ -609,8 +623,10 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D9" s="2" t="n">
-        <v>1.63</v>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
@@ -629,19 +645,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D10" s="2" t="n">
-        <v>1.19</v>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Darkslick Shores</t>
+          <t>Dragonskull Summit</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Phyrexia: All Will Be One</t>
+          <t>Magic 2013</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -649,19 +667,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D11" s="2" t="n">
-        <v>3.38</v>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dragonskull Summit</t>
+          <t>Rockfall Vale</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Magic 2013</t>
+          <t>Innistrad: Midnight Hunt</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -669,19 +689,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D12" s="2" t="n">
-        <v>2.65</v>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Rockfall Vale</t>
+          <t>Temple of Epiphany</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Innistrad: Midnight Hunt</t>
+          <t>Core Set 2021</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -689,19 +711,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D13" s="2" t="n">
-        <v>0.77</v>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Temple of Epiphany</t>
+          <t>Orzhov Basilica</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Core Set 2021</t>
+          <t>Double Masters 2022: Extras</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -709,19 +733,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D14" s="2" t="n">
-        <v>0.24</v>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Orzhov Basilica</t>
+          <t>Boros Garrison</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Double Masters 2022: Extras</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -729,14 +755,16 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D15" s="2" t="n">
-        <v>0.73</v>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Boros Garrison</t>
+          <t>Selesnya Sanctuary</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -749,19 +777,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D16" s="2" t="n">
-        <v>0.1</v>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Selesnya Sanctuary</t>
+          <t>Izzet Boilerworks</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Double Masters 2022: Extras</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -769,19 +799,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D17" s="2" t="n">
-        <v>0.1</v>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Izzet Boilerworks</t>
+          <t>Jetmir's Garden</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Double Masters 2022: Extras</t>
+          <t>Streets of New Capenna</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -789,19 +821,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D18" s="2" t="n">
-        <v>0.59</v>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Jetmir's Garden</t>
+          <t>Lair of the Hydra</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Streets of New Capenna</t>
+          <t>Adventures in the Forgotten Realms</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -809,19 +843,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D19" s="2" t="n">
-        <v>7.81</v>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Lair of the Hydra</t>
+          <t>Argoth, Sanctum of Nature: Titania, Gaea Incarnate</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Adventures in the Forgotten Realms</t>
+          <t>The Brothers' War: Promos</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -829,19 +865,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D20" s="2" t="n">
-        <v>2.87</v>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Argoth, Sanctum of Nature: Titania, Gaea Incarnate</t>
+          <t>Gond Gate</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>The Brothers' War: Promos</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -849,19 +887,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D21" s="2" t="n">
-        <v>2.99</v>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Gond Gate</t>
+          <t>Maze's End</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Dragon's Maze</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -869,19 +909,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D22" s="2" t="n">
-        <v>0.75</v>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Maze's End</t>
+          <t>Nykthos, Shrine to Nyx</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Dragon's Maze</t>
+          <t>Theros</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -889,19 +931,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D23" s="2" t="n">
-        <v>3.64</v>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Nykthos, Shrine to Nyx</t>
+          <t>Ajani Steadfast</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Theros</t>
+          <t>Magic 2015</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -909,19 +953,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D24" s="2" t="n">
-        <v>30.54</v>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Ajani Steadfast</t>
+          <t>Esper Sentinel</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Magic 2015</t>
+          <t>Modern Horizons 2</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -929,19 +975,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D25" s="2" t="n">
-        <v>5.8</v>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Esper Sentinel</t>
+          <t>The Eternal Wanderer</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Modern Horizons 2</t>
+          <t>Phyrexia: All Will Be One</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -949,19 +997,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D26" s="2" t="n">
-        <v>20.05</v>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1">
       <c r="A27" t="inlineStr">
         <is>
-          <t>The Eternal Wanderer</t>
+          <t>Valiant Veteran</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Phyrexia: All Will Be One</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -969,19 +1019,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D27" s="2" t="n">
-        <v>2.13</v>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Valiant Veteran</t>
+          <t>White Plume Adventurer</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -989,19 +1041,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D28" s="2" t="n">
-        <v>0.64</v>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1">
       <c r="A29" t="inlineStr">
         <is>
-          <t>White Plume Adventurer</t>
+          <t>Sage of Hours</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Journey into Nyx</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1009,59 +1063,65 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D29" s="2" t="n">
-        <v>4.41</v>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Sage of Hours</t>
+          <t>Talrand, Sky Summoner</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Journey into Nyx</t>
+          <t>Magic 2013</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>4.07</v>
+          <t>Foil</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Talrand, Sky Summoner</t>
+          <t>Mystical Dispute</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Magic 2013</t>
+          <t>Throne of Eldraine</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Foil</t>
-        </is>
-      </c>
-      <c r="D31" s="2" t="n">
-        <v>0.75</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Mystical Dispute</t>
+          <t>Narset, Parter of Veils</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Throne of Eldraine</t>
+          <t>War of the Spark</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1069,19 +1129,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D32" s="2" t="n">
-        <v>0.6899999999999999</v>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Narset, Parter of Veils</t>
+          <t>Consider</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>War of the Spark</t>
+          <t>Innistrad: Midnight Hunt</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1089,19 +1151,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D33" s="2" t="n">
-        <v>0.83</v>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Consider</t>
+          <t>Ancient Brass Dragon</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Innistrad: Midnight Hunt</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1109,19 +1173,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D34" s="2" t="n">
-        <v>0.98</v>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Ancient Brass Dragon</t>
+          <t>Gravecrawler</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Dark Ascension</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1129,14 +1195,16 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D35" s="2" t="n">
-        <v>15.1</v>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Diabolic Intent</t>
+          <t>Painful Quandary</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1149,59 +1217,65 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D36" s="2" t="n">
-        <v>6.61</v>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Entomb</t>
+          <t>Scourge of the Skyclaves</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Dominaria Remastered: Extras</t>
+          <t>Zendikar Rising: Promos</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>V.2</t>
-        </is>
-      </c>
-      <c r="D37" s="2" t="n">
-        <v>8.08</v>
+          <t>V.1</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Gravecrawler</t>
+          <t>Sheoldred, the Apocalypse</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>Dominaria United: Promos</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D38" s="2" t="n">
-        <v>4.14</v>
+          <t>V.2</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Painful Quandary</t>
+          <t>The Cruelty of Gix</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1209,59 +1283,65 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D39" s="2" t="n">
-        <v>0.67</v>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Scourge of the Skyclaves</t>
+          <t>The Cruelty of Gix</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Zendikar Rising: Promos</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>V.1</t>
-        </is>
-      </c>
-      <c r="D40" s="2" t="n">
-        <v>1.33</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Sheoldred, the Apocalypse</t>
+          <t>Tree of Perdition</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Dominaria United: Promos</t>
+          <t>Eldritch Moon</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>V.2</t>
-        </is>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>54.62</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1">
       <c r="A42" t="inlineStr">
         <is>
-          <t>The Cruelty of Gix</t>
+          <t>Inquisition of Kozilek</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1269,39 +1349,43 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D42" s="2" t="n">
-        <v>0.96</v>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1">
       <c r="A43" t="inlineStr">
         <is>
-          <t>The Cruelty of Gix</t>
+          <t>Deadly Dispute</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D43" s="2" t="n">
-        <v>0.96</v>
+          <t>Foil</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Tree of Perdition</t>
+          <t>Brotherhood's End</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Eldritch Moon</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1309,54 +1393,60 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D44" s="2" t="n">
-        <v>5.06</v>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Inquisition of Kozilek</t>
+          <t>Flame-Wreathed Phoenix</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>0.99</v>
+          <t>Foil</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Deadly Dispute</t>
+          <t>Shivan Devastator</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Foil</t>
-        </is>
-      </c>
-      <c r="D46" s="2" t="n">
-        <v>3.39</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Brotherhood's End</t>
+          <t>Skitterbeam Battalion</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1369,19 +1459,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D47" s="2" t="n">
-        <v>6.07</v>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Capricious Hellraiser</t>
+          <t>Vexing Devil</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Phyrexia: All Will Be One</t>
+          <t>Avacyn Restored</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1389,54 +1481,60 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D48" s="2" t="n">
-        <v>1.49</v>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Flame-Wreathed Phoenix</t>
+          <t>Bane of Progress</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Commander 2015</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Foil</t>
-        </is>
-      </c>
-      <c r="D49" s="2" t="n">
-        <v>1.6</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Shivan Devastator</t>
+          <t>Conduit of Worlds</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Phyrexia: All Will Be One: Promos</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D50" s="2" t="n">
-        <v>4.95</v>
+          <t>V.2</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Skitterbeam Battalion</t>
+          <t>Fauna Shaman</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1449,19 +1547,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D51" s="2" t="n">
-        <v>0.87</v>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Vexing Devil</t>
+          <t>Fauna Shaman</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Avacyn Restored</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1469,59 +1569,65 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D52" s="2" t="n">
-        <v>4.17</v>
-      </c>
-    </row>
-    <row r="53" ht="15" customHeight="1">
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="53" ht="13.5" customHeight="1">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Bane of Progress</t>
+          <t>Fyndhorn Elves</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Commander 2015</t>
+          <t>30th Anniversary Celebration</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D53" s="2" t="n">
-        <v>3.14</v>
+          <t>German</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Conduit of Worlds</t>
+          <t>Gyre Sage</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Phyrexia: All Will Be One: Promos</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>V.2</t>
-        </is>
-      </c>
-      <c r="D54" s="2" t="n">
-        <v>1.56</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Eidolon of Blossoms</t>
+          <t>Hardened Scales</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Buy a Box Promos</t>
+          <t>Khans of Tarkir</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1529,39 +1635,43 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D55" s="2" t="n">
-        <v>1.3</v>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Fauna Shaman</t>
+          <t>Majestic Genesis</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Commander Legends: Battle For Baldur's Gate: Promos</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D56" s="2" t="n">
-        <v>1.28</v>
+          <t>Foil</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Fauna Shaman</t>
+          <t>Majestic Genesis</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1569,39 +1679,43 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D57" s="2" t="n">
-        <v>1.28</v>
-      </c>
-    </row>
-    <row r="58" ht="13.5" customHeight="1">
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" ht="15" customHeight="1">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Fyndhorn Elves</t>
+          <t>Nylea, God of the Hunt</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>30th Anniversary Celebration</t>
+          <t>Theros</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>German</t>
-        </is>
-      </c>
-      <c r="D58" s="2" t="n">
-        <v>1.61</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Gyre Sage</t>
+          <t>Parallel Lives</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Innistrad</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1609,19 +1723,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D59" s="2" t="n">
-        <v>1.73</v>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Hardened Scales</t>
+          <t>Silverback Elder</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Khans of Tarkir</t>
+          <t>Dominaria United: Extras</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1629,39 +1745,43 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D60" s="2" t="n">
-        <v>2.63</v>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Majestic Genesis</t>
+          <t>Haywire Mite</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate: Promos</t>
+          <t>The Brothers' War</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Foil</t>
-        </is>
-      </c>
-      <c r="D61" s="2" t="n">
-        <v>3.28</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Majestic Genesis</t>
+          <t>Sphinx's Revelation</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Return to Ravnica</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1669,14 +1789,16 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D62" s="2" t="n">
-        <v>1.83</v>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Nylea, God of the Hunt</t>
+          <t>Ashiok, Nightmare Weaver</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1689,19 +1811,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D63" s="2" t="n">
-        <v>4.95</v>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Parallel Lives</t>
+          <t>Mind Grind</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Innistrad</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1709,19 +1833,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D64" s="2" t="n">
-        <v>27.63</v>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Silverback Elder</t>
+          <t>Satoru Umezawa</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Dominaria United: Extras</t>
+          <t>Buy a Box Promos</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1729,19 +1855,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D65" s="2" t="n">
-        <v>9.49</v>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Haywire Mite</t>
+          <t>Legion's Initiative</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>The Brothers' War</t>
+          <t>Dragon's Maze</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1749,19 +1877,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D66" s="2" t="n">
-        <v>1.56</v>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Sphinx's Revelation</t>
+          <t>Expressive Iteration</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Return to Ravnica</t>
+          <t>Strixhaven: School of Mages</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1769,19 +1899,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D67" s="2" t="n">
-        <v>1</v>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Ashiok, Nightmare Weaver</t>
+          <t>Kolaghan's Command</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Theros</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1789,19 +1921,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D68" s="2" t="n">
-        <v>3.49</v>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Mind Grind</t>
+          <t>Mogis, God of Slaughter</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1809,79 +1943,87 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D69" s="2" t="n">
-        <v>4.19</v>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Satoru Umezawa</t>
+          <t>Ajani, Sleeper Agent</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Buy a Box Promos</t>
+          <t>Dominaria United</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D70" s="2" t="n">
-        <v>0.64</v>
+          <t>Foil</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Legion's Initiative</t>
+          <t>Ivy, Gleeful Spellthief</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Dragon's Maze</t>
+          <t>Dominaria United: Promos</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D71" s="2" t="n">
-        <v>0.76</v>
+          <t>V.1</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Expressive Iteration</t>
+          <t>Vorel of the Hull Clade</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Strixhaven: School of Mages</t>
+          <t>Dragon's Maze</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D72" s="2" t="n">
-        <v>2.6</v>
+          <t>Foil</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Kolaghan's Command</t>
+          <t>Deathrite Shaman</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Return to Ravnica</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1889,19 +2031,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D73" s="2" t="n">
-        <v>2.95</v>
+      <c r="D73" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Mogis, God of Slaughter</t>
+          <t>The Gitrog Monster</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Shadows over Innistrad</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1909,79 +2053,87 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D74" s="2" t="n">
-        <v>6.76</v>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Ajani, Sleeper Agent</t>
+          <t>Arlinn Kord: Arlinn, Embraced by the Moon</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Dominaria United</t>
+          <t>Shadows over Innistrad</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Foil</t>
-        </is>
-      </c>
-      <c r="D75" s="2" t="n">
-        <v>4.94</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Ivy, Gleeful Spellthief</t>
+          <t>Rith, Liberated Primeval V1</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Dominaria United: Promos</t>
+          <t>Dominaria United: Extras</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>V.1</t>
-        </is>
-      </c>
-      <c r="D76" s="2" t="n">
-        <v>0.96</v>
+          <t>Foil</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Vorel of the Hull Clade</t>
+          <t>Miirym, Sentinel Wyrm</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Dragon's Maze</t>
+          <t>Commander Legends: Battle For Baldur's Gate</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Foil</t>
-        </is>
-      </c>
-      <c r="D77" s="2" t="n">
-        <v>1.21</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D77" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="78" ht="15" customHeight="1">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Deathrite Shaman</t>
+          <t>Aether Vial</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Return to Ravnica</t>
+          <t>Double Masters 2022</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1989,19 +2141,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D78" s="2" t="n">
-        <v>6.07</v>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1">
       <c r="A79" t="inlineStr">
         <is>
-          <t>The Gitrog Monster</t>
+          <t>Akroma's Memorial</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Shadows over Innistrad</t>
+          <t>Magic 2013</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2009,59 +2163,65 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D79" s="2" t="n">
-        <v>3.76</v>
+      <c r="D79" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="80" ht="15" customHeight="1">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Arlinn Kord: Arlinn, Embraced by the Moon</t>
+          <t>Amulet of Vigor</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Shadows over Innistrad</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D80" s="2" t="n">
-        <v>3.47</v>
+          <t>Foil</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="81" ht="15" customHeight="1">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Rith, Liberated Primeval V1</t>
+          <t>Astral Cornucopia</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Dominaria United: Extras</t>
+          <t>Born of the Gods</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Foil</t>
-        </is>
-      </c>
-      <c r="D81" s="2" t="n">
-        <v>1.44</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="82" ht="15" customHeight="1">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Miirym, Sentinel Wyrm</t>
+          <t>Coat of Arms</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Commander Legends: Battle For Baldur's Gate</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2069,19 +2229,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D82" s="2" t="n">
-        <v>1.38</v>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="83" ht="15" customHeight="1">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Aether Vial</t>
+          <t>Dolmen Gate</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Double Masters 2022</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2089,19 +2251,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D83" s="2" t="n">
-        <v>9.6</v>
+      <c r="D83" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="84" ht="15" customHeight="1">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Akroma's Memorial</t>
+          <t>Elbrus, the Binding Blade: Withengar Unbound</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Magic 2013</t>
+          <t>Dark Ascension</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2109,59 +2273,65 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D84" s="2" t="n">
-        <v>7.28</v>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="85" ht="15" customHeight="1">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Amulet of Vigor</t>
+          <t>Grafdigger's Cage</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Dark Ascension</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Foil</t>
-        </is>
-      </c>
-      <c r="D85" s="2" t="n">
-        <v>18.29</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D85" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="86" ht="15" customHeight="1">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Astral Cornucopia</t>
+          <t>Helm of Awakening</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Born of the Gods</t>
+          <t>Dominaria Remastered</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D86" s="2" t="n">
-        <v>1.07</v>
+          <t>Foil</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="87" ht="15" customHeight="1">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Coat of Arms</t>
+          <t>Illusionist's Bracers</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Gatecrash</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2169,39 +2339,43 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D87" s="2" t="n">
-        <v>9.699999999999999</v>
+      <c r="D87" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="88" ht="15" customHeight="1">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Dolmen Gate</t>
+          <t>Karn, Living Legacy</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Mystery Booster</t>
+          <t>Dominaria United: Promos</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D88" s="2" t="n">
-        <v>9.33</v>
+          <t>V.2</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="89" ht="15" customHeight="1">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Elbrus, the Binding Blade: Withengar Unbound</t>
+          <t>Mirror Box</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>Kamigawa: Neon Dynasty</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2209,19 +2383,21 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D89" s="2" t="n">
-        <v>3.28</v>
+      <c r="D89" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="90" ht="15" customHeight="1">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Grafdigger's Cage</t>
+          <t>Clock of Omens</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Dark Ascension</t>
+          <t>Magic 2013</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2229,39 +2405,43 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D90" s="2" t="n">
-        <v>1.9</v>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="91" ht="15" customHeight="1">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Helm of Awakening</t>
+          <t>Mishra's Bauble</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Dominaria Remastered</t>
+          <t>Retro Frame Artifacts</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Foil</t>
-        </is>
-      </c>
-      <c r="D91" s="2" t="n">
-        <v>0.61</v>
+          <t>V.1</t>
+        </is>
+      </c>
+      <c r="D91" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="92" ht="15" customHeight="1">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Illusionist's Bracers</t>
+          <t>Sol Ring</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Gatecrash</t>
+          <t>Commander 2017</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2269,153 +2449,59 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="D92" s="2" t="n">
-        <v>4.82</v>
+      <c r="D92" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="93" ht="15" customHeight="1">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Karn, Living Legacy</t>
+          <t>Swiftfoot Boots</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Dominaria United: Promos</t>
+          <t>Commander 2017</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>V.2</t>
-        </is>
-      </c>
-      <c r="D93" s="2" t="n">
-        <v>3.61</v>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="D93" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="94" ht="15" customHeight="1">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Mirror Box</t>
+          <t>Pili-Pala</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Kamigawa: Neon Dynasty</t>
+          <t>Mystery Booster</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D94" s="2" t="n">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="95" ht="15" customHeight="1">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>Clock of Omens</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>Magic 2013</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D95" s="2" t="n">
-        <v>0.59</v>
+          <t>Foil</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
     </row>
     <row r="96" ht="15" customHeight="1">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>Mishra's Bauble</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Retro Frame Artifacts</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>V.1</t>
-        </is>
-      </c>
-      <c r="D96" s="2" t="n">
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="97" ht="15" customHeight="1">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>Sol Ring</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Commander 2017</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D97" s="2" t="n">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="98" ht="15" customHeight="1">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>Swiftfoot Boots</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Commander 2017</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="D98" s="2" t="n">
-        <v>0.6899999999999999</v>
-      </c>
-    </row>
-    <row r="99" ht="15" customHeight="1">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>Pili-Pala</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Mystery Booster</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>Foil</t>
-        </is>
-      </c>
-      <c r="D99" s="2" t="n">
-        <v>1.36</v>
-      </c>
-    </row>
-    <row r="101" ht="15" customHeight="1">
-      <c r="D101" s="1">
-        <f>SUM(D2:D99)</f>
+      <c r="D96" s="1">
+        <f>SUM(D2:D94)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Upgraded the new deck
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\o\git-repos\mtg-card-price-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A267B96D-19C1-4AA5-AB29-E22DED710EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D563FF5E-8F1D-4E4C-B72B-BB95668DBB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="142">
   <si>
     <t>Name</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Sacred Foundry</t>
   </si>
   <si>
-    <t>Blood Crypt</t>
-  </si>
-  <si>
     <t>Return to Ravnica</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>The Brothers' War</t>
   </si>
   <si>
-    <t>Dragonskull Summit</t>
-  </si>
-  <si>
     <t>Magic 2013</t>
   </si>
   <si>
@@ -209,9 +203,6 @@
     <t>Consider</t>
   </si>
   <si>
-    <t>Ancient Brass Dragon</t>
-  </si>
-  <si>
     <t>Gravecrawler</t>
   </si>
   <si>
@@ -227,9 +218,6 @@
     <t>V.1</t>
   </si>
   <si>
-    <t>Sheoldred, the Apocalypse</t>
-  </si>
-  <si>
     <t>Dominaria United: Promos</t>
   </si>
   <si>
@@ -239,18 +227,9 @@
     <t>The Cruelty of Gix</t>
   </si>
   <si>
-    <t>Tree of Perdition</t>
-  </si>
-  <si>
-    <t>Eldritch Moon</t>
-  </si>
-  <si>
     <t>Inquisition of Kozilek</t>
   </si>
   <si>
-    <t>Deadly Dispute</t>
-  </si>
-  <si>
     <t>Flame-Wreathed Phoenix</t>
   </si>
   <si>
@@ -347,12 +326,6 @@
     <t>Strixhaven: School of Mages</t>
   </si>
   <si>
-    <t>Kolaghan's Command</t>
-  </si>
-  <si>
-    <t>Mogis, God of Slaughter</t>
-  </si>
-  <si>
     <t>Ajani, Sleeper Agent</t>
   </si>
   <si>
@@ -447,15 +420,6 @@
   </si>
   <si>
     <t>March of the Machine: Promos</t>
-  </si>
-  <si>
-    <t>Chandra, Hope's Beacon</t>
-  </si>
-  <si>
-    <t>Goldspan Dragon</t>
-  </si>
-  <si>
-    <t>Kaldheim: Promos</t>
   </si>
   <si>
     <t>Extra: Pokemon</t>
@@ -504,7 +468,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* \-??\ [$€-1]_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00\ [$€-1]"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -546,8 +510,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -851,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,16 +873,16 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>17.59</v>
+        <v>9.5399999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -926,102 +890,102 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2">
-        <v>9.5399999999999991</v>
+        <v>9.1199999999999992</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="2">
-        <v>9.1199999999999992</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="2">
-        <v>0.79</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="2">
-        <v>0.89</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="2">
-        <v>2.75</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="2">
-        <v>0.72</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="2">
-        <v>0.27</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -1030,21 +994,21 @@
         <v>6</v>
       </c>
       <c r="D12" s="2">
-        <v>0.85</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="2">
-        <v>0.09</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1052,125 +1016,125 @@
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="2">
-        <v>0.14000000000000001</v>
+        <v>7.76</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="2">
-        <v>0.6</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="2">
-        <v>7.76</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="2">
-        <v>2.87</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="2">
-        <v>3.02</v>
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="2">
-        <v>0.69</v>
+        <v>31.36</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="2">
-        <v>4.1500000000000004</v>
+        <v>6.35</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="2">
-        <v>31.36</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D22" s="2">
-        <v>6.35</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1184,35 +1148,35 @@
         <v>6</v>
       </c>
       <c r="D23" s="2">
-        <v>20.2</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D24" s="2">
-        <v>1.24</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="2">
-        <v>1.94</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1220,1011 +1184,857 @@
         <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="2">
-        <v>0.79</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D27" s="2">
-        <v>4.0999999999999996</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="2">
-        <v>4.2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D29" s="2">
-        <v>0.69</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="2">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" s="2">
-        <v>0.81</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D32" s="2">
-        <v>0.9</v>
+        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="2">
-        <v>14.7</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="2">
-        <v>3.41</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D35" s="2">
-        <v>1.1399999999999999</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D36" s="2">
-        <v>57.47</v>
+        <v>4.8600000000000003</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="2">
-        <v>0.83</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="2">
-        <v>0.83</v>
+        <v>5.21</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="2">
-        <v>5.3</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D40" s="2">
-        <v>0.89</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D41" s="2">
-        <v>3.08</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>17</v>
       </c>
       <c r="C42" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D42" s="2">
-        <v>4.41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="D43" s="2">
-        <v>1.74</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>140</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D44" s="2">
-        <v>11.34</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="2">
-        <v>4.8600000000000003</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D46" s="2">
-        <v>0.77</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47" s="2">
-        <v>5.21</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="2">
-        <v>3.32</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C49" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D49" s="2">
-        <v>1.99</v>
+        <v>27.28</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
       </c>
       <c r="D50" s="2">
-        <v>1.27</v>
+        <v>8.7200000000000006</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="2">
-        <v>1.27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="D52" s="2">
-        <v>1.38</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="2">
-        <v>1.18</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="2">
-        <v>2.98</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B55" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C55" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D55" s="2">
-        <v>3.28</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="2">
-        <v>1.82</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="2">
-        <v>4.41</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B58" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D58" s="2">
-        <v>27.28</v>
+        <v>5.27</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D59" s="2">
-        <v>8.7200000000000006</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B60" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D60" s="2">
-        <v>1.79</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="2">
-        <v>1.34</v>
+        <v>5.68</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62" s="2">
-        <v>3.44</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="2">
-        <v>4.28</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B64" t="s">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D64" s="2">
-        <v>0.61</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B65" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="2">
-        <v>0.82</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>26</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" s="2">
-        <v>2.79</v>
+        <v>8.76</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B67" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" s="2">
-        <v>3.01</v>
+        <v>7.73</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B68" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D68" s="2">
-        <v>5.66</v>
+        <v>18.46</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B69" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="C69" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D69" s="2">
-        <v>5.27</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B70" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="C70" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="D70" s="2">
-        <v>1.1499999999999999</v>
+        <v>9.85</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B71" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="C71" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D71" s="2">
-        <v>1.3</v>
+        <v>9.2899999999999991</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="C72" t="s">
         <v>6</v>
       </c>
       <c r="D72" s="2">
-        <v>5.68</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B73" t="s">
-        <v>111</v>
+        <v>57</v>
       </c>
       <c r="C73" t="s">
         <v>6</v>
       </c>
       <c r="D73" s="2">
-        <v>3.67</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D74" s="2">
-        <v>3.36</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B75" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D75" s="2">
-        <v>0.76</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B76" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D76" s="2">
-        <v>1.48</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B77" t="s">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" s="2">
-        <v>8.76</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B78" t="s">
-        <v>20</v>
+        <v>122</v>
       </c>
       <c r="C78" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D78" s="2">
-        <v>7.73</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B79" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C79" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D79" s="2">
-        <v>18.46</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B80" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" s="2">
-        <v>1.41</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B81" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C81" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D81" s="2">
-        <v>9.85</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>121</v>
-      </c>
-      <c r="B82" t="s">
-        <v>118</v>
-      </c>
-      <c r="C82" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" s="2">
-        <v>9.2899999999999991</v>
-      </c>
+      <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>122</v>
-      </c>
-      <c r="B83" t="s">
-        <v>60</v>
-      </c>
-      <c r="C83" t="s">
-        <v>6</v>
-      </c>
-      <c r="D83" s="2">
-        <v>3.45</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B84" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
       <c r="C84" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" s="2">
-        <v>1.94</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="D84" s="3">
+        <v>11.15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B85" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C85" t="s">
-        <v>52</v>
-      </c>
-      <c r="D85" s="2">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="D85" s="3">
+        <v>41.91</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>137</v>
       </c>
       <c r="C86" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" s="2">
-        <v>5.64</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="D86" s="3">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B87" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="C87" t="s">
-        <v>66</v>
-      </c>
-      <c r="D87" s="2">
-        <v>3.42</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>128</v>
-      </c>
-      <c r="B88" t="s">
-        <v>129</v>
-      </c>
-      <c r="C88" t="s">
-        <v>6</v>
-      </c>
-      <c r="D88" s="2">
-        <v>0.84</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="D87" s="3">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="3"/>
     </row>
     <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>130</v>
-      </c>
-      <c r="B89" t="s">
-        <v>131</v>
-      </c>
-      <c r="C89" t="s">
-        <v>63</v>
-      </c>
-      <c r="D89" s="2">
-        <v>1.88</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>132</v>
-      </c>
-      <c r="B90" t="s">
-        <v>133</v>
-      </c>
-      <c r="C90" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" s="2">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>134</v>
-      </c>
-      <c r="B91" t="s">
-        <v>133</v>
-      </c>
-      <c r="C91" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" s="2">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>135</v>
-      </c>
-      <c r="B92" t="s">
-        <v>118</v>
-      </c>
-      <c r="C92" t="s">
-        <v>52</v>
-      </c>
-      <c r="D92" s="2">
-        <v>1.27</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D93" s="2"/>
-    </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>141</v>
-      </c>
-      <c r="D94" s="2"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>145</v>
-      </c>
-      <c r="B95" t="s">
-        <v>146</v>
-      </c>
-      <c r="C95" t="s">
-        <v>147</v>
-      </c>
-      <c r="D95" s="3">
-        <v>11.15</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>142</v>
-      </c>
-      <c r="B96" t="s">
-        <v>143</v>
-      </c>
-      <c r="C96" t="s">
-        <v>144</v>
-      </c>
-      <c r="D96" s="3">
-        <v>41.91</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>148</v>
-      </c>
-      <c r="B97" t="s">
-        <v>149</v>
-      </c>
-      <c r="C97" t="s">
-        <v>150</v>
-      </c>
-      <c r="D97" s="3">
-        <v>4.25</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>151</v>
-      </c>
-      <c r="B98" t="s">
-        <v>152</v>
-      </c>
-      <c r="C98" t="s">
-        <v>153</v>
-      </c>
-      <c r="D98" s="3">
-        <v>4.54</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="3"/>
-    </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D100" s="3">
-        <f>SUM(D2:D98)</f>
-        <v>516.41999999999996</v>
+      <c r="D89" s="3">
+        <f>SUM(D2:D87)</f>
+        <v>390.34999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Didn't pull a fetch :sob:
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\o\git-repos\mtg-card-price-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D563FF5E-8F1D-4E4C-B72B-BB95668DBB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58080733-2A63-44DE-AC88-7A6F1464C7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="143">
   <si>
     <t>Name</t>
   </si>
@@ -459,6 +459,9 @@
   </si>
   <si>
     <t>BW36</t>
+  </si>
+  <si>
+    <t>Mirari's Wake</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* \-??\ [$€-1]_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00\ [$€-1]"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1]"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -510,8 +513,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -815,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,63 +1646,63 @@
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C59" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D59" s="2">
-        <v>1.1499999999999999</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D60" s="2">
-        <v>1.3</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B61" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D61" s="2">
-        <v>5.68</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B62" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62" s="2">
-        <v>3.67</v>
+        <v>5.68</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B63" t="s">
         <v>102</v>
@@ -1708,110 +1711,110 @@
         <v>6</v>
       </c>
       <c r="D63" s="2">
-        <v>3.36</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B64" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="C64" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D64" s="2">
-        <v>0.76</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B65" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D65" s="2">
-        <v>1.48</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B66" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" s="2">
-        <v>8.76</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B67" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" s="2">
-        <v>7.73</v>
+        <v>8.76</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B68" t="s">
-        <v>109</v>
+        <v>18</v>
       </c>
       <c r="C68" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D68" s="2">
-        <v>18.46</v>
+        <v>7.73</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B69" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D69" s="2">
-        <v>1.41</v>
+        <v>18.46</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B70" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="C70" t="s">
         <v>6</v>
       </c>
       <c r="D70" s="2">
-        <v>9.85</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B71" t="s">
         <v>109</v>
@@ -1820,26 +1823,26 @@
         <v>6</v>
       </c>
       <c r="D71" s="2">
-        <v>9.2899999999999991</v>
+        <v>9.85</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B72" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="C72" t="s">
         <v>6</v>
       </c>
       <c r="D72" s="2">
-        <v>3.45</v>
+        <v>9.2899999999999991</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B73" t="s">
         <v>57</v>
@@ -1848,96 +1851,96 @@
         <v>6</v>
       </c>
       <c r="D73" s="2">
-        <v>1.94</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B74" t="s">
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="C74" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D74" s="2">
-        <v>0.56999999999999995</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="C75" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D75" s="2">
-        <v>5.64</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B76" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D76" s="2">
-        <v>3.42</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B77" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D77" s="2">
-        <v>0.84</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B78" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C78" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D78" s="2">
-        <v>1.88</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B79" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C79" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D79" s="2">
-        <v>0.93</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B80" t="s">
         <v>124</v>
@@ -1946,95 +1949,109 @@
         <v>6</v>
       </c>
       <c r="D80" s="2">
-        <v>0.84</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" t="s">
+        <v>124</v>
+      </c>
+      <c r="C81" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="2">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>126</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>109</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>50</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D82" s="2">
         <v>1.27</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D82" s="2"/>
-    </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>129</v>
       </c>
-      <c r="D83" s="2"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>133</v>
-      </c>
-      <c r="B84" t="s">
-        <v>134</v>
-      </c>
-      <c r="C84" t="s">
-        <v>135</v>
-      </c>
-      <c r="D84" s="3">
-        <v>11.15</v>
-      </c>
+      <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B85" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C85" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D85" s="3">
-        <v>41.91</v>
+        <v>11.15</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B86" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C86" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D86" s="3">
-        <v>4.25</v>
+        <v>41.91</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>136</v>
+      </c>
+      <c r="B87" t="s">
+        <v>137</v>
+      </c>
+      <c r="C87" t="s">
+        <v>138</v>
+      </c>
+      <c r="D87" s="3">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>139</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>140</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>141</v>
       </c>
-      <c r="D87" s="3">
+      <c r="D88" s="3">
         <v>4.54</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D88" s="3"/>
-    </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D89" s="3">
-        <f>SUM(D2:D87)</f>
-        <v>390.34999999999997</v>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="3"/>
+    </row>
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D90" s="3">
+        <f>SUM(D2:D88)</f>
+        <v>393.14000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I can't believe I paid 10.50€ for this
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\o\git-repos\mtg-card-price-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58080733-2A63-44DE-AC88-7A6F1464C7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4919A9-43DA-4373-A309-88CDA30A6E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="144">
   <si>
     <t>Name</t>
   </si>
@@ -462,6 +462,9 @@
   </si>
   <si>
     <t>Mirari's Wake</t>
+  </si>
+  <si>
+    <t>Titania, Protector of Argoth</t>
   </si>
 </sst>
 </file>
@@ -820,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,7 +860,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2">
-        <v>8.11</v>
+        <v>9.92</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -871,7 +874,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="2">
-        <v>13.77</v>
+        <v>14.13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -885,7 +888,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>9.5399999999999991</v>
+        <v>9.85</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -899,7 +902,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="2">
-        <v>9.1199999999999992</v>
+        <v>8.51</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -913,7 +916,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="2">
-        <v>0.79</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -927,7 +930,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="2">
-        <v>0.89</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -941,7 +944,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="2">
-        <v>0.72</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -955,7 +958,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="2">
-        <v>0.27</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -969,7 +972,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="2">
-        <v>0.85</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -983,7 +986,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="2">
-        <v>0.09</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -997,7 +1000,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="2">
-        <v>0.14000000000000001</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1011,7 +1014,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="2">
-        <v>0.6</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1025,7 +1028,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="2">
-        <v>7.76</v>
+        <v>7.84</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1039,7 +1042,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="2">
-        <v>2.87</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1053,7 +1056,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="2">
-        <v>3.02</v>
+        <v>2.92</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1067,7 +1070,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="2">
-        <v>0.69</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1081,7 +1084,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="2">
-        <v>4.1500000000000004</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1095,7 +1098,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="2">
-        <v>31.36</v>
+        <v>33.119999999999997</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1109,7 +1112,7 @@
         <v>6</v>
       </c>
       <c r="D20" s="2">
-        <v>6.35</v>
+        <v>6.86</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1123,7 +1126,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="2">
-        <v>20.2</v>
+        <v>20.58</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1137,7 +1140,7 @@
         <v>62</v>
       </c>
       <c r="D22" s="2">
-        <v>1.24</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1151,7 +1154,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="2">
-        <v>1.94</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1165,7 +1168,7 @@
         <v>6</v>
       </c>
       <c r="D24" s="2">
-        <v>0.79</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1179,7 +1182,7 @@
         <v>6</v>
       </c>
       <c r="D25" s="2">
-        <v>4.0999999999999996</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1193,7 +1196,7 @@
         <v>6</v>
       </c>
       <c r="D26" s="2">
-        <v>4.2</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1207,7 +1210,7 @@
         <v>50</v>
       </c>
       <c r="D27" s="2">
-        <v>0.69</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1221,7 +1224,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="2">
-        <v>0.7</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1235,7 +1238,7 @@
         <v>6</v>
       </c>
       <c r="D29" s="2">
-        <v>0.81</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1249,7 +1252,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="2">
-        <v>0.9</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1263,7 +1266,7 @@
         <v>6</v>
       </c>
       <c r="D31" s="2">
-        <v>3.41</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1277,7 +1280,7 @@
         <v>60</v>
       </c>
       <c r="D32" s="2">
-        <v>1.1399999999999999</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1291,7 +1294,7 @@
         <v>6</v>
       </c>
       <c r="D33" s="2">
-        <v>0.9</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1305,7 +1308,7 @@
         <v>6</v>
       </c>
       <c r="D34" s="2">
-        <v>0.89</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1319,7 +1322,7 @@
         <v>50</v>
       </c>
       <c r="D35" s="2">
-        <v>1.74</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1333,7 +1336,7 @@
         <v>6</v>
       </c>
       <c r="D36" s="2">
-        <v>4.8600000000000003</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1347,7 +1350,7 @@
         <v>6</v>
       </c>
       <c r="D37" s="2">
-        <v>0.77</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1361,7 +1364,7 @@
         <v>6</v>
       </c>
       <c r="D38" s="2">
-        <v>5.21</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1375,7 +1378,7 @@
         <v>6</v>
       </c>
       <c r="D39" s="2">
-        <v>3.32</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1389,7 +1392,7 @@
         <v>62</v>
       </c>
       <c r="D40" s="2">
-        <v>1.99</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1403,63 +1406,63 @@
         <v>6</v>
       </c>
       <c r="D41" s="2">
-        <v>1.27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="D42" s="2">
-        <v>1.27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="D43" s="2">
-        <v>1.38</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="2">
-        <v>1.18</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D45" s="2">
-        <v>2.98</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1467,69 +1470,69 @@
         <v>82</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D46" s="2">
-        <v>3.28</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47" s="2">
-        <v>1.82</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="2">
-        <v>4.41</v>
+        <v>27.94</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
       </c>
       <c r="D49" s="2">
-        <v>27.28</v>
+        <v>9.86</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>143</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D50" s="2">
-        <v>8.7200000000000006</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1543,7 +1546,7 @@
         <v>6</v>
       </c>
       <c r="D51" s="2">
-        <v>1.79</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1557,7 +1560,7 @@
         <v>6</v>
       </c>
       <c r="D52" s="2">
-        <v>1.34</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1571,7 +1574,7 @@
         <v>6</v>
       </c>
       <c r="D53" s="2">
-        <v>3.44</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1585,7 +1588,7 @@
         <v>6</v>
       </c>
       <c r="D54" s="2">
-        <v>4.28</v>
+        <v>3.86</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1599,7 +1602,7 @@
         <v>6</v>
       </c>
       <c r="D55" s="2">
-        <v>0.61</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1613,7 +1616,7 @@
         <v>6</v>
       </c>
       <c r="D56" s="2">
-        <v>0.82</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1627,7 +1630,7 @@
         <v>6</v>
       </c>
       <c r="D57" s="2">
-        <v>2.79</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1641,7 +1644,7 @@
         <v>50</v>
       </c>
       <c r="D58" s="2">
-        <v>5.27</v>
+        <v>4.54</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1652,10 +1655,10 @@
         <v>42</v>
       </c>
       <c r="C59" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D59" s="2">
-        <v>2.79</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1669,7 +1672,7 @@
         <v>60</v>
       </c>
       <c r="D60" s="2">
-        <v>1.1499999999999999</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1683,7 +1686,7 @@
         <v>50</v>
       </c>
       <c r="D61" s="2">
-        <v>1.3</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1697,7 +1700,7 @@
         <v>6</v>
       </c>
       <c r="D62" s="2">
-        <v>5.68</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1711,7 +1714,7 @@
         <v>6</v>
       </c>
       <c r="D63" s="2">
-        <v>3.67</v>
+        <v>3.93</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1725,7 +1728,7 @@
         <v>6</v>
       </c>
       <c r="D64" s="2">
-        <v>3.36</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1739,7 +1742,7 @@
         <v>50</v>
       </c>
       <c r="D65" s="2">
-        <v>0.76</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1753,7 +1756,7 @@
         <v>6</v>
       </c>
       <c r="D66" s="2">
-        <v>1.48</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1767,7 +1770,7 @@
         <v>6</v>
       </c>
       <c r="D67" s="2">
-        <v>8.76</v>
+        <v>8.83</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1781,7 +1784,7 @@
         <v>6</v>
       </c>
       <c r="D68" s="2">
-        <v>7.73</v>
+        <v>8.3699999999999992</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1795,7 +1798,7 @@
         <v>50</v>
       </c>
       <c r="D69" s="2">
-        <v>18.46</v>
+        <v>17.809999999999999</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1809,7 +1812,7 @@
         <v>6</v>
       </c>
       <c r="D70" s="2">
-        <v>1.41</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1823,7 +1826,7 @@
         <v>6</v>
       </c>
       <c r="D71" s="2">
-        <v>9.85</v>
+        <v>9.4600000000000009</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1837,7 +1840,7 @@
         <v>6</v>
       </c>
       <c r="D72" s="2">
-        <v>9.2899999999999991</v>
+        <v>8.93</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1851,7 +1854,7 @@
         <v>6</v>
       </c>
       <c r="D73" s="2">
-        <v>3.45</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1865,7 +1868,7 @@
         <v>6</v>
       </c>
       <c r="D74" s="2">
-        <v>1.94</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1879,7 +1882,7 @@
         <v>50</v>
       </c>
       <c r="D75" s="2">
-        <v>0.56999999999999995</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1893,7 +1896,7 @@
         <v>6</v>
       </c>
       <c r="D76" s="2">
-        <v>5.64</v>
+        <v>4.8099999999999996</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1907,7 +1910,7 @@
         <v>62</v>
       </c>
       <c r="D77" s="2">
-        <v>3.42</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1921,7 +1924,7 @@
         <v>6</v>
       </c>
       <c r="D78" s="2">
-        <v>0.84</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1935,7 +1938,7 @@
         <v>60</v>
       </c>
       <c r="D79" s="2">
-        <v>1.88</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1949,7 +1952,7 @@
         <v>6</v>
       </c>
       <c r="D80" s="2">
-        <v>0.93</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1963,7 +1966,7 @@
         <v>6</v>
       </c>
       <c r="D81" s="2">
-        <v>0.84</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1977,7 +1980,7 @@
         <v>50</v>
       </c>
       <c r="D82" s="2">
-        <v>1.27</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2000,7 +2003,7 @@
         <v>135</v>
       </c>
       <c r="D85" s="3">
-        <v>11.15</v>
+        <v>11.52</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2014,7 +2017,7 @@
         <v>132</v>
       </c>
       <c r="D86" s="3">
-        <v>41.91</v>
+        <v>38.479999999999997</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2028,7 +2031,7 @@
         <v>138</v>
       </c>
       <c r="D87" s="3">
-        <v>4.25</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2042,7 +2045,7 @@
         <v>141</v>
       </c>
       <c r="D88" s="3">
-        <v>4.54</v>
+        <v>5.0199999999999996</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2051,7 +2054,7 @@
     <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D90" s="3">
         <f>SUM(D2:D88)</f>
-        <v>393.14000000000004</v>
+        <v>388.15999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I pulled that card with which Dean won a draft on Arena, I miss you a lot Dean, I love you
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\o\git-repos\mtg-card-price-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4919A9-43DA-4373-A309-88CDA30A6E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83817C4-5406-400B-9F8A-063FB7424F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="147">
   <si>
     <t>Name</t>
   </si>
@@ -465,6 +465,15 @@
   </si>
   <si>
     <t>Titania, Protector of Argoth</t>
+  </si>
+  <si>
+    <t>Portable Hole</t>
+  </si>
+  <si>
+    <t>Wizard Class</t>
+  </si>
+  <si>
+    <t>Vorpal Sword</t>
   </si>
 </sst>
 </file>
@@ -821,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,874 +1196,916 @@
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="2">
-        <v>3.87</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D27" s="2">
-        <v>0.45</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D28" s="2">
-        <v>0.52</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="2">
-        <v>0.74</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="2">
-        <v>0.65</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>145</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" s="2">
-        <v>3.7</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D32" s="2">
-        <v>1.31</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="2">
-        <v>1.08</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D34" s="2">
-        <v>0.92</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D35" s="2">
-        <v>1.7</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="2">
-        <v>4.74</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="2">
-        <v>0.88</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D38" s="2">
-        <v>3.58</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="2">
-        <v>2.98</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D40" s="2">
-        <v>1.7</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="2">
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="D42" s="2">
-        <v>1.23</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D43" s="2">
-        <v>1.4</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="2">
-        <v>3.38</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C45" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="D45" s="2">
-        <v>3.41</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="2">
-        <v>1.64</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47" s="2">
-        <v>4.3</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D48" s="2">
-        <v>27.94</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
       </c>
       <c r="D49" s="2">
-        <v>9.86</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>143</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C50" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D50" s="2">
-        <v>1.21</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="2">
-        <v>2.0299999999999998</v>
+        <v>27.94</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="2">
-        <v>1.07</v>
+        <v>9.86</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>143</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D53" s="2">
-        <v>2.93</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="2">
-        <v>3.86</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B55" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="2">
-        <v>0.72</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="2">
-        <v>0.97</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B57" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="2">
-        <v>2.46</v>
+        <v>3.86</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B58" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="C58" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D58" s="2">
-        <v>4.54</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="B59" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C59" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D59" s="2">
-        <v>2.68</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="C60" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D60" s="2">
-        <v>1.2</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C61" t="s">
         <v>50</v>
       </c>
       <c r="D61" s="2">
-        <v>1.26</v>
+        <v>4.54</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="B62" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D62" s="2">
-        <v>5.64</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B63" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D63" s="2">
-        <v>3.93</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D64" s="2">
-        <v>3.25</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B65" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D65" s="2">
-        <v>1.74</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B66" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" s="2">
-        <v>1.21</v>
+        <v>3.93</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B67" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" s="2">
-        <v>8.83</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B68" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D68" s="2">
-        <v>8.3699999999999992</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B69" t="s">
-        <v>109</v>
+        <v>11</v>
       </c>
       <c r="C69" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D69" s="2">
-        <v>17.809999999999999</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B70" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C70" t="s">
         <v>6</v>
       </c>
       <c r="D70" s="2">
-        <v>0.69</v>
+        <v>8.83</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B71" t="s">
-        <v>109</v>
+        <v>18</v>
       </c>
       <c r="C71" t="s">
         <v>6</v>
       </c>
       <c r="D71" s="2">
-        <v>9.4600000000000009</v>
+        <v>8.3699999999999992</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B72" t="s">
         <v>109</v>
       </c>
       <c r="C72" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D72" s="2">
-        <v>8.93</v>
+        <v>17.809999999999999</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B73" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C73" t="s">
         <v>6</v>
       </c>
       <c r="D73" s="2">
-        <v>3.18</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B74" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="C74" t="s">
         <v>6</v>
       </c>
       <c r="D74" s="2">
-        <v>1.96</v>
+        <v>9.4600000000000009</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B75" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C75" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D75" s="2">
-        <v>0.63</v>
+        <v>8.93</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="2">
-        <v>4.8099999999999996</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C77" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D77" s="2">
-        <v>3.31</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B78" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C78" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D78" s="2">
-        <v>0.79</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B79" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D79" s="2">
-        <v>1.66</v>
+        <v>4.8099999999999996</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B80" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="C80" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D80" s="2">
-        <v>1.1000000000000001</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B81" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" s="2">
-        <v>1.02</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B82" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C82" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D82" s="2">
-        <v>0.71</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D83" s="2"/>
+      <c r="A83" t="s">
+        <v>123</v>
+      </c>
+      <c r="B83" t="s">
+        <v>124</v>
+      </c>
+      <c r="C83" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="2">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>125</v>
+      </c>
+      <c r="B84" t="s">
+        <v>124</v>
+      </c>
+      <c r="C84" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B85" t="s">
+        <v>109</v>
+      </c>
+      <c r="C85" t="s">
+        <v>50</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>129</v>
       </c>
-      <c r="D84" s="2"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>133</v>
-      </c>
-      <c r="B85" t="s">
-        <v>134</v>
-      </c>
-      <c r="C85" t="s">
-        <v>135</v>
-      </c>
-      <c r="D85" s="3">
-        <v>11.52</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>130</v>
-      </c>
-      <c r="B86" t="s">
-        <v>131</v>
-      </c>
-      <c r="C86" t="s">
-        <v>132</v>
-      </c>
-      <c r="D86" s="3">
-        <v>38.479999999999997</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>136</v>
-      </c>
-      <c r="B87" t="s">
-        <v>137</v>
-      </c>
-      <c r="C87" t="s">
-        <v>138</v>
-      </c>
-      <c r="D87" s="3">
-        <v>4.08</v>
-      </c>
+      <c r="D87" s="2"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>133</v>
+      </c>
+      <c r="B88" t="s">
+        <v>134</v>
+      </c>
+      <c r="C88" t="s">
+        <v>135</v>
+      </c>
+      <c r="D88" s="3">
+        <v>11.52</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>130</v>
+      </c>
+      <c r="B89" t="s">
+        <v>131</v>
+      </c>
+      <c r="C89" t="s">
+        <v>132</v>
+      </c>
+      <c r="D89" s="3">
+        <v>38.479999999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>136</v>
+      </c>
+      <c r="B90" t="s">
+        <v>137</v>
+      </c>
+      <c r="C90" t="s">
+        <v>138</v>
+      </c>
+      <c r="D90" s="3">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>139</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B91" t="s">
         <v>140</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C91" t="s">
         <v>141</v>
       </c>
-      <c r="D88" s="3">
+      <c r="D91" s="3">
         <v>5.0199999999999996</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D89" s="3"/>
-    </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D90" s="3">
-        <f>SUM(D2:D88)</f>
-        <v>388.15999999999997</v>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="3"/>
+    </row>
+    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D93" s="3">
+        <f>SUM(D2:D91)</f>
+        <v>391.34999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I almost won a tournament
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\o\git-repos\mtg-card-price-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83817C4-5406-400B-9F8A-063FB7424F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F8D296-CB43-4E1A-AA39-62252B1C0E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="153">
   <si>
     <t>Name</t>
   </si>
@@ -474,6 +474,24 @@
   </si>
   <si>
     <t>Vorpal Sword</t>
+  </si>
+  <si>
+    <t>The Reality Chip</t>
+  </si>
+  <si>
+    <t>Kamigawa: Neon Dynasty: Promos</t>
+  </si>
+  <si>
+    <t>See Double</t>
+  </si>
+  <si>
+    <t>March of the Machine</t>
+  </si>
+  <si>
+    <t>Atraxa, Praetors' Voice</t>
+  </si>
+  <si>
+    <t>Multiverse Legends</t>
   </si>
 </sst>
 </file>
@@ -830,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,888 +1242,930 @@
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>150</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D28" s="2">
-        <v>0.45</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D29" s="2">
-        <v>0.52</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>147</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D30" s="2">
-        <v>0.74</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" s="2">
-        <v>0.87</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="D32" s="2">
-        <v>0.65</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="2">
-        <v>3.7</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D34" s="2">
-        <v>1.31</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="2">
-        <v>1.08</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D36" s="2">
-        <v>0.96</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="2">
-        <v>0.92</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>146</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D38" s="2">
-        <v>1.7</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="2">
-        <v>4.74</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D40" s="2">
-        <v>0.88</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="2">
-        <v>3.58</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="2">
-        <v>2.98</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D43" s="2">
-        <v>1.7</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="2">
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D45" s="2">
-        <v>1.23</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="D47" s="2">
-        <v>3.38</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D48" s="2">
-        <v>3.41</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
       </c>
       <c r="D49" s="2">
-        <v>1.64</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B50" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D50" s="2">
-        <v>4.3</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="2">
-        <v>27.94</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="2">
-        <v>9.86</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D53" s="2">
-        <v>1.21</v>
+        <v>27.94</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="2">
-        <v>2.0299999999999998</v>
+        <v>9.86</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D55" s="2">
-        <v>1.07</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="2">
-        <v>2.93</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="2">
-        <v>3.86</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B58" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
       </c>
       <c r="D58" s="2">
-        <v>0.72</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
       </c>
       <c r="D59" s="2">
-        <v>0.97</v>
+        <v>3.86</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B60" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="2">
-        <v>2.46</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C61" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D61" s="2">
-        <v>4.54</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="C62" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D62" s="2">
-        <v>2.68</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="C63" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D63" s="2">
-        <v>1.2</v>
+        <v>4.54</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="B64" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C64" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D64" s="2">
-        <v>1.26</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B65" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D65" s="2">
-        <v>5.64</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="C66" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D66" s="2">
-        <v>3.93</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B67" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" s="2">
-        <v>3.25</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B68" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="C68" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D68" s="2">
-        <v>1.74</v>
+        <v>3.93</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B69" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
       </c>
       <c r="D69" s="2">
-        <v>1.21</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B70" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D70" s="2">
-        <v>8.83</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B71" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C71" t="s">
         <v>6</v>
       </c>
       <c r="D71" s="2">
-        <v>8.3699999999999992</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="B72" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="C72" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D72" s="2">
-        <v>17.809999999999999</v>
+        <v>10.97</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B73" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C73" t="s">
         <v>6</v>
       </c>
       <c r="D73" s="2">
-        <v>0.69</v>
+        <v>8.83</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B74" t="s">
-        <v>109</v>
+        <v>18</v>
       </c>
       <c r="C74" t="s">
         <v>6</v>
       </c>
       <c r="D74" s="2">
-        <v>9.4600000000000009</v>
+        <v>8.3699999999999992</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B75" t="s">
         <v>109</v>
       </c>
       <c r="C75" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D75" s="2">
-        <v>8.93</v>
+        <v>17.809999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B76" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="2">
-        <v>3.18</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B77" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" s="2">
-        <v>1.96</v>
+        <v>9.4600000000000009</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B78" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C78" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D78" s="2">
-        <v>0.63</v>
+        <v>8.93</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
       <c r="D79" s="2">
-        <v>4.8099999999999996</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B80" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C80" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D80" s="2">
-        <v>3.31</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B81" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C81" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D81" s="2">
-        <v>0.79</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B82" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D82" s="2">
-        <v>1.66</v>
+        <v>4.8099999999999996</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B83" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="C83" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D83" s="2">
-        <v>1.1000000000000001</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B84" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C84" t="s">
         <v>6</v>
       </c>
       <c r="D84" s="2">
-        <v>1.02</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B85" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C85" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D85" s="2">
-        <v>0.71</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D86" s="2"/>
+      <c r="A86" t="s">
+        <v>123</v>
+      </c>
+      <c r="B86" t="s">
+        <v>124</v>
+      </c>
+      <c r="C86" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="2">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>125</v>
+      </c>
+      <c r="B87" t="s">
+        <v>124</v>
+      </c>
+      <c r="C87" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>126</v>
+      </c>
+      <c r="B88" t="s">
+        <v>109</v>
+      </c>
+      <c r="C88" t="s">
+        <v>50</v>
+      </c>
+      <c r="D88" s="2">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>129</v>
       </c>
-      <c r="D87" s="2"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>133</v>
-      </c>
-      <c r="B88" t="s">
-        <v>134</v>
-      </c>
-      <c r="C88" t="s">
-        <v>135</v>
-      </c>
-      <c r="D88" s="3">
-        <v>11.52</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>130</v>
-      </c>
-      <c r="B89" t="s">
-        <v>131</v>
-      </c>
-      <c r="C89" t="s">
-        <v>132</v>
-      </c>
-      <c r="D89" s="3">
-        <v>38.479999999999997</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>136</v>
-      </c>
-      <c r="B90" t="s">
-        <v>137</v>
-      </c>
-      <c r="C90" t="s">
-        <v>138</v>
-      </c>
-      <c r="D90" s="3">
-        <v>4.08</v>
-      </c>
+      <c r="D90" s="2"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>133</v>
+      </c>
+      <c r="B91" t="s">
+        <v>134</v>
+      </c>
+      <c r="C91" t="s">
+        <v>135</v>
+      </c>
+      <c r="D91" s="3">
+        <v>11.52</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>130</v>
+      </c>
+      <c r="B92" t="s">
+        <v>131</v>
+      </c>
+      <c r="C92" t="s">
+        <v>132</v>
+      </c>
+      <c r="D92" s="3">
+        <v>38.479999999999997</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>136</v>
+      </c>
+      <c r="B93" t="s">
+        <v>137</v>
+      </c>
+      <c r="C93" t="s">
+        <v>138</v>
+      </c>
+      <c r="D93" s="3">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>139</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B94" t="s">
         <v>140</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C94" t="s">
         <v>141</v>
       </c>
-      <c r="D91" s="3">
+      <c r="D94" s="3">
         <v>5.0199999999999996</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D92" s="3"/>
-    </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D93" s="3">
-        <f>SUM(D2:D91)</f>
-        <v>391.34999999999997</v>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="3"/>
+    </row>
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D96" s="3">
+        <f>SUM(D2:D94)</f>
+        <v>405.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MH2 pulls + Tin signed my card <3 <3 <3
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\o\git-repos\mtg-card-price-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B910B4-B337-4B55-B749-FE012072BE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4AF4DB-6DB2-4217-BE9E-BCDDAAA4AE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="159">
   <si>
     <t>Name</t>
   </si>
@@ -504,6 +504,12 @@
   </si>
   <si>
     <t>Release Promos</t>
+  </si>
+  <si>
+    <t>Imperial Recruiter</t>
+  </si>
+  <si>
+    <t>Academy Manufactor</t>
   </si>
 </sst>
 </file>
@@ -860,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,142 +1470,142 @@
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>157</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D43" s="2">
-        <v>4.74</v>
+        <v>4.84</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="2">
-        <v>0.88</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="2">
-        <v>3.58</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="2">
-        <v>2.98</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D47" s="2">
-        <v>1.7</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>75</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>17</v>
       </c>
-      <c r="C48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="2">
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="2">
         <v>1.43</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>76</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>77</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D50" s="2">
         <v>1.23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>79</v>
-      </c>
-      <c r="B50" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1.4</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="2">
-        <v>3.38</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D52" s="2">
-        <v>3.41</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1607,256 +1613,256 @@
         <v>82</v>
       </c>
       <c r="B53" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D53" s="2">
-        <v>1.64</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="2">
-        <v>4.3</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B55" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="2">
-        <v>27.94</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="2">
-        <v>9.86</v>
+        <v>27.94</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>143</v>
+        <v>87</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C57" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D57" s="2">
-        <v>1.21</v>
+        <v>9.86</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="B58" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D58" s="2">
-        <v>2.0299999999999998</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
       </c>
       <c r="D59" s="2">
-        <v>1.07</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="2">
-        <v>2.93</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="2">
-        <v>3.86</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62" s="2">
-        <v>0.72</v>
+        <v>3.86</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B63" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="2">
-        <v>0.97</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B64" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="C64" t="s">
         <v>6</v>
       </c>
       <c r="D64" s="2">
-        <v>2.46</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B65" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="C65" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D65" s="2">
-        <v>4.54</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="C66" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D66" s="2">
-        <v>2.68</v>
+        <v>4.54</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="B67" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C67" t="s">
         <v>60</v>
       </c>
       <c r="D67" s="2">
-        <v>1.2</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B68" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="C68" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D68" s="2">
-        <v>1.26</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D69" s="2">
-        <v>5.64</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B70" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="C70" t="s">
         <v>6</v>
       </c>
       <c r="D70" s="2">
-        <v>3.93</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B71" t="s">
         <v>102</v>
@@ -1865,361 +1871,389 @@
         <v>6</v>
       </c>
       <c r="D71" s="2">
-        <v>3.25</v>
+        <v>3.93</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B72" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="C72" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D72" s="2">
-        <v>1.74</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B73" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C73" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D73" s="2">
-        <v>1.21</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="B74" t="s">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="C74" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D74" s="2">
-        <v>10.97</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>26</v>
+        <v>152</v>
       </c>
       <c r="C75" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D75" s="2">
-        <v>8.83</v>
+        <v>10.97</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
       <c r="B76" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="2">
-        <v>8.3699999999999992</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B77" t="s">
-        <v>109</v>
+        <v>26</v>
       </c>
       <c r="C77" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D77" s="2">
-        <v>17.809999999999999</v>
+        <v>8.83</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B78" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" s="2">
-        <v>0.69</v>
+        <v>8.3699999999999992</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
       <c r="B79" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C79" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D79" s="2">
-        <v>1.53</v>
+        <v>17.809999999999999</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B80" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" s="2">
-        <v>9.4600000000000009</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="B81" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C81" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D81" s="2">
-        <v>8.93</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B82" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" s="2">
-        <v>3.18</v>
+        <v>9.4600000000000009</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B83" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
       </c>
       <c r="D83" s="2">
-        <v>1.96</v>
+        <v>8.93</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B84" t="s">
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="C84" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D84" s="2">
-        <v>0.63</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B85" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C85" t="s">
         <v>6</v>
       </c>
       <c r="D85" s="2">
-        <v>4.8099999999999996</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B86" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="C86" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D86" s="2">
-        <v>3.31</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B87" t="s">
-        <v>120</v>
+        <v>5</v>
       </c>
       <c r="C87" t="s">
         <v>6</v>
       </c>
       <c r="D87" s="2">
-        <v>0.79</v>
+        <v>4.8099999999999996</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B88" t="s">
-        <v>122</v>
+        <v>61</v>
       </c>
       <c r="C88" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D88" s="2">
-        <v>1.66</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B89" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C89" t="s">
         <v>6</v>
       </c>
       <c r="D89" s="2">
-        <v>1.1000000000000001</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B90" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C90" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D90" s="2">
-        <v>1.02</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B91" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="C91" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D91" s="2">
-        <v>0.71</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D92" s="2"/>
+      <c r="A92" t="s">
+        <v>125</v>
+      </c>
+      <c r="B92" t="s">
+        <v>124</v>
+      </c>
+      <c r="C92" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1.02</v>
+      </c>
     </row>
     <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>126</v>
+      </c>
+      <c r="B93" t="s">
+        <v>109</v>
+      </c>
+      <c r="C93" t="s">
+        <v>50</v>
+      </c>
+      <c r="D93" s="2">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>129</v>
       </c>
-      <c r="D93" s="2"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>133</v>
-      </c>
-      <c r="B94" t="s">
-        <v>134</v>
-      </c>
-      <c r="C94" t="s">
-        <v>135</v>
-      </c>
-      <c r="D94" s="3">
-        <v>11.52</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>130</v>
-      </c>
-      <c r="B95" t="s">
-        <v>131</v>
-      </c>
-      <c r="C95" t="s">
-        <v>132</v>
-      </c>
-      <c r="D95" s="3">
-        <v>38.479999999999997</v>
-      </c>
+      <c r="D95" s="2"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B96" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C96" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D96" s="3">
-        <v>4.08</v>
+        <v>11.52</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>130</v>
+      </c>
+      <c r="B97" t="s">
+        <v>131</v>
+      </c>
+      <c r="C97" t="s">
+        <v>132</v>
+      </c>
+      <c r="D97" s="3">
+        <v>38.479999999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>136</v>
+      </c>
+      <c r="B98" t="s">
+        <v>137</v>
+      </c>
+      <c r="C98" t="s">
+        <v>138</v>
+      </c>
+      <c r="D98" s="3">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>139</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B99" t="s">
         <v>140</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C99" t="s">
         <v>141</v>
       </c>
-      <c r="D97" s="3">
+      <c r="D99" s="3">
         <v>5.0199999999999996</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D98" s="3"/>
-    </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D99" s="3">
-        <f>SUM(D2:D97)</f>
-        <v>409.6699999999999</v>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="3"/>
+    </row>
+    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D101" s="3">
+        <f>SUM(D2:D99)</f>
+        <v>418.54999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pokemon Obsidian Flames Prerelease
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\o\git-repos\mtg-card-price-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4AF4DB-6DB2-4217-BE9E-BCDDAAA4AE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C47C59A-976D-46A7-96C1-637E711F1ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="161">
   <si>
     <t>Name</t>
   </si>
@@ -510,6 +510,12 @@
   </si>
   <si>
     <t>Academy Manufactor</t>
+  </si>
+  <si>
+    <t>Palafin</t>
+  </si>
+  <si>
+    <t>SVP036</t>
   </si>
 </sst>
 </file>
@@ -866,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,12 +2254,26 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D100" s="3"/>
-    </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D101" s="3">
-        <f>SUM(D2:D99)</f>
-        <v>418.54999999999995</v>
+      <c r="A100" t="s">
+        <v>159</v>
+      </c>
+      <c r="B100" t="s">
+        <v>137</v>
+      </c>
+      <c r="C100" t="s">
+        <v>160</v>
+      </c>
+      <c r="D100" s="3">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="3"/>
+    </row>
+    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D102" s="3">
+        <f>SUM(D2:D100)</f>
+        <v>422.74999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I'm fucking quitting Pioneer
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\o\git-repos\mtg-card-price-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C47C59A-976D-46A7-96C1-637E711F1ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DCCC24-BF72-433D-B7EF-C7C1FE2A4500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -516,6 +516,12 @@
   </si>
   <si>
     <t>SVP036</t>
+  </si>
+  <si>
+    <t>Katilda, Dawnhart Martyr: Katilda's Rising Dawn</t>
+  </si>
+  <si>
+    <t>Innistrad: Crimson Vow</t>
   </si>
 </sst>
 </file>
@@ -872,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,436 +1202,436 @@
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="B23" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D23" s="2">
-        <v>0.95</v>
+        <v>2.3199999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>127</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D24" s="2">
-        <v>1.91</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="2">
-        <v>0.7</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="2">
-        <v>4.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="2">
-        <v>1.36</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="2">
-        <v>3.87</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>150</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="2">
-        <v>1.35</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>149</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>150</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D30" s="2">
-        <v>0.45</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>147</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>148</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D31" s="2">
-        <v>1.42</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>148</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D32" s="2">
-        <v>0.52</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="2">
-        <v>0.74</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>145</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="2">
-        <v>0.87</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="2">
-        <v>0.65</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="2">
-        <v>3.7</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D37" s="2">
-        <v>1.31</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D38" s="2">
-        <v>1.08</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="2">
-        <v>0.96</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="2">
-        <v>0.92</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>155</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>156</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="2">
-        <v>1.39</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>155</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>156</v>
       </c>
       <c r="C42" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D42" s="2">
-        <v>1.7</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>157</v>
+        <v>65</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D43" s="2">
-        <v>4.84</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>157</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D44" s="2">
-        <v>4.74</v>
+        <v>4.84</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="2">
-        <v>0.88</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="2">
-        <v>3.58</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47" s="2">
-        <v>2.98</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C48" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D48" s="2">
-        <v>1.7</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>75</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>17</v>
       </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="2">
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="2">
         <v>1.43</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>76</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>77</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>78</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D51" s="2">
         <v>1.23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="2">
-        <v>1.4</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="2">
-        <v>3.38</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C53" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D53" s="2">
-        <v>3.41</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1633,256 +1639,256 @@
         <v>82</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D54" s="2">
-        <v>1.64</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="2">
-        <v>4.3</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="2">
-        <v>27.94</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="2">
-        <v>9.86</v>
+        <v>27.94</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>143</v>
+        <v>87</v>
       </c>
       <c r="B58" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C58" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D58" s="2">
-        <v>1.21</v>
+        <v>9.86</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D59" s="2">
-        <v>2.0299999999999998</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="2">
-        <v>1.07</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="2">
-        <v>2.93</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62" s="2">
-        <v>3.86</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="2">
-        <v>0.72</v>
+        <v>3.86</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B64" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="C64" t="s">
         <v>6</v>
       </c>
       <c r="D64" s="2">
-        <v>0.97</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B65" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="2">
-        <v>2.46</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B66" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="C66" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D66" s="2">
-        <v>4.54</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="B67" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="C67" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D67" s="2">
-        <v>2.68</v>
+        <v>4.54</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="B68" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C68" t="s">
         <v>60</v>
       </c>
       <c r="D68" s="2">
-        <v>1.2</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B69" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="C69" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D69" s="2">
-        <v>1.26</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B70" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D70" s="2">
-        <v>5.64</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B71" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="C71" t="s">
         <v>6</v>
       </c>
       <c r="D71" s="2">
-        <v>3.93</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B72" t="s">
         <v>102</v>
@@ -1891,152 +1897,152 @@
         <v>6</v>
       </c>
       <c r="D72" s="2">
-        <v>3.25</v>
+        <v>3.93</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B73" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="C73" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D73" s="2">
-        <v>1.74</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B74" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D74" s="2">
-        <v>1.21</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="B75" t="s">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="C75" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D75" s="2">
-        <v>10.97</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B76" t="s">
-        <v>42</v>
+        <v>152</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D76" s="2">
-        <v>4.04</v>
+        <v>10.97</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>106</v>
+        <v>158</v>
       </c>
       <c r="B77" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" s="2">
-        <v>8.83</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" s="2">
-        <v>8.3699999999999992</v>
+        <v>8.83</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B79" t="s">
-        <v>109</v>
+        <v>18</v>
       </c>
       <c r="C79" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D79" s="2">
-        <v>17.809999999999999</v>
+        <v>8.3699999999999992</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B80" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="C80" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D80" s="2">
-        <v>0.69</v>
+        <v>17.809999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="B81" t="s">
-        <v>122</v>
+        <v>66</v>
       </c>
       <c r="C81" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D81" s="2">
-        <v>1.53</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="B82" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C82" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D82" s="2">
-        <v>9.4600000000000009</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B83" t="s">
         <v>109</v>
@@ -2045,26 +2051,26 @@
         <v>6</v>
       </c>
       <c r="D83" s="2">
-        <v>8.93</v>
+        <v>9.4600000000000009</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B84" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="C84" t="s">
         <v>6</v>
       </c>
       <c r="D84" s="2">
-        <v>3.18</v>
+        <v>8.93</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B85" t="s">
         <v>57</v>
@@ -2073,96 +2079,96 @@
         <v>6</v>
       </c>
       <c r="D85" s="2">
-        <v>1.96</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B86" t="s">
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="C86" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D86" s="2">
-        <v>0.63</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="C87" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D87" s="2">
-        <v>4.8099999999999996</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B88" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="C88" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D88" s="2">
-        <v>3.31</v>
+        <v>4.8099999999999996</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B89" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
       <c r="C89" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D89" s="2">
-        <v>0.79</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B90" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C90" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D90" s="2">
-        <v>1.66</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B91" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C91" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D91" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B92" t="s">
         <v>124</v>
@@ -2171,109 +2177,123 @@
         <v>6</v>
       </c>
       <c r="D92" s="2">
-        <v>1.02</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>125</v>
+      </c>
+      <c r="B93" t="s">
+        <v>124</v>
+      </c>
+      <c r="C93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" s="2">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>126</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>109</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>50</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D94" s="2">
         <v>0.71</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D94" s="2"/>
-    </row>
     <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>129</v>
       </c>
-      <c r="D95" s="2"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>133</v>
-      </c>
-      <c r="B96" t="s">
-        <v>134</v>
-      </c>
-      <c r="C96" t="s">
-        <v>135</v>
-      </c>
-      <c r="D96" s="3">
-        <v>11.52</v>
-      </c>
+      <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B97" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C97" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D97" s="3">
-        <v>38.479999999999997</v>
+        <v>11.52</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B98" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C98" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D98" s="3">
-        <v>4.08</v>
+        <v>38.479999999999997</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B99" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C99" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D99" s="3">
-        <v>5.0199999999999996</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>139</v>
+      </c>
+      <c r="B100" t="s">
+        <v>140</v>
+      </c>
+      <c r="C100" t="s">
+        <v>141</v>
+      </c>
+      <c r="D100" s="3">
+        <v>5.0199999999999996</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>159</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>137</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>160</v>
       </c>
-      <c r="D100" s="3">
+      <c r="D101" s="3">
         <v>4.2</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D101" s="3"/>
-    </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D102" s="3">
-        <f>SUM(D2:D100)</f>
-        <v>422.74999999999994</v>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="3"/>
+    </row>
+    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D103" s="3">
+        <f>SUM(D2:D101)</f>
+        <v>425.06999999999988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
My entire MTG collection is worth around 1230 €
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\o\git-repos\mtg-card-price-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DCCC24-BF72-433D-B7EF-C7C1FE2A4500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5A5046-E22F-4728-BA2D-488ADE400951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="134">
   <si>
     <t>Name</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Commander Legends: Battle For Baldur's Gate</t>
   </si>
   <si>
-    <t>Caves of Koilos</t>
-  </si>
-  <si>
     <t>Magic 2015</t>
   </si>
   <si>
@@ -92,36 +89,9 @@
     <t>Magic 2013</t>
   </si>
   <si>
-    <t>Rockfall Vale</t>
-  </si>
-  <si>
-    <t>Innistrad: Midnight Hunt</t>
-  </si>
-  <si>
-    <t>Temple of Epiphany</t>
-  </si>
-  <si>
-    <t>Core Set 2021</t>
-  </si>
-  <si>
-    <t>Orzhov Basilica</t>
-  </si>
-  <si>
-    <t>Double Masters 2022: Extras</t>
-  </si>
-  <si>
-    <t>Boros Garrison</t>
-  </si>
-  <si>
     <t>Double Masters 2022</t>
   </si>
   <si>
-    <t>Selesnya Sanctuary</t>
-  </si>
-  <si>
-    <t>Izzet Boilerworks</t>
-  </si>
-  <si>
     <t>Jetmir's Garden</t>
   </si>
   <si>
@@ -140,9 +110,6 @@
     <t>The Brothers' War: Promos</t>
   </si>
   <si>
-    <t>Gond Gate</t>
-  </si>
-  <si>
     <t>Maze's End</t>
   </si>
   <si>
@@ -170,9 +137,6 @@
     <t>Phyrexia: All Will Be One</t>
   </si>
   <si>
-    <t>Valiant Veteran</t>
-  </si>
-  <si>
     <t>White Plume Adventurer</t>
   </si>
   <si>
@@ -188,21 +152,6 @@
     <t>Foil</t>
   </si>
   <si>
-    <t>Mystical Dispute</t>
-  </si>
-  <si>
-    <t>Throne of Eldraine</t>
-  </si>
-  <si>
-    <t>Narset, Parter of Veils</t>
-  </si>
-  <si>
-    <t>War of the Spark</t>
-  </si>
-  <si>
-    <t>Consider</t>
-  </si>
-  <si>
     <t>Gravecrawler</t>
   </si>
   <si>
@@ -227,9 +176,6 @@
     <t>The Cruelty of Gix</t>
   </si>
   <si>
-    <t>Inquisition of Kozilek</t>
-  </si>
-  <si>
     <t>Flame-Wreathed Phoenix</t>
   </si>
   <si>
@@ -239,15 +185,6 @@
     <t>Shivan Devastator</t>
   </si>
   <si>
-    <t>Skitterbeam Battalion</t>
-  </si>
-  <si>
-    <t>Vexing Devil</t>
-  </si>
-  <si>
-    <t>Avacyn Restored</t>
-  </si>
-  <si>
     <t>Bane of Progress</t>
   </si>
   <si>
@@ -302,9 +239,6 @@
     <t>Haywire Mite</t>
   </si>
   <si>
-    <t>Sphinx's Revelation</t>
-  </si>
-  <si>
     <t>Ashiok, Nightmare Weaver</t>
   </si>
   <si>
@@ -317,9 +251,6 @@
     <t>Buy a Box Promos</t>
   </si>
   <si>
-    <t>Legion's Initiative</t>
-  </si>
-  <si>
     <t>Expressive Iteration</t>
   </si>
   <si>
@@ -365,9 +296,6 @@
     <t>Mystery Booster</t>
   </si>
   <si>
-    <t>Astral Cornucopia</t>
-  </si>
-  <si>
     <t>Coat of Arms</t>
   </si>
   <si>
@@ -380,42 +308,21 @@
     <t>Grafdigger's Cage</t>
   </si>
   <si>
-    <t>Helm of Awakening</t>
-  </si>
-  <si>
-    <t>Dominaria Remastered</t>
-  </si>
-  <si>
     <t>Illusionist's Bracers</t>
   </si>
   <si>
     <t>Karn, Living Legacy</t>
   </si>
   <si>
-    <t>Mirror Box</t>
-  </si>
-  <si>
-    <t>Kamigawa: Neon Dynasty</t>
-  </si>
-  <si>
-    <t>Mishra's Bauble</t>
-  </si>
-  <si>
     <t>Retro Frame Artifacts</t>
   </si>
   <si>
-    <t>Sol Ring</t>
-  </si>
-  <si>
     <t>Commander 2017</t>
   </si>
   <si>
     <t>Swiftfoot Boots</t>
   </si>
   <si>
-    <t>Pili-Pala</t>
-  </si>
-  <si>
     <t>Sunfall</t>
   </si>
   <si>
@@ -473,9 +380,6 @@
     <t>Wizard Class</t>
   </si>
   <si>
-    <t>Vorpal Sword</t>
-  </si>
-  <si>
     <t>The Reality Chip</t>
   </si>
   <si>
@@ -500,12 +404,6 @@
     <t>Caged Sun</t>
   </si>
   <si>
-    <t>Disrupt Decorum</t>
-  </si>
-  <si>
-    <t>Release Promos</t>
-  </si>
-  <si>
     <t>Imperial Recruiter</t>
   </si>
   <si>
@@ -522,6 +420,21 @@
   </si>
   <si>
     <t>Innistrad: Crimson Vow</t>
+  </si>
+  <si>
+    <t>Bloodgift Demon</t>
+  </si>
+  <si>
+    <t>Starter Commander Decks</t>
+  </si>
+  <si>
+    <t>Ghalta and Mavren</t>
+  </si>
+  <si>
+    <t>Third Path Iconoclast</t>
+  </si>
+  <si>
+    <t>Soulless Jailer</t>
   </si>
 </sst>
 </file>
@@ -878,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +830,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2">
-        <v>9.92</v>
+        <v>8.84</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -931,7 +844,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="2">
-        <v>14.13</v>
+        <v>13.13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -945,7 +858,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>9.85</v>
+        <v>8.83</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -959,26 +872,26 @@
         <v>6</v>
       </c>
       <c r="D5" s="2">
-        <v>8.51</v>
+        <v>10.41</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="2">
-        <v>0.61</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -987,152 +900,152 @@
         <v>6</v>
       </c>
       <c r="D7" s="2">
-        <v>0.9</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="2">
-        <v>1.66</v>
+        <v>11.21</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="2">
-        <v>0.79</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="2">
-        <v>0.23</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="2">
-        <v>0.48</v>
+        <v>3.77</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="2">
-        <v>0.13</v>
+        <v>24.74</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="2">
-        <v>0.09</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="2">
-        <v>0.56999999999999995</v>
+        <v>20.61</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="2">
-        <v>7.84</v>
+        <v>2.89</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2">
-        <v>3.25</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="2">
-        <v>2.92</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -1141,147 +1054,147 @@
         <v>6</v>
       </c>
       <c r="D18" s="2">
-        <v>0.66</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="2">
-        <v>2.39</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="2">
-        <v>33.119999999999997</v>
+        <v>4.24</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="2">
-        <v>6.86</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D22" s="2">
-        <v>20.58</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D23" s="2">
-        <v>2.3199999999999998</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D24" s="2">
-        <v>0.95</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="2">
-        <v>1.91</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="2">
-        <v>0.7</v>
+        <v>4.09</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="D27" s="2">
-        <v>4.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="2">
-        <v>1.36</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1292,24 +1205,24 @@
         <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D29" s="2">
-        <v>3.87</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="B30" t="s">
-        <v>150</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="D30" s="2">
-        <v>1.35</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1317,139 +1230,139 @@
         <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D31" s="2">
-        <v>0.45</v>
+        <v>4.6399999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>147</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D32" s="2">
-        <v>1.42</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D33" s="2">
-        <v>0.52</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="2">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="D35" s="2">
-        <v>0.87</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="2">
-        <v>0.65</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="2">
-        <v>3.7</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="D38" s="2">
-        <v>1.31</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="2">
-        <v>1.08</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="2">
-        <v>0.96</v>
+        <v>4.5599999999999996</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1457,843 +1370,549 @@
         <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="2">
-        <v>0.92</v>
+        <v>16.28</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>155</v>
+        <v>66</v>
       </c>
       <c r="B42" t="s">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="2">
-        <v>1.39</v>
+        <v>8.0299999999999994</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D43" s="2">
-        <v>1.7</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>157</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D44" s="2">
-        <v>4.84</v>
+        <v>4.26</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="2">
-        <v>4.74</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="2">
-        <v>0.88</v>
+        <v>3.89</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B47" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47" s="2">
-        <v>3.58</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="2">
-        <v>2.98</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D49" s="2">
-        <v>1.7</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
       </c>
       <c r="D50" s="2">
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="C51" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="D51" s="2">
-        <v>1.23</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="D52" s="2">
-        <v>1.4</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D53" s="2">
-        <v>3.38</v>
+        <v>1.63</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D54" s="2">
-        <v>3.41</v>
+        <v>4.5199999999999996</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="2">
-        <v>1.64</v>
+        <v>3.64</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="2">
-        <v>4.3</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D57" s="2">
-        <v>27.94</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B58" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
       </c>
       <c r="D58" s="2">
-        <v>9.86</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="B59" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D59" s="2">
-        <v>1.21</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>132</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="2">
-        <v>2.0299999999999998</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="B61" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="2">
-        <v>1.07</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B62" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62" s="2">
-        <v>2.93</v>
+        <v>7.14</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="2">
-        <v>3.86</v>
+        <v>11.53</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B64" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D64" s="2">
-        <v>0.72</v>
+        <v>17.39</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="B65" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="D65" s="2">
-        <v>0.97</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B66" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" s="2">
-        <v>2.46</v>
+        <v>9.02</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B67" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D67" s="2">
-        <v>4.54</v>
+        <v>5.85</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C68" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D68" s="2">
-        <v>2.68</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B69" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C69" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D69" s="2">
-        <v>1.2</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B70" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D70" s="2">
-        <v>1.26</v>
+        <v>4.83</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B71" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D71" s="2">
-        <v>5.64</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="C72" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="D72" s="2">
-        <v>3.93</v>
+        <v>1.61</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B73" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C73" t="s">
         <v>6</v>
       </c>
       <c r="D73" s="2">
-        <v>3.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>104</v>
-      </c>
-      <c r="B74" t="s">
-        <v>16</v>
-      </c>
-      <c r="C74" t="s">
-        <v>50</v>
-      </c>
-      <c r="D74" s="2">
-        <v>1.74</v>
-      </c>
+      <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>98</v>
+      </c>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>102</v>
+      </c>
+      <c r="B76" t="s">
+        <v>103</v>
+      </c>
+      <c r="C76" t="s">
+        <v>104</v>
+      </c>
+      <c r="D76" s="3">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77" t="s">
+        <v>100</v>
+      </c>
+      <c r="C77" t="s">
+        <v>101</v>
+      </c>
+      <c r="D77" s="3">
+        <v>26.33</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>105</v>
       </c>
-      <c r="B75" t="s">
-        <v>11</v>
-      </c>
-      <c r="C75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" s="2">
-        <v>1.21</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>151</v>
-      </c>
-      <c r="B76" t="s">
-        <v>152</v>
-      </c>
-      <c r="C76" t="s">
-        <v>60</v>
-      </c>
-      <c r="D76" s="2">
-        <v>10.97</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>158</v>
-      </c>
-      <c r="B77" t="s">
-        <v>42</v>
-      </c>
-      <c r="C77" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77" s="2">
-        <v>4.04</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="B78" t="s">
         <v>106</v>
       </c>
-      <c r="B78" t="s">
-        <v>26</v>
-      </c>
       <c r="C78" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" s="2">
-        <v>8.83</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D78" s="3">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B79" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
       <c r="C79" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="2">
-        <v>8.3699999999999992</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="D79" s="3">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="B80" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C80" t="s">
-        <v>50</v>
-      </c>
-      <c r="D80" s="2">
-        <v>17.809999999999999</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>110</v>
-      </c>
-      <c r="B81" t="s">
-        <v>66</v>
-      </c>
-      <c r="C81" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" s="2">
-        <v>0.69</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>154</v>
-      </c>
-      <c r="B82" t="s">
-        <v>122</v>
-      </c>
-      <c r="C82" t="s">
-        <v>60</v>
-      </c>
-      <c r="D82" s="2">
-        <v>1.53</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>111</v>
-      </c>
-      <c r="B83" t="s">
-        <v>109</v>
-      </c>
-      <c r="C83" t="s">
-        <v>6</v>
-      </c>
-      <c r="D83" s="2">
-        <v>9.4600000000000009</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>112</v>
-      </c>
-      <c r="B84" t="s">
-        <v>109</v>
-      </c>
-      <c r="C84" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" s="2">
-        <v>8.93</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>113</v>
-      </c>
-      <c r="B85" t="s">
-        <v>57</v>
-      </c>
-      <c r="C85" t="s">
-        <v>6</v>
-      </c>
-      <c r="D85" s="2">
-        <v>3.18</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>114</v>
-      </c>
-      <c r="B86" t="s">
-        <v>57</v>
-      </c>
-      <c r="C86" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" s="2">
-        <v>1.96</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>115</v>
-      </c>
-      <c r="B87" t="s">
-        <v>116</v>
-      </c>
-      <c r="C87" t="s">
-        <v>50</v>
-      </c>
-      <c r="D87" s="2">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>117</v>
-      </c>
-      <c r="B88" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" t="s">
-        <v>6</v>
-      </c>
-      <c r="D88" s="2">
-        <v>4.8099999999999996</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>118</v>
-      </c>
-      <c r="B89" t="s">
-        <v>61</v>
-      </c>
-      <c r="C89" t="s">
-        <v>62</v>
-      </c>
-      <c r="D89" s="2">
-        <v>3.31</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>119</v>
-      </c>
-      <c r="B90" t="s">
-        <v>120</v>
-      </c>
-      <c r="C90" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" s="2">
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>121</v>
-      </c>
-      <c r="B91" t="s">
-        <v>122</v>
-      </c>
-      <c r="C91" t="s">
-        <v>60</v>
-      </c>
-      <c r="D91" s="2">
-        <v>1.66</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>123</v>
-      </c>
-      <c r="B92" t="s">
-        <v>124</v>
-      </c>
-      <c r="C92" t="s">
-        <v>6</v>
-      </c>
-      <c r="D92" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>125</v>
-      </c>
-      <c r="B93" t="s">
-        <v>124</v>
-      </c>
-      <c r="C93" t="s">
-        <v>6</v>
-      </c>
-      <c r="D93" s="2">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
         <v>126</v>
       </c>
-      <c r="B94" t="s">
-        <v>109</v>
-      </c>
-      <c r="C94" t="s">
-        <v>50</v>
-      </c>
-      <c r="D94" s="2">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D95" s="2"/>
-    </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>129</v>
-      </c>
-      <c r="D96" s="2"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>133</v>
-      </c>
-      <c r="B97" t="s">
-        <v>134</v>
-      </c>
-      <c r="C97" t="s">
-        <v>135</v>
-      </c>
-      <c r="D97" s="3">
-        <v>11.52</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>130</v>
-      </c>
-      <c r="B98" t="s">
-        <v>131</v>
-      </c>
-      <c r="C98" t="s">
-        <v>132</v>
-      </c>
-      <c r="D98" s="3">
-        <v>38.479999999999997</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>136</v>
-      </c>
-      <c r="B99" t="s">
-        <v>137</v>
-      </c>
-      <c r="C99" t="s">
-        <v>138</v>
-      </c>
-      <c r="D99" s="3">
-        <v>4.08</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>139</v>
-      </c>
-      <c r="B100" t="s">
-        <v>140</v>
-      </c>
-      <c r="C100" t="s">
-        <v>141</v>
-      </c>
-      <c r="D100" s="3">
-        <v>5.0199999999999996</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>159</v>
-      </c>
-      <c r="B101" t="s">
-        <v>137</v>
-      </c>
-      <c r="C101" t="s">
-        <v>160</v>
-      </c>
-      <c r="D101" s="3">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D102" s="3"/>
-    </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D103" s="3">
-        <f>SUM(D2:D101)</f>
-        <v>425.06999999999988</v>
+      <c r="D80" s="3">
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D82" s="3">
+        <f>SUM(D2:D80)</f>
+        <v>362.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>